<commit_message>
Edited accessibility chart to accomodate for user history. Started saving info to user when signing up.
</commit_message>
<xml_diff>
--- a/Accessibility Chart.xlsx
+++ b/Accessibility Chart.xlsx
@@ -15,12 +15,12 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1226" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1251" uniqueCount="168">
   <si>
     <t>APP</t>
   </si>
@@ -509,6 +509,21 @@
   </si>
   <si>
     <t>issues</t>
+  </si>
+  <si>
+    <t>cellNum</t>
+  </si>
+  <si>
+    <t>History</t>
+  </si>
+  <si>
+    <t>history</t>
+  </si>
+  <si>
+    <t>UserId</t>
+  </si>
+  <si>
+    <t>uID</t>
   </si>
 </sst>
 </file>
@@ -686,15 +701,6 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -706,6 +712,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1938,15 +1953,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -4883,1837 +4898,1929 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G167"/>
+  <dimension ref="A1:G172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="G96" sqref="G96"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" style="18" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="18" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" style="18" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" style="18" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="18" customWidth="1"/>
-    <col min="6" max="6" width="1.42578125" style="18" customWidth="1"/>
-    <col min="7" max="7" width="27.5703125" style="18" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="18"/>
+    <col min="1" max="1" width="11.140625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="15" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" style="15" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="15" customWidth="1"/>
+    <col min="6" max="6" width="1.42578125" style="15" customWidth="1"/>
+    <col min="7" max="7" width="27.5703125" style="15" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" style="15" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="20"/>
-      <c r="G1" s="17" t="s">
+      <c r="F1" s="17"/>
+      <c r="G1" s="14" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B2" s="17" t="s">
+      <c r="A2" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="F2" s="20"/>
-      <c r="G2" s="17" t="s">
+      <c r="F2" s="17"/>
+      <c r="G2" s="14" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C3" s="17" t="s">
+      <c r="A3" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="F3" s="17"/>
+      <c r="G3" s="14" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="F3" s="20"/>
-      <c r="G3" s="17" t="s">
+      <c r="F4" s="17"/>
+      <c r="G4" s="14" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" s="17" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="20"/>
-      <c r="G4" s="17" t="s">
+      <c r="F5" s="17"/>
+      <c r="G5" s="14" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C5" s="17" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="20"/>
-      <c r="G5" s="17" t="s">
+      <c r="F6" s="17"/>
+      <c r="G6" s="14" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" s="17" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="F6" s="20"/>
-      <c r="G6" s="17" t="s">
+      <c r="F7" s="17"/>
+      <c r="G7" s="14" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C7" s="17" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="F7" s="20"/>
-      <c r="G7" s="17" t="s">
+      <c r="F8" s="17"/>
+      <c r="G8" s="14" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C8" s="17" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="20"/>
-      <c r="G8" s="17" t="s">
+      <c r="F9" s="17"/>
+      <c r="G9" s="14" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C9" s="17" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="F9" s="20"/>
-      <c r="G9" s="17" t="s">
+      <c r="F10" s="17"/>
+      <c r="G10" s="14" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B10" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C10" s="17" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="20"/>
-      <c r="G10" s="17" t="s">
+      <c r="F11" s="17"/>
+      <c r="G11" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="F12" s="17"/>
+      <c r="G12" s="14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="17"/>
+      <c r="G13" s="14" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="F14" s="17"/>
+      <c r="G14" s="14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="F15" s="17"/>
+      <c r="G15" s="14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="D16" s="14"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="14" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="17"/>
+      <c r="G17" s="14" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" s="17"/>
+      <c r="G18" s="14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="F19" s="17"/>
+      <c r="G19" s="14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="F20" s="17"/>
+      <c r="G20" s="14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F21" s="17"/>
+      <c r="G21" s="14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="17"/>
+      <c r="G22" s="14" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="17"/>
+      <c r="G23" s="14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="F24" s="17"/>
+      <c r="G24" s="14" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F25" s="17"/>
+      <c r="G25" s="14" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="F26" s="17"/>
+      <c r="G26" s="14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" s="17"/>
+      <c r="G27" s="14" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C11" s="17" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="F11" s="20"/>
-      <c r="G11" s="17" t="s">
+      <c r="F28" s="17"/>
+      <c r="G28" s="14" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C12" s="17" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="20"/>
-      <c r="G12" s="17" t="s">
+      <c r="F29" s="17"/>
+      <c r="G29" s="14" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C13" s="17" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C30" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="F13" s="20"/>
-      <c r="G13" s="17" t="s">
+      <c r="F30" s="17"/>
+      <c r="G30" s="14" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D14" s="17" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D31" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="F14" s="20"/>
-      <c r="G14" s="17" t="s">
+      <c r="F31" s="17"/>
+      <c r="G31" s="14" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="F15" s="20"/>
-      <c r="G15" s="17" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="F16" s="20"/>
-      <c r="G16" s="17" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="F17" s="20"/>
-      <c r="G17" s="17" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" s="20"/>
-      <c r="G18" s="17" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="F19" s="20"/>
-      <c r="G19" s="17" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="F20" s="20"/>
-      <c r="G20" s="17" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="F21" s="20"/>
-      <c r="G21" s="17" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="F22" s="20"/>
-      <c r="G22" s="17" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="F23" s="20"/>
-      <c r="G23" s="17" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="F24" s="20"/>
-      <c r="G24" s="17" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="F25" s="20"/>
-      <c r="G25" s="17" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B26" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D26" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="F26" s="20"/>
-      <c r="G26" s="17" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="17" t="s">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F27" s="20"/>
-      <c r="G27" s="17" t="s">
+      <c r="F32" s="17"/>
+      <c r="G32" s="14" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B28" s="17" t="s">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B33" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F28" s="20"/>
-      <c r="G28" s="17" t="s">
+      <c r="F33" s="17"/>
+      <c r="G33" s="14" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B29" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C29" s="17" t="s">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C34" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="F29" s="20"/>
-      <c r="G29" s="17" t="s">
+      <c r="F34" s="17"/>
+      <c r="G34" s="14" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B30" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C30" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D30" s="17" t="s">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D35" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="F30" s="20"/>
-      <c r="G30" s="17" t="s">
+      <c r="F35" s="17"/>
+      <c r="G35" s="14" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B31" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D31" s="17" t="s">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D36" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="F31" s="20"/>
-      <c r="G31" s="17" t="s">
+      <c r="F36" s="17"/>
+      <c r="G36" s="14" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B32" s="17" t="s">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B37" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="F32" s="20"/>
-      <c r="G32" s="17" t="s">
+      <c r="F37" s="17"/>
+      <c r="G37" s="14" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B33" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C33" s="17" t="s">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F33" s="20"/>
-      <c r="G33" s="17" t="s">
+      <c r="F38" s="17"/>
+      <c r="G38" s="14" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B34" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D34" s="17" t="s">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D39" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="F34" s="20"/>
-      <c r="G34" s="17" t="s">
+      <c r="F39" s="17"/>
+      <c r="G39" s="14" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B35" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C35" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D35" s="17" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D40" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="F35" s="20"/>
-      <c r="G35" s="17" t="s">
+      <c r="F40" s="17"/>
+      <c r="G40" s="14" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B36" s="17" t="s">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B41" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="C36" s="17"/>
-      <c r="D36" s="17"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="17" t="s">
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="14" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B37" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C37" s="17" t="s">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C42" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D37" s="17"/>
-      <c r="F37" s="20"/>
-      <c r="G37" s="17" t="s">
+      <c r="D42" s="14"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="14" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B38" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C38" s="17" t="s">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C43" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D38" s="17"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="17" t="s">
+      <c r="D43" s="14"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="14" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B39" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C39" s="17" t="s">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C44" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="F39" s="20"/>
-      <c r="G39" s="17" t="s">
+      <c r="F44" s="17"/>
+      <c r="G44" s="14" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B40" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C40" s="17" t="s">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B45" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C45" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="F40" s="20"/>
-      <c r="G40" s="17" t="s">
+      <c r="F45" s="17"/>
+      <c r="G45" s="14" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B41" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C41" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D41" s="17" t="s">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D46" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="F41" s="20"/>
-      <c r="G41" s="17" t="s">
+      <c r="F46" s="17"/>
+      <c r="G46" s="14" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B42" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C42" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D42" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="E42" s="17" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D47" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E47" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="F42" s="20"/>
-      <c r="G42" s="17" t="s">
+      <c r="F47" s="17"/>
+      <c r="G47" s="14" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B43" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C43" s="17" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C48" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F43" s="20"/>
-      <c r="G43" s="17" t="s">
+      <c r="F48" s="17"/>
+      <c r="G48" s="14" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B44" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C44" s="17" t="s">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B49" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C49" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="F44" s="20"/>
-      <c r="G44" s="17" t="s">
+      <c r="F49" s="17"/>
+      <c r="G49" s="14" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B45" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C45" s="17" t="s">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B50" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C50" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="F45" s="20"/>
-      <c r="G45" s="17" t="s">
+      <c r="F50" s="17"/>
+      <c r="G50" s="14" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B46" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C46" s="17" t="s">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B51" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C51" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="F46" s="20"/>
-      <c r="G46" s="17" t="s">
+      <c r="F51" s="17"/>
+      <c r="G51" s="14" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B47" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C47" s="17" t="s">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B52" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C52" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F47" s="20"/>
-      <c r="G47" s="17" t="s">
+      <c r="F52" s="17"/>
+      <c r="G52" s="14" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B48" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C48" s="17" t="s">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B53" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C53" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F48" s="20"/>
-      <c r="G48" s="17" t="s">
+      <c r="F53" s="17"/>
+      <c r="G53" s="14" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B49" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C49" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D49" s="17" t="s">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B54" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D54" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="F49" s="20"/>
-      <c r="G49" s="17" t="s">
+      <c r="F54" s="17"/>
+      <c r="G54" s="14" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B50" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C50" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D50" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="E50" s="17" t="s">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B55" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C55" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D55" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E55" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="F50" s="20"/>
-      <c r="G50" s="17" t="s">
+      <c r="F55" s="17"/>
+      <c r="G55" s="14" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B51" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C51" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D51" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="E51" s="17" t="s">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B56" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C56" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D56" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E56" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="F51" s="20"/>
-      <c r="G51" s="17" t="s">
+      <c r="F56" s="17"/>
+      <c r="G56" s="14" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B52" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C52" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D52" s="17" t="s">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B57" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C57" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D57" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="F52" s="20"/>
-      <c r="G52" s="17" t="s">
+      <c r="F57" s="17"/>
+      <c r="G57" s="14" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B53" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C53" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D53" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="E53" s="17" t="s">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B58" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C58" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D58" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E58" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="F53" s="20"/>
-      <c r="G53" s="17" t="s">
+      <c r="F58" s="17"/>
+      <c r="G58" s="14" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B54" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C54" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D54" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="E54" s="17" t="s">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B59" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C59" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D59" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E59" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="F54" s="20"/>
-      <c r="G54" s="17" t="s">
+      <c r="F59" s="17"/>
+      <c r="G59" s="14" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B55" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C55" s="17" t="s">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B60" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C60" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="F55" s="20"/>
-      <c r="G55" s="17" t="s">
+      <c r="F60" s="17"/>
+      <c r="G60" s="14" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B56" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C56" s="17" t="s">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B61" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C61" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="F56" s="20"/>
-      <c r="G56" s="17" t="s">
+      <c r="F61" s="17"/>
+      <c r="G61" s="14" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B57" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C57" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D57" s="17" t="s">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B62" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C62" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D62" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="F57" s="20"/>
-      <c r="G57" s="17" t="s">
+      <c r="F62" s="17"/>
+      <c r="G62" s="14" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B58" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C58" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D58" s="17" t="s">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B63" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C63" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D63" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="F58" s="20"/>
-      <c r="G58" s="17" t="s">
+      <c r="F63" s="17"/>
+      <c r="G63" s="14" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B59" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C59" s="17" t="s">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B64" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C64" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="F59" s="20"/>
-      <c r="G59" s="17" t="s">
+      <c r="F64" s="17"/>
+      <c r="G64" s="14" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B60" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C60" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D60" s="17" t="s">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B65" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C65" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D65" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="F60" s="20"/>
-      <c r="G60" s="17" t="s">
+      <c r="F65" s="17"/>
+      <c r="G65" s="14" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B61" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C61" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D61" s="17" t="s">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B66" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C66" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D66" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="F61" s="20"/>
-      <c r="G61" s="17" t="s">
+      <c r="F66" s="17"/>
+      <c r="G66" s="14" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B62" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C62" s="17" t="s">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B67" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C67" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="F62" s="20"/>
-      <c r="G62" s="17" t="s">
+      <c r="F67" s="17"/>
+      <c r="G67" s="14" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B63" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C63" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D63" s="17" t="s">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B68" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C68" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D68" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="F63" s="20"/>
-      <c r="G63" s="17" t="s">
+      <c r="F68" s="17"/>
+      <c r="G68" s="14" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B64" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C64" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D64" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="E64" s="17" t="s">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B69" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C69" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D69" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E69" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="F64" s="20"/>
-      <c r="G64" s="17" t="s">
+      <c r="F69" s="17"/>
+      <c r="G69" s="14" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B65" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C65" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D65" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="E65" s="17" t="s">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B70" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C70" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D70" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E70" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="F65" s="20"/>
-      <c r="G65" s="17" t="s">
+      <c r="F70" s="17"/>
+      <c r="G70" s="14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B66" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C66" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D66" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="E66" s="17" t="s">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B71" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C71" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D71" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E71" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="F66" s="20"/>
-      <c r="G66" s="17" t="s">
+      <c r="F71" s="17"/>
+      <c r="G71" s="14" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B67" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C67" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D67" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="E67" s="17" t="s">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B72" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C72" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D72" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E72" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="F67" s="20"/>
-      <c r="G67" s="17" t="s">
+      <c r="F72" s="17"/>
+      <c r="G72" s="14" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B68" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C68" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D68" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="E68" s="17" t="s">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B73" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C73" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D73" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E73" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="F68" s="20"/>
-      <c r="G68" s="17" t="s">
+      <c r="F73" s="17"/>
+      <c r="G73" s="14" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="17" t="s">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="F69" s="20"/>
-      <c r="G69" s="17" t="s">
+      <c r="F74" s="17"/>
+      <c r="G74" s="14" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B70" s="17" t="s">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B75" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F70" s="20"/>
-      <c r="G70" s="17" t="s">
+      <c r="F75" s="17"/>
+      <c r="G75" s="14" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B71" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C71" s="17" t="s">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B76" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C76" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="F71" s="20"/>
-      <c r="G71" s="17" t="s">
+      <c r="F76" s="17"/>
+      <c r="G76" s="14" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B72" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C72" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D72" s="17" t="s">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B77" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C77" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D77" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="F72" s="20"/>
-      <c r="G72" s="17" t="s">
+      <c r="F77" s="17"/>
+      <c r="G77" s="14" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B73" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C73" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D73" s="17" t="s">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B78" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C78" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D78" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="F73" s="20"/>
-      <c r="G73" s="17" t="s">
+      <c r="F78" s="17"/>
+      <c r="G78" s="14" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B74" s="17" t="s">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B79" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="F74" s="20"/>
-      <c r="G74" s="17" t="s">
+      <c r="F79" s="17"/>
+      <c r="G79" s="14" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B75" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C75" s="17" t="s">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B80" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C80" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F75" s="20"/>
-      <c r="G75" s="17" t="s">
+      <c r="F80" s="17"/>
+      <c r="G80" s="14" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B76" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C76" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D76" s="17" t="s">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B81" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C81" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D81" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="F76" s="20"/>
-      <c r="G76" s="17" t="s">
+      <c r="F81" s="17"/>
+      <c r="G81" s="14" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B77" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C77" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D77" s="17" t="s">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B82" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C82" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D82" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="F77" s="20"/>
-      <c r="G77" s="17" t="s">
+      <c r="F82" s="17"/>
+      <c r="G82" s="14" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B78" s="17" t="s">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B83" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="C78" s="17"/>
-      <c r="D78" s="17"/>
-      <c r="F78" s="20"/>
-      <c r="G78" s="17" t="s">
+      <c r="C83" s="14"/>
+      <c r="D83" s="14"/>
+      <c r="F83" s="17"/>
+      <c r="G83" s="14" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B79" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C79" s="17" t="s">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B84" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C84" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D79" s="17"/>
-      <c r="F79" s="20"/>
-      <c r="G79" s="17" t="s">
+      <c r="D84" s="14"/>
+      <c r="F84" s="17"/>
+      <c r="G84" s="14" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B80" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C80" s="17" t="s">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B85" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C85" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D80" s="17"/>
-      <c r="F80" s="20"/>
-      <c r="G80" s="17" t="s">
+      <c r="D85" s="14"/>
+      <c r="F85" s="17"/>
+      <c r="G85" s="14" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B81" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C81" s="17" t="s">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B86" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C86" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="F81" s="20"/>
-      <c r="G81" s="17" t="s">
+      <c r="F86" s="17"/>
+      <c r="G86" s="14" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B82" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C82" s="17" t="s">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B87" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C87" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="F82" s="20"/>
-      <c r="G82" s="17" t="s">
+      <c r="F87" s="17"/>
+      <c r="G87" s="14" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B83" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C83" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D83" s="17" t="s">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B88" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C88" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D88" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="F83" s="20"/>
-      <c r="G83" s="17" t="s">
+      <c r="F88" s="17"/>
+      <c r="G88" s="14" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B84" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C84" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D84" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="E84" s="17" t="s">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B89" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C89" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D89" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E89" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="F84" s="20"/>
-      <c r="G84" s="17" t="s">
+      <c r="F89" s="17"/>
+      <c r="G89" s="14" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B85" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C85" s="17" t="s">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B90" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C90" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="F85" s="20"/>
-      <c r="G85" s="17" t="s">
+      <c r="F90" s="17"/>
+      <c r="G90" s="14" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B86" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C86" s="17" t="s">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B91" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C91" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="F86" s="20"/>
-      <c r="G86" s="17" t="s">
+      <c r="F91" s="17"/>
+      <c r="G91" s="14" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B87" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C87" s="17" t="s">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B92" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C92" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="F87" s="20"/>
-      <c r="G87" s="17" t="s">
+      <c r="F92" s="17"/>
+      <c r="G92" s="14" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B88" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C88" s="17" t="s">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B93" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C93" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="F88" s="20"/>
-      <c r="G88" s="17" t="s">
+      <c r="F93" s="17"/>
+      <c r="G93" s="14" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B89" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C89" s="17" t="s">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B94" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C94" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="D89" s="19" t="s">
+      <c r="D94" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="F89" s="20"/>
-      <c r="G89" s="17" t="s">
+      <c r="F94" s="17"/>
+      <c r="G94" s="14" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B90" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C90" s="17" t="s">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B95" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C95" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="F90" s="20"/>
-      <c r="G90" s="17" t="s">
+      <c r="F95" s="17"/>
+      <c r="G95" s="14" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B91" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C91" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D91" s="17" t="s">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B96" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C96" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D96" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="F91" s="20"/>
-      <c r="G91" s="17" t="s">
+      <c r="F96" s="17"/>
+      <c r="G96" s="14" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B92" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C92" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D92" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="E92" s="17" t="s">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B97" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C97" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D97" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E97" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="F92" s="20"/>
-      <c r="G92" s="17" t="s">
+      <c r="F97" s="17"/>
+      <c r="G97" s="14" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B93" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C93" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D93" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="E93" s="17" t="s">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B98" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C98" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D98" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E98" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="F93" s="20"/>
-      <c r="G93" s="17" t="s">
+      <c r="F98" s="17"/>
+      <c r="G98" s="14" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B94" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C94" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D94" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="E94" s="17" t="s">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B99" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C99" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D99" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E99" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="F94" s="20"/>
-      <c r="G94" s="17" t="s">
+      <c r="F99" s="17"/>
+      <c r="G99" s="14" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B95" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C95" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D95" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="E95" s="17" t="s">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B100" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C100" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D100" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E100" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="F95" s="20"/>
-      <c r="G95" s="17" t="s">
+      <c r="F100" s="17"/>
+      <c r="G100" s="14" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B96" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C96" s="17" t="s">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B101" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C101" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="F96" s="20"/>
-      <c r="G96" s="17" t="s">
+      <c r="F101" s="17"/>
+      <c r="G101" s="14" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="17"/>
-      <c r="B97" s="17"/>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="17"/>
-      <c r="B98" s="17"/>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="17"/>
-      <c r="B99" s="17"/>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="17"/>
-      <c r="B100" s="17"/>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="17"/>
-      <c r="B101" s="17"/>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="17"/>
-      <c r="B102" s="17"/>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="17"/>
-      <c r="B103" s="17"/>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="17"/>
-      <c r="B104" s="17"/>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="17"/>
-      <c r="B105" s="17"/>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="17"/>
-      <c r="B106" s="17"/>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="17"/>
-      <c r="B107" s="17"/>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="17"/>
-      <c r="B108" s="17"/>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="17"/>
-      <c r="B109" s="17"/>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="17"/>
-      <c r="B110" s="17"/>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="17"/>
-      <c r="B111" s="17"/>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="17"/>
-      <c r="B112" s="17"/>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" s="14"/>
+      <c r="B102" s="14"/>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" s="14"/>
+      <c r="B103" s="14"/>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" s="14"/>
+      <c r="B104" s="14"/>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" s="14"/>
+      <c r="B105" s="14"/>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" s="14"/>
+      <c r="B106" s="14"/>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" s="14"/>
+      <c r="B107" s="14"/>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" s="14"/>
+      <c r="B108" s="14"/>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" s="14"/>
+      <c r="B109" s="14"/>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" s="14"/>
+      <c r="B110" s="14"/>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" s="14"/>
+      <c r="B111" s="14"/>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" s="14"/>
+      <c r="B112" s="14"/>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="17"/>
-      <c r="B113" s="17"/>
+      <c r="A113" s="14"/>
+      <c r="B113" s="14"/>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="17"/>
-      <c r="B114" s="17"/>
+      <c r="A114" s="14"/>
+      <c r="B114" s="14"/>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="17"/>
-      <c r="B115" s="17"/>
+      <c r="A115" s="14"/>
+      <c r="B115" s="14"/>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="17"/>
-      <c r="B116" s="17"/>
+      <c r="A116" s="14"/>
+      <c r="B116" s="14"/>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="17"/>
-      <c r="B117" s="17"/>
+      <c r="A117" s="14"/>
+      <c r="B117" s="14"/>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="17"/>
-      <c r="B118" s="17"/>
+      <c r="A118" s="14"/>
+      <c r="B118" s="14"/>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="17"/>
-      <c r="B119" s="17"/>
+      <c r="A119" s="14"/>
+      <c r="B119" s="14"/>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="17"/>
-      <c r="B120" s="17"/>
+      <c r="A120" s="14"/>
+      <c r="B120" s="14"/>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="17"/>
-      <c r="B121" s="17"/>
+      <c r="A121" s="14"/>
+      <c r="B121" s="14"/>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="17"/>
-      <c r="B122" s="17"/>
+      <c r="A122" s="14"/>
+      <c r="B122" s="14"/>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="17"/>
-      <c r="B123" s="17"/>
+      <c r="A123" s="14"/>
+      <c r="B123" s="14"/>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" s="17"/>
-      <c r="B124" s="17"/>
+      <c r="A124" s="14"/>
+      <c r="B124" s="14"/>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" s="17"/>
-      <c r="B125" s="17"/>
+      <c r="A125" s="14"/>
+      <c r="B125" s="14"/>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" s="17"/>
-      <c r="B126" s="17"/>
+      <c r="A126" s="14"/>
+      <c r="B126" s="14"/>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" s="17"/>
-      <c r="B127" s="17"/>
+      <c r="A127" s="14"/>
+      <c r="B127" s="14"/>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" s="17"/>
-      <c r="B128" s="17"/>
+      <c r="A128" s="14"/>
+      <c r="B128" s="14"/>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="17"/>
-      <c r="B129" s="17"/>
+      <c r="A129" s="14"/>
+      <c r="B129" s="14"/>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="17"/>
-      <c r="B130" s="17"/>
+      <c r="A130" s="14"/>
+      <c r="B130" s="14"/>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="17"/>
-      <c r="B131" s="17"/>
+      <c r="A131" s="14"/>
+      <c r="B131" s="14"/>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="17"/>
-      <c r="B132" s="17"/>
+      <c r="A132" s="14"/>
+      <c r="B132" s="14"/>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="17"/>
-      <c r="B133" s="17"/>
+      <c r="A133" s="14"/>
+      <c r="B133" s="14"/>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="17"/>
-      <c r="B134" s="17"/>
+      <c r="A134" s="14"/>
+      <c r="B134" s="14"/>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="17"/>
-      <c r="B135" s="17"/>
+      <c r="A135" s="14"/>
+      <c r="B135" s="14"/>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="17"/>
-      <c r="B136" s="17"/>
+      <c r="A136" s="14"/>
+      <c r="B136" s="14"/>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="17"/>
-      <c r="B137" s="17"/>
+      <c r="A137" s="14"/>
+      <c r="B137" s="14"/>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" s="17"/>
-      <c r="B138" s="17"/>
+      <c r="A138" s="14"/>
+      <c r="B138" s="14"/>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" s="17"/>
+      <c r="A139" s="14"/>
+      <c r="B139" s="14"/>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" s="17"/>
+      <c r="A140" s="14"/>
+      <c r="B140" s="14"/>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="17"/>
+      <c r="A141" s="14"/>
+      <c r="B141" s="14"/>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" s="17"/>
+      <c r="A142" s="14"/>
+      <c r="B142" s="14"/>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" s="17"/>
+      <c r="A143" s="14"/>
+      <c r="B143" s="14"/>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" s="17"/>
+      <c r="A144" s="14"/>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" s="17"/>
+      <c r="A145" s="14"/>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" s="17"/>
+      <c r="A146" s="14"/>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" s="17"/>
+      <c r="A147" s="14"/>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148" s="17"/>
+      <c r="A148" s="14"/>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A149" s="17"/>
+      <c r="A149" s="14"/>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" s="17"/>
+      <c r="A150" s="14"/>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151" s="17"/>
+      <c r="A151" s="14"/>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152" s="17"/>
+      <c r="A152" s="14"/>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" s="17"/>
+      <c r="A153" s="14"/>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154" s="17"/>
+      <c r="A154" s="14"/>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155" s="17"/>
+      <c r="A155" s="14"/>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A156" s="17"/>
+      <c r="A156" s="14"/>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A157" s="17"/>
+      <c r="A157" s="14"/>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158" s="17"/>
+      <c r="A158" s="14"/>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A159" s="17"/>
+      <c r="A159" s="14"/>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A160" s="17"/>
+      <c r="A160" s="14"/>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161" s="17"/>
+      <c r="A161" s="14"/>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A162" s="17"/>
+      <c r="A162" s="14"/>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A163" s="17"/>
+      <c r="A163" s="14"/>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164" s="17"/>
+      <c r="A164" s="14"/>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A165" s="17"/>
+      <c r="A165" s="14"/>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A166" s="17"/>
+      <c r="A166" s="14"/>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A167" s="17"/>
+      <c r="A167" s="14"/>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" s="14"/>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" s="14"/>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" s="14"/>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" s="14"/>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Figured out that i am not able to make changes to a new user on the same page as it is created. Will need to redirect to a new profile page when creating a new user.
</commit_message>
<xml_diff>
--- a/Accessibility Chart.xlsx
+++ b/Accessibility Chart.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1251" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1262" uniqueCount="169">
   <si>
     <t>APP</t>
   </si>
@@ -524,6 +524,9 @@
   </si>
   <si>
     <t>uID</t>
+  </si>
+  <si>
+    <t>nameFull</t>
   </si>
 </sst>
 </file>
@@ -4898,10 +4901,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G172"/>
+  <dimension ref="A1:G174"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4933,6 +4936,9 @@
       <c r="B2" s="14" t="s">
         <v>77</v>
       </c>
+      <c r="C2" s="14" t="s">
+        <v>82</v>
+      </c>
       <c r="F2" s="17"/>
       <c r="G2" s="14" t="s">
         <v>114</v>
@@ -5010,7 +5016,7 @@
       </c>
       <c r="F7" s="17"/>
       <c r="G7" s="14" t="s">
-        <v>133</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -5219,6 +5225,9 @@
       <c r="B20" s="14" t="s">
         <v>86</v>
       </c>
+      <c r="C20" s="14" t="s">
+        <v>82</v>
+      </c>
       <c r="F20" s="17"/>
       <c r="G20" s="14" t="s">
         <v>126</v>
@@ -5447,9 +5456,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="14" t="s">
-        <v>81</v>
-      </c>
+      <c r="A36" s="14"/>
       <c r="B36" s="14" t="s">
         <v>81</v>
       </c>
@@ -5457,11 +5464,11 @@
         <v>81</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="F36" s="17"/>
       <c r="G36" s="14" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -5469,11 +5476,17 @@
         <v>81</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>30</v>
+        <v>81</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>105</v>
       </c>
       <c r="F37" s="17"/>
       <c r="G37" s="14" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -5481,14 +5494,11 @@
         <v>81</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C38" s="14" t="s">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="F38" s="17"/>
       <c r="G38" s="14" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -5499,14 +5509,11 @@
         <v>81</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D39" s="14" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="F39" s="17"/>
       <c r="G39" s="14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -5520,11 +5527,11 @@
         <v>81</v>
       </c>
       <c r="D40" s="14" t="s">
-        <v>105</v>
+        <v>29</v>
       </c>
       <c r="F40" s="17"/>
       <c r="G40" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -5532,13 +5539,17 @@
         <v>81</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
+        <v>81</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>82</v>
+      </c>
       <c r="F41" s="17"/>
       <c r="G41" s="14" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -5549,12 +5560,14 @@
         <v>81</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="D42" s="14"/>
+        <v>81</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>105</v>
+      </c>
       <c r="F42" s="17"/>
       <c r="G42" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -5562,15 +5575,13 @@
         <v>81</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C43" s="14" t="s">
-        <v>30</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="C43" s="14"/>
       <c r="D43" s="14"/>
       <c r="F43" s="17"/>
       <c r="G43" s="14" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -5581,11 +5592,12 @@
         <v>81</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>29</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="D44" s="14"/>
       <c r="F44" s="17"/>
       <c r="G44" s="14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -5596,11 +5608,12 @@
         <v>81</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>104</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="D45" s="14"/>
       <c r="F45" s="17"/>
       <c r="G45" s="14" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -5611,14 +5624,11 @@
         <v>81</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D46" s="14" t="s">
-        <v>94</v>
+        <v>29</v>
       </c>
       <c r="F46" s="17"/>
       <c r="G46" s="14" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -5629,17 +5639,11 @@
         <v>81</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D47" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E47" s="14" t="s">
-        <v>30</v>
+        <v>104</v>
       </c>
       <c r="F47" s="17"/>
       <c r="G47" s="14" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -5650,11 +5654,14 @@
         <v>81</v>
       </c>
       <c r="C48" s="14" t="s">
-        <v>31</v>
+        <v>81</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>94</v>
       </c>
       <c r="F48" s="17"/>
       <c r="G48" s="14" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -5665,11 +5672,17 @@
         <v>81</v>
       </c>
       <c r="C49" s="14" t="s">
-        <v>87</v>
+        <v>81</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E49" s="14" t="s">
+        <v>30</v>
       </c>
       <c r="F49" s="17"/>
       <c r="G49" s="14" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -5680,11 +5693,11 @@
         <v>81</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F50" s="17"/>
       <c r="G50" s="14" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -5695,11 +5708,11 @@
         <v>81</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>33</v>
+        <v>87</v>
       </c>
       <c r="F51" s="17"/>
       <c r="G51" s="14" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -5710,11 +5723,11 @@
         <v>81</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="F52" s="17"/>
       <c r="G52" s="14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -5725,11 +5738,11 @@
         <v>81</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F53" s="17"/>
       <c r="G53" s="14" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -5740,14 +5753,11 @@
         <v>81</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D54" s="14" t="s">
-        <v>94</v>
+        <v>9</v>
       </c>
       <c r="F54" s="17"/>
       <c r="G54" s="14" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -5758,17 +5768,11 @@
         <v>81</v>
       </c>
       <c r="C55" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D55" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E55" s="14" t="s">
-        <v>88</v>
+        <v>34</v>
       </c>
       <c r="F55" s="17"/>
       <c r="G55" s="14" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -5782,14 +5786,11 @@
         <v>81</v>
       </c>
       <c r="D56" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E56" s="14" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="F56" s="17"/>
       <c r="G56" s="14" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -5803,11 +5804,14 @@
         <v>81</v>
       </c>
       <c r="D57" s="14" t="s">
-        <v>94</v>
+        <v>81</v>
+      </c>
+      <c r="E57" s="14" t="s">
+        <v>88</v>
       </c>
       <c r="F57" s="17"/>
       <c r="G57" s="14" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -5824,11 +5828,11 @@
         <v>81</v>
       </c>
       <c r="E58" s="14" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F58" s="17"/>
       <c r="G58" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -5842,14 +5846,11 @@
         <v>81</v>
       </c>
       <c r="D59" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E59" s="14" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="F59" s="17"/>
       <c r="G59" s="14" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -5860,11 +5861,17 @@
         <v>81</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>90</v>
+        <v>81</v>
+      </c>
+      <c r="D60" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E60" s="14" t="s">
+        <v>88</v>
       </c>
       <c r="F60" s="17"/>
       <c r="G60" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -5875,11 +5882,17 @@
         <v>81</v>
       </c>
       <c r="C61" s="14" t="s">
-        <v>91</v>
+        <v>81</v>
+      </c>
+      <c r="D61" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E61" s="14" t="s">
+        <v>89</v>
       </c>
       <c r="F61" s="17"/>
       <c r="G61" s="14" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -5890,14 +5903,11 @@
         <v>81</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D62" s="14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F62" s="17"/>
       <c r="G62" s="14" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -5908,14 +5918,11 @@
         <v>81</v>
       </c>
       <c r="C63" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D63" s="14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F63" s="17"/>
       <c r="G63" s="14" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -5926,11 +5933,14 @@
         <v>81</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>95</v>
+        <v>81</v>
+      </c>
+      <c r="D64" s="14" t="s">
+        <v>92</v>
       </c>
       <c r="F64" s="17"/>
       <c r="G64" s="14" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -5944,11 +5954,11 @@
         <v>81</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F65" s="17"/>
       <c r="G65" s="14" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -5959,14 +5969,11 @@
         <v>81</v>
       </c>
       <c r="C66" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D66" s="14" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F66" s="17"/>
       <c r="G66" s="14" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -5977,11 +5984,14 @@
         <v>81</v>
       </c>
       <c r="C67" s="14" t="s">
-        <v>98</v>
+        <v>81</v>
+      </c>
+      <c r="D67" s="14" t="s">
+        <v>96</v>
       </c>
       <c r="F67" s="17"/>
       <c r="G67" s="14" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -5999,7 +6009,7 @@
       </c>
       <c r="F68" s="17"/>
       <c r="G68" s="14" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -6010,17 +6020,11 @@
         <v>81</v>
       </c>
       <c r="C69" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D69" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E69" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F69" s="17"/>
       <c r="G69" s="14" t="s">
-        <v>99</v>
+        <v>148</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -6034,14 +6038,11 @@
         <v>81</v>
       </c>
       <c r="D70" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E70" s="14" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F70" s="17"/>
       <c r="G70" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -6058,11 +6059,11 @@
         <v>81</v>
       </c>
       <c r="E71" s="14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F71" s="17"/>
       <c r="G71" s="14" t="s">
-        <v>151</v>
+        <v>99</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -6079,11 +6080,11 @@
         <v>81</v>
       </c>
       <c r="E72" s="14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F72" s="17"/>
       <c r="G72" s="14" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -6100,20 +6101,32 @@
         <v>81</v>
       </c>
       <c r="E73" s="14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F73" s="17"/>
       <c r="G73" s="14" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="14" t="s">
-        <v>106</v>
+        <v>81</v>
+      </c>
+      <c r="B74" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C74" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D74" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E74" s="14" t="s">
+        <v>102</v>
       </c>
       <c r="F74" s="17"/>
       <c r="G74" s="14" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -6121,26 +6134,29 @@
         <v>81</v>
       </c>
       <c r="B75" s="14" t="s">
-        <v>63</v>
+        <v>81</v>
+      </c>
+      <c r="C75" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D75" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E75" s="14" t="s">
+        <v>103</v>
       </c>
       <c r="F75" s="17"/>
       <c r="G75" s="14" t="s">
-        <v>128</v>
+        <v>155</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B76" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C76" s="14" t="s">
-        <v>30</v>
+        <v>106</v>
       </c>
       <c r="F76" s="17"/>
       <c r="G76" s="14" t="s">
-        <v>129</v>
+        <v>156</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -6148,17 +6164,11 @@
         <v>81</v>
       </c>
       <c r="B77" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C77" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D77" s="14" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="F77" s="17"/>
       <c r="G77" s="14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -6169,14 +6179,11 @@
         <v>81</v>
       </c>
       <c r="C78" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D78" s="14" t="s">
-        <v>105</v>
+        <v>30</v>
       </c>
       <c r="F78" s="17"/>
       <c r="G78" s="14" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -6184,11 +6191,17 @@
         <v>81</v>
       </c>
       <c r="B79" s="14" t="s">
-        <v>30</v>
+        <v>81</v>
+      </c>
+      <c r="C79" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D79" s="14" t="s">
+        <v>29</v>
       </c>
       <c r="F79" s="17"/>
       <c r="G79" s="14" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -6199,11 +6212,14 @@
         <v>81</v>
       </c>
       <c r="C80" s="14" t="s">
-        <v>63</v>
+        <v>81</v>
+      </c>
+      <c r="D80" s="14" t="s">
+        <v>105</v>
       </c>
       <c r="F80" s="17"/>
       <c r="G80" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -6211,17 +6227,11 @@
         <v>81</v>
       </c>
       <c r="B81" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C81" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D81" s="14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F81" s="17"/>
       <c r="G81" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -6232,14 +6242,11 @@
         <v>81</v>
       </c>
       <c r="C82" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D82" s="14" t="s">
-        <v>105</v>
+        <v>63</v>
       </c>
       <c r="F82" s="17"/>
       <c r="G82" s="14" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -6247,13 +6254,17 @@
         <v>81</v>
       </c>
       <c r="B83" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="C83" s="14"/>
-      <c r="D83" s="14"/>
+        <v>81</v>
+      </c>
+      <c r="C83" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D83" s="14" t="s">
+        <v>29</v>
+      </c>
       <c r="F83" s="17"/>
       <c r="G83" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -6264,12 +6275,14 @@
         <v>81</v>
       </c>
       <c r="C84" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="D84" s="14"/>
+        <v>81</v>
+      </c>
+      <c r="D84" s="14" t="s">
+        <v>105</v>
+      </c>
       <c r="F84" s="17"/>
       <c r="G84" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -6277,15 +6290,13 @@
         <v>81</v>
       </c>
       <c r="B85" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C85" s="14" t="s">
-        <v>30</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="C85" s="14"/>
       <c r="D85" s="14"/>
       <c r="F85" s="17"/>
       <c r="G85" s="14" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -6296,11 +6307,12 @@
         <v>81</v>
       </c>
       <c r="C86" s="14" t="s">
-        <v>29</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="D86" s="14"/>
       <c r="F86" s="17"/>
       <c r="G86" s="14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -6311,11 +6323,12 @@
         <v>81</v>
       </c>
       <c r="C87" s="14" t="s">
-        <v>104</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="D87" s="14"/>
       <c r="F87" s="17"/>
       <c r="G87" s="14" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -6326,14 +6339,11 @@
         <v>81</v>
       </c>
       <c r="C88" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D88" s="14" t="s">
-        <v>94</v>
+        <v>29</v>
       </c>
       <c r="F88" s="17"/>
       <c r="G88" s="14" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -6344,17 +6354,11 @@
         <v>81</v>
       </c>
       <c r="C89" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D89" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E89" s="14" t="s">
-        <v>30</v>
+        <v>104</v>
       </c>
       <c r="F89" s="17"/>
       <c r="G89" s="14" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -6365,11 +6369,14 @@
         <v>81</v>
       </c>
       <c r="C90" s="14" t="s">
-        <v>31</v>
+        <v>81</v>
+      </c>
+      <c r="D90" s="14" t="s">
+        <v>94</v>
       </c>
       <c r="F90" s="17"/>
       <c r="G90" s="14" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -6380,11 +6387,17 @@
         <v>81</v>
       </c>
       <c r="C91" s="14" t="s">
-        <v>32</v>
+        <v>81</v>
+      </c>
+      <c r="D91" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E91" s="14" t="s">
+        <v>30</v>
       </c>
       <c r="F91" s="17"/>
       <c r="G91" s="14" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -6395,11 +6408,11 @@
         <v>81</v>
       </c>
       <c r="C92" s="14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F92" s="17"/>
       <c r="G92" s="14" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -6410,11 +6423,11 @@
         <v>81</v>
       </c>
       <c r="C93" s="14" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="F93" s="17"/>
       <c r="G93" s="14" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -6425,14 +6438,11 @@
         <v>81</v>
       </c>
       <c r="C94" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="D94" s="16" t="s">
-        <v>112</v>
+        <v>33</v>
       </c>
       <c r="F94" s="17"/>
       <c r="G94" s="14" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -6443,11 +6453,11 @@
         <v>81</v>
       </c>
       <c r="C95" s="14" t="s">
-        <v>107</v>
+        <v>50</v>
       </c>
       <c r="F95" s="17"/>
       <c r="G95" s="14" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -6458,14 +6468,14 @@
         <v>81</v>
       </c>
       <c r="C96" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D96" s="14" t="s">
-        <v>65</v>
+        <v>111</v>
+      </c>
+      <c r="D96" s="16" t="s">
+        <v>112</v>
       </c>
       <c r="F96" s="17"/>
       <c r="G96" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -6476,17 +6486,11 @@
         <v>81</v>
       </c>
       <c r="C97" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D97" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E97" s="14" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F97" s="17"/>
       <c r="G97" s="14" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -6500,14 +6504,11 @@
         <v>81</v>
       </c>
       <c r="D98" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E98" s="14" t="s">
-        <v>108</v>
+        <v>65</v>
       </c>
       <c r="F98" s="17"/>
       <c r="G98" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -6524,11 +6525,11 @@
         <v>81</v>
       </c>
       <c r="E99" s="14" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F99" s="17"/>
       <c r="G99" s="14" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -6545,11 +6546,11 @@
         <v>81</v>
       </c>
       <c r="E100" s="14" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="F100" s="17"/>
       <c r="G100" s="14" t="s">
-        <v>141</v>
+        <v>160</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -6560,20 +6561,54 @@
         <v>81</v>
       </c>
       <c r="C101" s="14" t="s">
-        <v>54</v>
+        <v>81</v>
+      </c>
+      <c r="D101" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E101" s="14" t="s">
+        <v>109</v>
       </c>
       <c r="F101" s="17"/>
       <c r="G101" s="14" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B102" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C102" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D102" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E102" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="F102" s="17"/>
+      <c r="G102" s="14" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B103" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C103" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F103" s="17"/>
+      <c r="G103" s="14" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A102" s="14"/>
-      <c r="B102" s="14"/>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103" s="14"/>
-      <c r="B103" s="14"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="14"/>
@@ -6737,53 +6772,55 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="14"/>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B144" s="14"/>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="14"/>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B145" s="14"/>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="14"/>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="14"/>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="14"/>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="14"/>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="14"/>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="14"/>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="14"/>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="14"/>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="14"/>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="14"/>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="14"/>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="14"/>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="14"/>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="14"/>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="14"/>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
@@ -6821,6 +6858,12 @@
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" s="14"/>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" s="14"/>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Created "new-profile.html" to deal with new user's data. This page is only visited when user is created for the first time. Set all data needed to process on "profile.html" and updates database as well as html page when clicking the "UPDATE" button.
</commit_message>
<xml_diff>
--- a/Accessibility Chart.xlsx
+++ b/Accessibility Chart.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1262" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1283" uniqueCount="168">
   <si>
     <t>APP</t>
   </si>
@@ -362,9 +362,6 @@
   </si>
   <si>
     <t>employees</t>
-  </si>
-  <si>
-    <t>employed</t>
   </si>
   <si>
     <t>access</t>
@@ -1943,8 +1940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV93"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2056,7 +2053,7 @@
         <v>4</v>
       </c>
       <c r="L4" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2582,7 +2579,9 @@
       <c r="K23" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="L23" s="10"/>
+      <c r="L23" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="24" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
@@ -2614,7 +2613,9 @@
       <c r="K24" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="L24" s="10"/>
+      <c r="L24" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="25" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
@@ -2646,7 +2647,9 @@
       <c r="K25" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="L25" s="10"/>
+      <c r="L25" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="26" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
@@ -2678,7 +2681,9 @@
       <c r="K26" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="L26" s="10"/>
+      <c r="L26" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="27" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
@@ -2710,7 +2715,9 @@
       <c r="K27" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="L27" s="10"/>
+      <c r="L27" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="28" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
@@ -2742,7 +2749,9 @@
       <c r="K28" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="L28" s="10"/>
+      <c r="L28" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="29" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
@@ -2774,7 +2783,9 @@
       <c r="K29" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="L29" s="10"/>
+      <c r="L29" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="30" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
@@ -2806,7 +2817,9 @@
       <c r="K30" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="L30" s="10"/>
+      <c r="L30" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="31" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="11"/>
@@ -2838,7 +2851,9 @@
       <c r="K31" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="L31" s="10"/>
+      <c r="L31" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="32" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11"/>
@@ -2870,7 +2885,9 @@
       <c r="K32" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="L32" s="10"/>
+      <c r="L32" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="33" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
@@ -2902,7 +2919,9 @@
       <c r="K33" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="L33" s="10"/>
+      <c r="L33" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="34" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
@@ -2934,7 +2953,9 @@
       <c r="K34" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="L34" s="10"/>
+      <c r="L34" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="35" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
@@ -2966,7 +2987,9 @@
       <c r="K35" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="L35" s="10"/>
+      <c r="L35" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="36" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="11"/>
@@ -2998,7 +3021,9 @@
       <c r="K36" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="L36" s="10"/>
+      <c r="L36" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="37" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
@@ -3030,7 +3055,9 @@
       <c r="K37" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="L37" s="10"/>
+      <c r="L37" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="38" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11"/>
@@ -3062,7 +3089,9 @@
       <c r="K38" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="L38" s="10"/>
+      <c r="L38" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="39" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="11"/>
@@ -3094,7 +3123,9 @@
       <c r="K39" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="L39" s="10"/>
+      <c r="L39" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="40" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
@@ -3126,7 +3157,9 @@
       <c r="K40" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="L40" s="10"/>
+      <c r="L40" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="41" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="11"/>
@@ -3158,7 +3191,9 @@
       <c r="K41" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="L41" s="10"/>
+      <c r="L41" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="42" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="11"/>
@@ -3190,7 +3225,9 @@
       <c r="K42" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="L42" s="10"/>
+      <c r="L42" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="43" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="11"/>
@@ -3222,7 +3259,9 @@
       <c r="K43" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="L43" s="10"/>
+      <c r="L43" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="44" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
@@ -4904,7 +4943,7 @@
   <dimension ref="A1:G174"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4937,11 +4976,11 @@
         <v>77</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>82</v>
+        <v>165</v>
       </c>
       <c r="F2" s="17"/>
       <c r="G2" s="14" t="s">
-        <v>114</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -4952,11 +4991,11 @@
         <v>81</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F3" s="17"/>
       <c r="G3" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -4971,7 +5010,7 @@
       </c>
       <c r="F4" s="17"/>
       <c r="G4" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -4986,7 +5025,7 @@
       </c>
       <c r="F5" s="17"/>
       <c r="G5" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -5001,7 +5040,7 @@
       </c>
       <c r="F6" s="17"/>
       <c r="G6" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -5012,11 +5051,11 @@
         <v>81</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F7" s="17"/>
       <c r="G7" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -5031,7 +5070,7 @@
       </c>
       <c r="F8" s="17"/>
       <c r="G8" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -5046,7 +5085,7 @@
       </c>
       <c r="F9" s="17"/>
       <c r="G9" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -5061,7 +5100,7 @@
       </c>
       <c r="F10" s="17"/>
       <c r="G10" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -5076,7 +5115,7 @@
       </c>
       <c r="F11" s="17"/>
       <c r="G11" s="14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -5091,7 +5130,7 @@
       </c>
       <c r="F12" s="17"/>
       <c r="G12" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -5106,7 +5145,7 @@
       </c>
       <c r="F13" s="17"/>
       <c r="G13" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -5121,7 +5160,7 @@
       </c>
       <c r="F14" s="17"/>
       <c r="G14" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -5139,7 +5178,7 @@
       </c>
       <c r="F15" s="17"/>
       <c r="G15" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -5150,12 +5189,12 @@
         <v>81</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D16" s="14"/>
       <c r="F16" s="17"/>
       <c r="G16" s="14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -5173,7 +5212,7 @@
       </c>
       <c r="F17" s="17"/>
       <c r="G17" s="14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -5194,7 +5233,7 @@
       </c>
       <c r="F18" s="17"/>
       <c r="G18" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -5215,7 +5254,7 @@
       </c>
       <c r="F19" s="17"/>
       <c r="G19" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -5230,7 +5269,7 @@
       </c>
       <c r="F20" s="17"/>
       <c r="G20" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -5245,7 +5284,7 @@
       </c>
       <c r="F21" s="17"/>
       <c r="G21" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -5260,7 +5299,7 @@
       </c>
       <c r="F22" s="17"/>
       <c r="G22" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -5275,7 +5314,7 @@
       </c>
       <c r="F23" s="17"/>
       <c r="G23" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -5290,7 +5329,7 @@
       </c>
       <c r="F24" s="17"/>
       <c r="G24" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -5305,7 +5344,7 @@
       </c>
       <c r="F25" s="17"/>
       <c r="G25" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -5320,7 +5359,7 @@
       </c>
       <c r="F26" s="17"/>
       <c r="G26" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -5335,7 +5374,7 @@
       </c>
       <c r="F27" s="17"/>
       <c r="G27" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -5350,7 +5389,7 @@
       </c>
       <c r="F28" s="17"/>
       <c r="G28" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -5365,7 +5404,7 @@
       </c>
       <c r="F29" s="17"/>
       <c r="G29" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -5380,7 +5419,7 @@
       </c>
       <c r="F30" s="17"/>
       <c r="G30" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -5398,7 +5437,7 @@
       </c>
       <c r="F31" s="17"/>
       <c r="G31" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -5407,7 +5446,7 @@
       </c>
       <c r="F32" s="17"/>
       <c r="G32" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -5419,7 +5458,7 @@
       </c>
       <c r="F33" s="17"/>
       <c r="G33" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -5434,7 +5473,7 @@
       </c>
       <c r="F34" s="17"/>
       <c r="G34" s="14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -5452,7 +5491,7 @@
       </c>
       <c r="F35" s="17"/>
       <c r="G35" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -5468,7 +5507,7 @@
       </c>
       <c r="F36" s="17"/>
       <c r="G36" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -5486,7 +5525,7 @@
       </c>
       <c r="F37" s="17"/>
       <c r="G37" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -5498,7 +5537,7 @@
       </c>
       <c r="F38" s="17"/>
       <c r="G38" s="14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -5513,7 +5552,7 @@
       </c>
       <c r="F39" s="17"/>
       <c r="G39" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -5531,7 +5570,7 @@
       </c>
       <c r="F40" s="17"/>
       <c r="G40" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -5549,7 +5588,7 @@
       </c>
       <c r="F41" s="17"/>
       <c r="G41" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -5567,7 +5606,7 @@
       </c>
       <c r="F42" s="17"/>
       <c r="G42" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -5581,7 +5620,7 @@
       <c r="D43" s="14"/>
       <c r="F43" s="17"/>
       <c r="G43" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -5597,7 +5636,7 @@
       <c r="D44" s="14"/>
       <c r="F44" s="17"/>
       <c r="G44" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -5613,7 +5652,7 @@
       <c r="D45" s="14"/>
       <c r="F45" s="17"/>
       <c r="G45" s="14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -5628,7 +5667,7 @@
       </c>
       <c r="F46" s="17"/>
       <c r="G46" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -5643,7 +5682,7 @@
       </c>
       <c r="F47" s="17"/>
       <c r="G47" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -5661,7 +5700,7 @@
       </c>
       <c r="F48" s="17"/>
       <c r="G48" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -5682,7 +5721,7 @@
       </c>
       <c r="F49" s="17"/>
       <c r="G49" s="14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -5697,7 +5736,7 @@
       </c>
       <c r="F50" s="17"/>
       <c r="G50" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -5712,7 +5751,7 @@
       </c>
       <c r="F51" s="17"/>
       <c r="G51" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -5727,7 +5766,7 @@
       </c>
       <c r="F52" s="17"/>
       <c r="G52" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -5742,7 +5781,7 @@
       </c>
       <c r="F53" s="17"/>
       <c r="G53" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -5757,7 +5796,7 @@
       </c>
       <c r="F54" s="17"/>
       <c r="G54" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -5772,7 +5811,7 @@
       </c>
       <c r="F55" s="17"/>
       <c r="G55" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -5790,7 +5829,7 @@
       </c>
       <c r="F56" s="17"/>
       <c r="G56" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -5811,7 +5850,7 @@
       </c>
       <c r="F57" s="17"/>
       <c r="G57" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -5832,7 +5871,7 @@
       </c>
       <c r="F58" s="17"/>
       <c r="G58" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -5850,7 +5889,7 @@
       </c>
       <c r="F59" s="17"/>
       <c r="G59" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -5871,7 +5910,7 @@
       </c>
       <c r="F60" s="17"/>
       <c r="G60" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -5892,7 +5931,7 @@
       </c>
       <c r="F61" s="17"/>
       <c r="G61" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -5907,7 +5946,7 @@
       </c>
       <c r="F62" s="17"/>
       <c r="G62" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -5922,7 +5961,7 @@
       </c>
       <c r="F63" s="17"/>
       <c r="G63" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -5940,7 +5979,7 @@
       </c>
       <c r="F64" s="17"/>
       <c r="G64" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -5958,7 +5997,7 @@
       </c>
       <c r="F65" s="17"/>
       <c r="G65" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -5973,7 +6012,7 @@
       </c>
       <c r="F66" s="17"/>
       <c r="G66" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -5991,7 +6030,7 @@
       </c>
       <c r="F67" s="17"/>
       <c r="G67" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -6009,7 +6048,7 @@
       </c>
       <c r="F68" s="17"/>
       <c r="G68" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -6024,7 +6063,7 @@
       </c>
       <c r="F69" s="17"/>
       <c r="G69" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -6042,7 +6081,7 @@
       </c>
       <c r="F70" s="17"/>
       <c r="G70" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -6084,7 +6123,7 @@
       </c>
       <c r="F72" s="17"/>
       <c r="G72" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -6105,7 +6144,7 @@
       </c>
       <c r="F73" s="17"/>
       <c r="G73" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -6126,7 +6165,7 @@
       </c>
       <c r="F74" s="17"/>
       <c r="G74" s="14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -6147,7 +6186,7 @@
       </c>
       <c r="F75" s="17"/>
       <c r="G75" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -6156,7 +6195,7 @@
       </c>
       <c r="F76" s="17"/>
       <c r="G76" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -6168,7 +6207,7 @@
       </c>
       <c r="F77" s="17"/>
       <c r="G77" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -6183,7 +6222,7 @@
       </c>
       <c r="F78" s="17"/>
       <c r="G78" s="14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -6201,7 +6240,7 @@
       </c>
       <c r="F79" s="17"/>
       <c r="G79" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -6219,7 +6258,7 @@
       </c>
       <c r="F80" s="17"/>
       <c r="G80" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -6231,7 +6270,7 @@
       </c>
       <c r="F81" s="17"/>
       <c r="G81" s="14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -6246,7 +6285,7 @@
       </c>
       <c r="F82" s="17"/>
       <c r="G82" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -6264,7 +6303,7 @@
       </c>
       <c r="F83" s="17"/>
       <c r="G83" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -6282,7 +6321,7 @@
       </c>
       <c r="F84" s="17"/>
       <c r="G84" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -6296,7 +6335,7 @@
       <c r="D85" s="14"/>
       <c r="F85" s="17"/>
       <c r="G85" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -6312,7 +6351,7 @@
       <c r="D86" s="14"/>
       <c r="F86" s="17"/>
       <c r="G86" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -6328,7 +6367,7 @@
       <c r="D87" s="14"/>
       <c r="F87" s="17"/>
       <c r="G87" s="14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -6343,7 +6382,7 @@
       </c>
       <c r="F88" s="17"/>
       <c r="G88" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -6358,7 +6397,7 @@
       </c>
       <c r="F89" s="17"/>
       <c r="G89" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -6376,7 +6415,7 @@
       </c>
       <c r="F90" s="17"/>
       <c r="G90" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -6397,7 +6436,7 @@
       </c>
       <c r="F91" s="17"/>
       <c r="G91" s="14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -6412,7 +6451,7 @@
       </c>
       <c r="F92" s="17"/>
       <c r="G92" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -6427,7 +6466,7 @@
       </c>
       <c r="F93" s="17"/>
       <c r="G93" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -6442,7 +6481,7 @@
       </c>
       <c r="F94" s="17"/>
       <c r="G94" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -6457,7 +6496,7 @@
       </c>
       <c r="F95" s="17"/>
       <c r="G95" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -6475,7 +6514,7 @@
       </c>
       <c r="F96" s="17"/>
       <c r="G96" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -6490,7 +6529,7 @@
       </c>
       <c r="F97" s="17"/>
       <c r="G97" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -6508,7 +6547,7 @@
       </c>
       <c r="F98" s="17"/>
       <c r="G98" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -6529,7 +6568,7 @@
       </c>
       <c r="F99" s="17"/>
       <c r="G99" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -6550,7 +6589,7 @@
       </c>
       <c r="F100" s="17"/>
       <c r="G100" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -6571,7 +6610,7 @@
       </c>
       <c r="F101" s="17"/>
       <c r="G101" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -6592,7 +6631,7 @@
       </c>
       <c r="F102" s="17"/>
       <c r="G102" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -6607,7 +6646,7 @@
       </c>
       <c r="F103" s="17"/>
       <c r="G103" s="14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Started creating DPR page. Need to figure out how to select technicians from a drop down list to easily add them. Editing new-profile page to potentially add a "technicians" list in the database.
</commit_message>
<xml_diff>
--- a/Accessibility Chart.xlsx
+++ b/Accessibility Chart.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1283" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1324" uniqueCount="172">
   <si>
     <t>APP</t>
   </si>
@@ -524,6 +524,18 @@
   </si>
   <si>
     <t>nameFull</t>
+  </si>
+  <si>
+    <t>UserID</t>
+  </si>
+  <si>
+    <t>Submitted Initials</t>
+  </si>
+  <si>
+    <t>submittedInitials</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -4940,17 +4952,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G174"/>
+  <dimension ref="A1:H179"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" style="15" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" style="15" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" style="15" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="15" customWidth="1"/>
     <col min="4" max="4" width="12.140625" style="15" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" style="15" customWidth="1"/>
     <col min="6" max="6" width="1.42578125" style="15" customWidth="1"/>
@@ -4959,7 +4971,7 @@
     <col min="9" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>80</v>
       </c>
@@ -4968,7 +4980,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>81</v>
       </c>
@@ -4982,8 +4994,11 @@
       <c r="G2" s="14" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>81</v>
       </c>
@@ -4997,8 +5012,11 @@
       <c r="G3" s="14" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>81</v>
       </c>
@@ -5012,8 +5030,11 @@
       <c r="G4" s="14" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>81</v>
       </c>
@@ -5027,8 +5048,11 @@
       <c r="G5" s="14" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>81</v>
       </c>
@@ -5042,8 +5066,11 @@
       <c r="G6" s="14" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>81</v>
       </c>
@@ -5057,8 +5084,11 @@
       <c r="G7" s="14" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>81</v>
       </c>
@@ -5072,8 +5102,11 @@
       <c r="G8" s="14" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>81</v>
       </c>
@@ -5087,8 +5120,11 @@
       <c r="G9" s="14" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>81</v>
       </c>
@@ -5102,8 +5138,11 @@
       <c r="G10" s="14" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" s="14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>81</v>
       </c>
@@ -5117,8 +5156,11 @@
       <c r="G11" s="14" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>81</v>
       </c>
@@ -5132,8 +5174,11 @@
       <c r="G12" s="14" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" s="14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>81</v>
       </c>
@@ -5147,8 +5192,11 @@
       <c r="G13" s="14" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" s="14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>81</v>
       </c>
@@ -5162,8 +5210,11 @@
       <c r="G14" s="14" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" s="14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>81</v>
       </c>
@@ -5180,8 +5231,11 @@
       <c r="G15" s="14" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" s="14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>81</v>
       </c>
@@ -5196,8 +5250,9 @@
       <c r="G16" s="14" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" s="14"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>81</v>
       </c>
@@ -5214,8 +5269,9 @@
       <c r="G17" s="14" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" s="14"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>81</v>
       </c>
@@ -5235,8 +5291,9 @@
       <c r="G18" s="14" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" s="14"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>81</v>
       </c>
@@ -5256,8 +5313,9 @@
       <c r="G19" s="14" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" s="14"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>81</v>
       </c>
@@ -5272,7 +5330,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>81</v>
       </c>
@@ -5287,7 +5345,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>81</v>
       </c>
@@ -5302,7 +5360,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>81</v>
       </c>
@@ -5317,7 +5375,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
         <v>81</v>
       </c>
@@ -5325,14 +5383,14 @@
         <v>81</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>78</v>
+        <v>133</v>
       </c>
       <c r="F24" s="17"/>
       <c r="G24" s="14" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
         <v>81</v>
       </c>
@@ -5340,14 +5398,14 @@
         <v>81</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>21</v>
+        <v>78</v>
       </c>
       <c r="F25" s="17"/>
       <c r="G25" s="14" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
         <v>81</v>
       </c>
@@ -5355,14 +5413,14 @@
         <v>81</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>82</v>
+        <v>21</v>
       </c>
       <c r="F26" s="17"/>
       <c r="G26" s="14" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>81</v>
       </c>
@@ -5370,14 +5428,14 @@
         <v>81</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
       <c r="F27" s="17"/>
       <c r="G27" s="14" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
         <v>81</v>
       </c>
@@ -5385,14 +5443,14 @@
         <v>81</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>83</v>
+        <v>23</v>
       </c>
       <c r="F28" s="17"/>
       <c r="G28" s="14" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>81</v>
       </c>
@@ -5400,14 +5458,14 @@
         <v>81</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>25</v>
+        <v>83</v>
       </c>
       <c r="F29" s="17"/>
       <c r="G29" s="14" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
         <v>81</v>
       </c>
@@ -5415,14 +5473,14 @@
         <v>81</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>84</v>
+        <v>25</v>
       </c>
       <c r="F30" s="17"/>
       <c r="G30" s="14" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
         <v>81</v>
       </c>
@@ -5430,38 +5488,46 @@
         <v>81</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D31" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F31" s="17"/>
       <c r="G31" s="14" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
-        <v>27</v>
+        <v>81</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>85</v>
       </c>
       <c r="F32" s="17"/>
       <c r="G32" s="14" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>81</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>63</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
       <c r="F33" s="17"/>
       <c r="G33" s="14" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
         <v>81</v>
       </c>
@@ -5469,48 +5535,36 @@
         <v>81</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>30</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="D34" s="14"/>
       <c r="F34" s="17"/>
       <c r="G34" s="14" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B35" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C35" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D35" s="14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F35" s="17"/>
       <c r="G35" s="14" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="14"/>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="14" t="s">
+        <v>81</v>
+      </c>
       <c r="B36" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C36" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D36" s="14" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="F36" s="17"/>
       <c r="G36" s="14" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
         <v>81</v>
       </c>
@@ -5518,44 +5572,48 @@
         <v>81</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D37" s="14" t="s">
-        <v>105</v>
+        <v>30</v>
       </c>
       <c r="F37" s="17"/>
       <c r="G37" s="14" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
         <v>81</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>30</v>
+        <v>81</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>29</v>
       </c>
       <c r="F38" s="17"/>
       <c r="G38" s="14" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="14" t="s">
-        <v>81</v>
-      </c>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="14"/>
       <c r="B39" s="14" t="s">
         <v>81</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>63</v>
+        <v>81</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>168</v>
       </c>
       <c r="F39" s="17"/>
       <c r="G39" s="14" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
         <v>81</v>
       </c>
@@ -5566,32 +5624,26 @@
         <v>81</v>
       </c>
       <c r="D40" s="14" t="s">
-        <v>29</v>
+        <v>105</v>
       </c>
       <c r="F40" s="17"/>
       <c r="G40" s="14" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
         <v>81</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C41" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D41" s="14" t="s">
-        <v>82</v>
+        <v>30</v>
       </c>
       <c r="F41" s="17"/>
       <c r="G41" s="14" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
         <v>81</v>
       </c>
@@ -5599,31 +5651,32 @@
         <v>81</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D42" s="14" t="s">
-        <v>105</v>
+        <v>63</v>
       </c>
       <c r="F42" s="17"/>
       <c r="G42" s="14" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
         <v>81</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
+        <v>81</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>29</v>
+      </c>
       <c r="F43" s="17"/>
       <c r="G43" s="14" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
         <v>81</v>
       </c>
@@ -5631,15 +5684,17 @@
         <v>81</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="D44" s="14"/>
+        <v>81</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>168</v>
+      </c>
       <c r="F44" s="17"/>
       <c r="G44" s="14" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
         <v>81</v>
       </c>
@@ -5647,30 +5702,31 @@
         <v>81</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D45" s="14"/>
+        <v>81</v>
+      </c>
+      <c r="D45" s="14" t="s">
+        <v>105</v>
+      </c>
       <c r="F45" s="17"/>
       <c r="G45" s="14" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
         <v>81</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C46" s="14" t="s">
-        <v>29</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
       <c r="F46" s="17"/>
       <c r="G46" s="14" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
         <v>81</v>
       </c>
@@ -5678,14 +5734,18 @@
         <v>81</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>104</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="D47" s="14"/>
       <c r="F47" s="17"/>
       <c r="G47" s="14" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+      <c r="H47" s="14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
         <v>81</v>
       </c>
@@ -5693,17 +5753,18 @@
         <v>81</v>
       </c>
       <c r="C48" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D48" s="14" t="s">
-        <v>94</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="D48" s="14"/>
       <c r="F48" s="17"/>
       <c r="G48" s="14" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+      <c r="H48" s="14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
         <v>81</v>
       </c>
@@ -5711,20 +5772,14 @@
         <v>81</v>
       </c>
       <c r="C49" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D49" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E49" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F49" s="17"/>
       <c r="G49" s="14" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
         <v>81</v>
       </c>
@@ -5732,14 +5787,14 @@
         <v>81</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>31</v>
+        <v>169</v>
       </c>
       <c r="F50" s="17"/>
       <c r="G50" s="14" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
         <v>81</v>
       </c>
@@ -5747,14 +5802,14 @@
         <v>81</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="F51" s="17"/>
       <c r="G51" s="14" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
         <v>81</v>
       </c>
@@ -5762,14 +5817,17 @@
         <v>81</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>32</v>
+        <v>81</v>
+      </c>
+      <c r="D52" s="14" t="s">
+        <v>94</v>
       </c>
       <c r="F52" s="17"/>
       <c r="G52" s="14" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
         <v>81</v>
       </c>
@@ -5777,14 +5835,20 @@
         <v>81</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>33</v>
+        <v>81</v>
+      </c>
+      <c r="D53" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E53" s="14" t="s">
+        <v>30</v>
       </c>
       <c r="F53" s="17"/>
       <c r="G53" s="14" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
         <v>81</v>
       </c>
@@ -5792,14 +5856,17 @@
         <v>81</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="F54" s="17"/>
       <c r="G54" s="14" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="H54" s="14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
         <v>81</v>
       </c>
@@ -5807,14 +5874,17 @@
         <v>81</v>
       </c>
       <c r="C55" s="14" t="s">
-        <v>34</v>
+        <v>87</v>
       </c>
       <c r="F55" s="17"/>
       <c r="G55" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+      <c r="H55" s="14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
         <v>81</v>
       </c>
@@ -5822,17 +5892,17 @@
         <v>81</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D56" s="14" t="s">
-        <v>94</v>
+        <v>32</v>
       </c>
       <c r="F56" s="17"/>
       <c r="G56" s="14" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="H56" s="14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
         <v>81</v>
       </c>
@@ -5840,20 +5910,17 @@
         <v>81</v>
       </c>
       <c r="C57" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D57" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E57" s="14" t="s">
-        <v>88</v>
+        <v>33</v>
       </c>
       <c r="F57" s="17"/>
       <c r="G57" s="14" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+      <c r="H57" s="14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
         <v>81</v>
       </c>
@@ -5861,20 +5928,17 @@
         <v>81</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D58" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E58" s="14" t="s">
-        <v>89</v>
+        <v>9</v>
       </c>
       <c r="F58" s="17"/>
       <c r="G58" s="14" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+      <c r="H58" s="14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="14" t="s">
         <v>81</v>
       </c>
@@ -5882,17 +5946,17 @@
         <v>81</v>
       </c>
       <c r="C59" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D59" s="14" t="s">
-        <v>94</v>
+        <v>34</v>
       </c>
       <c r="F59" s="17"/>
       <c r="G59" s="14" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+      <c r="H59" s="14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="14" t="s">
         <v>81</v>
       </c>
@@ -5903,17 +5967,14 @@
         <v>81</v>
       </c>
       <c r="D60" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E60" s="14" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="F60" s="17"/>
       <c r="G60" s="14" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="14" t="s">
         <v>81</v>
       </c>
@@ -5927,14 +5988,14 @@
         <v>81</v>
       </c>
       <c r="E61" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F61" s="17"/>
       <c r="G61" s="14" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="14" t="s">
         <v>81</v>
       </c>
@@ -5942,14 +6003,20 @@
         <v>81</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>90</v>
+        <v>81</v>
+      </c>
+      <c r="D62" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E62" s="14" t="s">
+        <v>89</v>
       </c>
       <c r="F62" s="17"/>
       <c r="G62" s="14" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="s">
         <v>81</v>
       </c>
@@ -5957,14 +6024,17 @@
         <v>81</v>
       </c>
       <c r="C63" s="14" t="s">
-        <v>91</v>
+        <v>81</v>
+      </c>
+      <c r="D63" s="14" t="s">
+        <v>94</v>
       </c>
       <c r="F63" s="17"/>
       <c r="G63" s="14" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="14" t="s">
         <v>81</v>
       </c>
@@ -5975,11 +6045,14 @@
         <v>81</v>
       </c>
       <c r="D64" s="14" t="s">
-        <v>92</v>
+        <v>81</v>
+      </c>
+      <c r="E64" s="14" t="s">
+        <v>88</v>
       </c>
       <c r="F64" s="17"/>
       <c r="G64" s="14" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -5993,11 +6066,14 @@
         <v>81</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>93</v>
+        <v>81</v>
+      </c>
+      <c r="E65" s="14" t="s">
+        <v>89</v>
       </c>
       <c r="F65" s="17"/>
       <c r="G65" s="14" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -6008,11 +6084,11 @@
         <v>81</v>
       </c>
       <c r="C66" s="14" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F66" s="17"/>
       <c r="G66" s="14" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -6023,14 +6099,11 @@
         <v>81</v>
       </c>
       <c r="C67" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D67" s="14" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="F67" s="17"/>
       <c r="G67" s="14" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -6044,11 +6117,11 @@
         <v>81</v>
       </c>
       <c r="D68" s="14" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F68" s="17"/>
       <c r="G68" s="14" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -6059,11 +6132,14 @@
         <v>81</v>
       </c>
       <c r="C69" s="14" t="s">
-        <v>98</v>
+        <v>81</v>
+      </c>
+      <c r="D69" s="14" t="s">
+        <v>93</v>
       </c>
       <c r="F69" s="17"/>
       <c r="G69" s="14" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -6074,14 +6150,11 @@
         <v>81</v>
       </c>
       <c r="C70" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D70" s="14" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F70" s="17"/>
       <c r="G70" s="14" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -6095,14 +6168,11 @@
         <v>81</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E71" s="14" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F71" s="17"/>
       <c r="G71" s="14" t="s">
-        <v>99</v>
+        <v>145</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -6116,14 +6186,11 @@
         <v>81</v>
       </c>
       <c r="D72" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E72" s="14" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F72" s="17"/>
       <c r="G72" s="14" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -6134,17 +6201,11 @@
         <v>81</v>
       </c>
       <c r="C73" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D73" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E73" s="14" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F73" s="17"/>
       <c r="G73" s="14" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -6158,14 +6219,11 @@
         <v>81</v>
       </c>
       <c r="D74" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E74" s="14" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F74" s="17"/>
       <c r="G74" s="14" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -6182,20 +6240,32 @@
         <v>81</v>
       </c>
       <c r="E75" s="14" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F75" s="17"/>
       <c r="G75" s="14" t="s">
-        <v>154</v>
+        <v>99</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="14" t="s">
-        <v>106</v>
+        <v>81</v>
+      </c>
+      <c r="B76" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C76" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D76" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E76" s="14" t="s">
+        <v>100</v>
       </c>
       <c r="F76" s="17"/>
       <c r="G76" s="14" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -6203,11 +6273,20 @@
         <v>81</v>
       </c>
       <c r="B77" s="14" t="s">
-        <v>63</v>
+        <v>81</v>
+      </c>
+      <c r="C77" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D77" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E77" s="14" t="s">
+        <v>101</v>
       </c>
       <c r="F77" s="17"/>
       <c r="G77" s="14" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -6218,11 +6297,17 @@
         <v>81</v>
       </c>
       <c r="C78" s="14" t="s">
-        <v>30</v>
+        <v>81</v>
+      </c>
+      <c r="D78" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E78" s="14" t="s">
+        <v>102</v>
       </c>
       <c r="F78" s="17"/>
       <c r="G78" s="14" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -6236,29 +6321,23 @@
         <v>81</v>
       </c>
       <c r="D79" s="14" t="s">
-        <v>29</v>
+        <v>81</v>
+      </c>
+      <c r="E79" s="14" t="s">
+        <v>103</v>
       </c>
       <c r="F79" s="17"/>
       <c r="G79" s="14" t="s">
-        <v>129</v>
+        <v>154</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B80" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C80" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D80" s="14" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F80" s="17"/>
       <c r="G80" s="14" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -6266,11 +6345,11 @@
         <v>81</v>
       </c>
       <c r="B81" s="14" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="F81" s="17"/>
       <c r="G81" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -6281,11 +6360,11 @@
         <v>81</v>
       </c>
       <c r="C82" s="14" t="s">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="F82" s="17"/>
       <c r="G82" s="14" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -6329,13 +6408,11 @@
         <v>81</v>
       </c>
       <c r="B85" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="C85" s="14"/>
-      <c r="D85" s="14"/>
+        <v>30</v>
+      </c>
       <c r="F85" s="17"/>
       <c r="G85" s="14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -6348,7 +6425,6 @@
       <c r="C86" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D86" s="14"/>
       <c r="F86" s="17"/>
       <c r="G86" s="14" t="s">
         <v>127</v>
@@ -6362,12 +6438,14 @@
         <v>81</v>
       </c>
       <c r="C87" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D87" s="14"/>
+        <v>81</v>
+      </c>
+      <c r="D87" s="14" t="s">
+        <v>29</v>
+      </c>
       <c r="F87" s="17"/>
       <c r="G87" s="14" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -6378,11 +6456,14 @@
         <v>81</v>
       </c>
       <c r="C88" s="14" t="s">
-        <v>29</v>
+        <v>81</v>
+      </c>
+      <c r="D88" s="14" t="s">
+        <v>105</v>
       </c>
       <c r="F88" s="17"/>
       <c r="G88" s="14" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -6390,14 +6471,13 @@
         <v>81</v>
       </c>
       <c r="B89" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C89" s="14" t="s">
-        <v>104</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="C89" s="14"/>
+      <c r="D89" s="14"/>
       <c r="F89" s="17"/>
       <c r="G89" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -6408,14 +6488,12 @@
         <v>81</v>
       </c>
       <c r="C90" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D90" s="14" t="s">
-        <v>94</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="D90" s="14"/>
       <c r="F90" s="17"/>
       <c r="G90" s="14" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -6426,14 +6504,9 @@
         <v>81</v>
       </c>
       <c r="C91" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D91" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E91" s="14" t="s">
         <v>30</v>
       </c>
+      <c r="D91" s="14"/>
       <c r="F91" s="17"/>
       <c r="G91" s="14" t="s">
         <v>128</v>
@@ -6447,11 +6520,11 @@
         <v>81</v>
       </c>
       <c r="C92" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F92" s="17"/>
       <c r="G92" s="14" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -6462,11 +6535,11 @@
         <v>81</v>
       </c>
       <c r="C93" s="14" t="s">
-        <v>32</v>
+        <v>169</v>
       </c>
       <c r="F93" s="17"/>
       <c r="G93" s="14" t="s">
-        <v>136</v>
+        <v>170</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -6477,11 +6550,11 @@
         <v>81</v>
       </c>
       <c r="C94" s="14" t="s">
-        <v>33</v>
+        <v>104</v>
       </c>
       <c r="F94" s="17"/>
       <c r="G94" s="14" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -6492,11 +6565,14 @@
         <v>81</v>
       </c>
       <c r="C95" s="14" t="s">
-        <v>50</v>
+        <v>81</v>
+      </c>
+      <c r="D95" s="14" t="s">
+        <v>94</v>
       </c>
       <c r="F95" s="17"/>
       <c r="G95" s="14" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -6507,14 +6583,17 @@
         <v>81</v>
       </c>
       <c r="C96" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="D96" s="16" t="s">
-        <v>112</v>
+        <v>81</v>
+      </c>
+      <c r="D96" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E96" s="14" t="s">
+        <v>30</v>
       </c>
       <c r="F96" s="17"/>
       <c r="G96" s="14" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -6525,11 +6604,11 @@
         <v>81</v>
       </c>
       <c r="C97" s="14" t="s">
-        <v>107</v>
+        <v>31</v>
       </c>
       <c r="F97" s="17"/>
       <c r="G97" s="14" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -6540,14 +6619,11 @@
         <v>81</v>
       </c>
       <c r="C98" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D98" s="14" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="F98" s="17"/>
       <c r="G98" s="14" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -6558,17 +6634,11 @@
         <v>81</v>
       </c>
       <c r="C99" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D99" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E99" s="14" t="s">
-        <v>110</v>
+        <v>33</v>
       </c>
       <c r="F99" s="17"/>
       <c r="G99" s="14" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -6579,17 +6649,11 @@
         <v>81</v>
       </c>
       <c r="C100" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D100" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E100" s="14" t="s">
-        <v>108</v>
+        <v>50</v>
       </c>
       <c r="F100" s="17"/>
       <c r="G100" s="14" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -6600,17 +6664,14 @@
         <v>81</v>
       </c>
       <c r="C101" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D101" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E101" s="14" t="s">
-        <v>109</v>
+        <v>111</v>
+      </c>
+      <c r="D101" s="16" t="s">
+        <v>112</v>
       </c>
       <c r="F101" s="17"/>
       <c r="G101" s="14" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -6621,17 +6682,11 @@
         <v>81</v>
       </c>
       <c r="C102" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D102" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E102" s="14" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="F102" s="17"/>
       <c r="G102" s="14" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -6642,32 +6697,114 @@
         <v>81</v>
       </c>
       <c r="C103" s="14" t="s">
-        <v>54</v>
+        <v>81</v>
+      </c>
+      <c r="D103" s="14" t="s">
+        <v>65</v>
       </c>
       <c r="F103" s="17"/>
       <c r="G103" s="14" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B104" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C104" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D104" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E104" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="F104" s="17"/>
+      <c r="G104" s="14" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B105" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C105" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D105" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E105" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="F105" s="17"/>
+      <c r="G105" s="14" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B106" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C106" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D106" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E106" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="F106" s="17"/>
+      <c r="G106" s="14" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B107" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C107" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D107" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E107" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="F107" s="17"/>
+      <c r="G107" s="14" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B108" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C108" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F108" s="17"/>
+      <c r="G108" s="14" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A104" s="14"/>
-      <c r="B104" s="14"/>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="14"/>
-      <c r="B105" s="14"/>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="14"/>
-      <c r="B106" s="14"/>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" s="14"/>
-      <c r="B107" s="14"/>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="14"/>
-      <c r="B108" s="14"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="14"/>
@@ -6819,18 +6956,23 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="14"/>
+      <c r="B146" s="14"/>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="14"/>
+      <c r="B147" s="14"/>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="14"/>
+      <c r="B148" s="14"/>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="14"/>
+      <c r="B149" s="14"/>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="14"/>
+      <c r="B150" s="14"/>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="14"/>
@@ -6903,6 +7045,21 @@
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" s="14"/>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" s="14"/>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" s="14"/>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" s="14"/>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" s="14"/>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modified DPR page with more fields. Solved problem of having to display a list of all techs. Need to now figure out how to select more than one. Modified profile and index page to properly show user.displayName.
</commit_message>
<xml_diff>
--- a/Accessibility Chart.xlsx
+++ b/Accessibility Chart.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1324" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1363" uniqueCount="174">
   <si>
     <t>APP</t>
   </si>
@@ -536,6 +536,12 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>contactNum</t>
+  </si>
+  <si>
+    <t>Contact #</t>
   </si>
 </sst>
 </file>
@@ -4952,10 +4958,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H179"/>
+  <dimension ref="A1:H187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I64" sqref="I64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5168,11 +5174,11 @@
         <v>81</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>83</v>
+        <v>173</v>
       </c>
       <c r="F12" s="17"/>
       <c r="G12" s="14" t="s">
-        <v>121</v>
+        <v>172</v>
       </c>
       <c r="H12" s="14" t="s">
         <v>171</v>
@@ -5186,11 +5192,11 @@
         <v>81</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>25</v>
+        <v>83</v>
       </c>
       <c r="F13" s="17"/>
       <c r="G13" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H13" s="14" t="s">
         <v>171</v>
@@ -5204,11 +5210,11 @@
         <v>81</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>84</v>
+        <v>25</v>
       </c>
       <c r="F14" s="17"/>
       <c r="G14" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H14" s="14" t="s">
         <v>171</v>
@@ -5222,14 +5228,11 @@
         <v>81</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F15" s="17"/>
       <c r="G15" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H15" s="14" t="s">
         <v>171</v>
@@ -5243,14 +5246,18 @@
         <v>81</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="D16" s="14"/>
+        <v>81</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>85</v>
+      </c>
       <c r="F16" s="17"/>
       <c r="G16" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="H16" s="14"/>
+        <v>124</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
@@ -5260,14 +5267,12 @@
         <v>81</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>30</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="D17" s="14"/>
       <c r="F17" s="17"/>
       <c r="G17" s="14" t="s">
-        <v>128</v>
+        <v>164</v>
       </c>
       <c r="H17" s="14"/>
     </row>
@@ -5282,14 +5287,11 @@
         <v>81</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="F18" s="17"/>
       <c r="G18" s="14" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H18" s="14"/>
     </row>
@@ -5307,11 +5309,11 @@
         <v>81</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>105</v>
+        <v>63</v>
       </c>
       <c r="F19" s="17"/>
       <c r="G19" s="14" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H19" s="14"/>
     </row>
@@ -5320,29 +5322,36 @@
         <v>81</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>105</v>
       </c>
       <c r="F20" s="17"/>
       <c r="G20" s="14" t="s">
-        <v>125</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="H20" s="14"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>81</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="F21" s="17"/>
       <c r="G21" s="14" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -5353,11 +5362,11 @@
         <v>81</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>19</v>
+        <v>79</v>
       </c>
       <c r="F22" s="17"/>
       <c r="G22" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -5368,11 +5377,11 @@
         <v>81</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F23" s="17"/>
       <c r="G23" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -5383,11 +5392,11 @@
         <v>81</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>133</v>
+        <v>20</v>
       </c>
       <c r="F24" s="17"/>
       <c r="G24" s="14" t="s">
-        <v>167</v>
+        <v>116</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -5398,11 +5407,11 @@
         <v>81</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>78</v>
+        <v>133</v>
       </c>
       <c r="F25" s="17"/>
       <c r="G25" s="14" t="s">
-        <v>117</v>
+        <v>167</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -5413,11 +5422,11 @@
         <v>81</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>21</v>
+        <v>78</v>
       </c>
       <c r="F26" s="17"/>
       <c r="G26" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -5428,11 +5437,11 @@
         <v>81</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>82</v>
+        <v>21</v>
       </c>
       <c r="F27" s="17"/>
       <c r="G27" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -5443,11 +5452,11 @@
         <v>81</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
       <c r="F28" s="17"/>
       <c r="G28" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -5458,11 +5467,11 @@
         <v>81</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>83</v>
+        <v>23</v>
       </c>
       <c r="F29" s="17"/>
       <c r="G29" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -5473,12 +5482,13 @@
         <v>81</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>25</v>
+        <v>173</v>
       </c>
       <c r="F30" s="17"/>
       <c r="G30" s="14" t="s">
-        <v>122</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="H30" s="14"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
@@ -5488,11 +5498,11 @@
         <v>81</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F31" s="17"/>
       <c r="G31" s="14" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -5503,31 +5513,29 @@
         <v>81</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="F32" s="17"/>
       <c r="G32" s="14" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>81</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
+        <v>81</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>84</v>
+      </c>
       <c r="F33" s="17"/>
       <c r="G33" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
         <v>81</v>
       </c>
@@ -5535,85 +5543,83 @@
         <v>81</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="D34" s="14"/>
+        <v>81</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>85</v>
+      </c>
       <c r="F34" s="17"/>
       <c r="G34" s="14" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>27</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
       <c r="F35" s="17"/>
       <c r="G35" s="14" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
         <v>81</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>63</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="D36" s="14"/>
       <c r="F36" s="17"/>
       <c r="G36" s="14" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B37" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C37" s="14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F37" s="17"/>
       <c r="G37" s="14" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
         <v>81</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C38" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D38" s="14" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="F38" s="17"/>
       <c r="G38" s="14" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="14" t="s">
+        <v>81</v>
+      </c>
       <c r="B39" s="14" t="s">
         <v>81</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D39" s="14" t="s">
-        <v>168</v>
+        <v>30</v>
       </c>
       <c r="F39" s="17"/>
       <c r="G39" s="14" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
         <v>81</v>
       </c>
@@ -5624,26 +5630,30 @@
         <v>81</v>
       </c>
       <c r="D40" s="14" t="s">
-        <v>105</v>
+        <v>29</v>
       </c>
       <c r="F40" s="17"/>
       <c r="G40" s="14" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="14" t="s">
-        <v>81</v>
-      </c>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="14"/>
       <c r="B41" s="14" t="s">
-        <v>30</v>
+        <v>81</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>168</v>
       </c>
       <c r="F41" s="17"/>
       <c r="G41" s="14" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
         <v>81</v>
       </c>
@@ -5651,32 +5661,29 @@
         <v>81</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>63</v>
+        <v>81</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>105</v>
       </c>
       <c r="F42" s="17"/>
       <c r="G42" s="14" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
         <v>81</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C43" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D43" s="14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F43" s="17"/>
       <c r="G43" s="14" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
         <v>81</v>
       </c>
@@ -5684,17 +5691,14 @@
         <v>81</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D44" s="14" t="s">
-        <v>168</v>
+        <v>63</v>
       </c>
       <c r="F44" s="17"/>
       <c r="G44" s="14" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
         <v>81</v>
       </c>
@@ -5705,28 +5709,32 @@
         <v>81</v>
       </c>
       <c r="D45" s="14" t="s">
-        <v>105</v>
+        <v>29</v>
       </c>
       <c r="F45" s="17"/>
       <c r="G45" s="14" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
         <v>81</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="C46" s="14"/>
-      <c r="D46" s="14"/>
+        <v>81</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>168</v>
+      </c>
       <c r="F46" s="17"/>
       <c r="G46" s="14" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
         <v>81</v>
       </c>
@@ -5734,34 +5742,28 @@
         <v>81</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="D47" s="14"/>
+        <v>81</v>
+      </c>
+      <c r="D47" s="14" t="s">
+        <v>105</v>
+      </c>
       <c r="F47" s="17"/>
       <c r="G47" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="H47" s="14" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
         <v>81</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C48" s="14" t="s">
-        <v>30</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="C48" s="14"/>
       <c r="D48" s="14"/>
       <c r="F48" s="17"/>
       <c r="G48" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="H48" s="14" t="s">
-        <v>171</v>
+        <v>130</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -5772,11 +5774,15 @@
         <v>81</v>
       </c>
       <c r="C49" s="14" t="s">
-        <v>29</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="D49" s="14"/>
       <c r="F49" s="17"/>
       <c r="G49" s="14" t="s">
-        <v>129</v>
+        <v>127</v>
+      </c>
+      <c r="H49" s="14" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -5787,11 +5793,15 @@
         <v>81</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>169</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="D50" s="14"/>
       <c r="F50" s="17"/>
       <c r="G50" s="14" t="s">
-        <v>170</v>
+        <v>128</v>
+      </c>
+      <c r="H50" s="14" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -5802,11 +5812,11 @@
         <v>81</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>104</v>
+        <v>29</v>
       </c>
       <c r="F51" s="17"/>
       <c r="G51" s="14" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -5817,14 +5827,11 @@
         <v>81</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D52" s="14" t="s">
-        <v>94</v>
+        <v>169</v>
       </c>
       <c r="F52" s="17"/>
       <c r="G52" s="14" t="s">
-        <v>132</v>
+        <v>170</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -5835,17 +5842,11 @@
         <v>81</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D53" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E53" s="14" t="s">
-        <v>30</v>
+        <v>104</v>
       </c>
       <c r="F53" s="17"/>
       <c r="G53" s="14" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -5856,14 +5857,14 @@
         <v>81</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>31</v>
+        <v>81</v>
+      </c>
+      <c r="D54" s="14" t="s">
+        <v>94</v>
       </c>
       <c r="F54" s="17"/>
       <c r="G54" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="H54" s="14" t="s">
-        <v>171</v>
+        <v>132</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -5874,14 +5875,17 @@
         <v>81</v>
       </c>
       <c r="C55" s="14" t="s">
-        <v>87</v>
+        <v>81</v>
+      </c>
+      <c r="D55" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E55" s="14" t="s">
+        <v>30</v>
       </c>
       <c r="F55" s="17"/>
       <c r="G55" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="H55" s="14" t="s">
-        <v>171</v>
+        <v>128</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -5892,11 +5896,11 @@
         <v>81</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F56" s="17"/>
       <c r="G56" s="14" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H56" s="14" t="s">
         <v>171</v>
@@ -5910,11 +5914,11 @@
         <v>81</v>
       </c>
       <c r="C57" s="14" t="s">
-        <v>33</v>
+        <v>87</v>
       </c>
       <c r="F57" s="17"/>
       <c r="G57" s="14" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H57" s="14" t="s">
         <v>171</v>
@@ -5928,11 +5932,11 @@
         <v>81</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="F58" s="17"/>
       <c r="G58" s="14" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H58" s="14" t="s">
         <v>171</v>
@@ -5946,11 +5950,11 @@
         <v>81</v>
       </c>
       <c r="C59" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F59" s="17"/>
       <c r="G59" s="14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H59" s="14" t="s">
         <v>171</v>
@@ -5964,14 +5968,14 @@
         <v>81</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D60" s="14" t="s">
-        <v>94</v>
+        <v>9</v>
       </c>
       <c r="F60" s="17"/>
       <c r="G60" s="14" t="s">
-        <v>132</v>
+        <v>138</v>
+      </c>
+      <c r="H60" s="14" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -5982,17 +5986,14 @@
         <v>81</v>
       </c>
       <c r="C61" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D61" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E61" s="14" t="s">
-        <v>88</v>
+        <v>34</v>
       </c>
       <c r="F61" s="17"/>
       <c r="G61" s="14" t="s">
-        <v>141</v>
+        <v>139</v>
+      </c>
+      <c r="H61" s="14" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -6006,14 +6007,11 @@
         <v>81</v>
       </c>
       <c r="D62" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E62" s="14" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="F62" s="17"/>
       <c r="G62" s="14" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -6027,11 +6025,14 @@
         <v>81</v>
       </c>
       <c r="D63" s="14" t="s">
-        <v>94</v>
+        <v>81</v>
+      </c>
+      <c r="E63" s="14" t="s">
+        <v>88</v>
       </c>
       <c r="F63" s="17"/>
       <c r="G63" s="14" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -6048,11 +6049,11 @@
         <v>81</v>
       </c>
       <c r="E64" s="14" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F64" s="17"/>
       <c r="G64" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -6066,14 +6067,11 @@
         <v>81</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E65" s="14" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="F65" s="17"/>
       <c r="G65" s="14" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -6084,11 +6082,17 @@
         <v>81</v>
       </c>
       <c r="C66" s="14" t="s">
-        <v>90</v>
+        <v>81</v>
+      </c>
+      <c r="D66" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E66" s="14" t="s">
+        <v>88</v>
       </c>
       <c r="F66" s="17"/>
       <c r="G66" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -6099,11 +6103,17 @@
         <v>81</v>
       </c>
       <c r="C67" s="14" t="s">
-        <v>91</v>
+        <v>81</v>
+      </c>
+      <c r="D67" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E67" s="14" t="s">
+        <v>89</v>
       </c>
       <c r="F67" s="17"/>
       <c r="G67" s="14" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -6114,14 +6124,11 @@
         <v>81</v>
       </c>
       <c r="C68" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D68" s="14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F68" s="17"/>
       <c r="G68" s="14" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -6132,14 +6139,11 @@
         <v>81</v>
       </c>
       <c r="C69" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D69" s="14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F69" s="17"/>
       <c r="G69" s="14" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -6150,11 +6154,14 @@
         <v>81</v>
       </c>
       <c r="C70" s="14" t="s">
-        <v>95</v>
+        <v>81</v>
+      </c>
+      <c r="D70" s="14" t="s">
+        <v>92</v>
       </c>
       <c r="F70" s="17"/>
       <c r="G70" s="14" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -6168,11 +6175,11 @@
         <v>81</v>
       </c>
       <c r="D71" s="14" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F71" s="17"/>
       <c r="G71" s="14" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -6183,14 +6190,11 @@
         <v>81</v>
       </c>
       <c r="C72" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D72" s="14" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F72" s="17"/>
       <c r="G72" s="14" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -6201,11 +6205,14 @@
         <v>81</v>
       </c>
       <c r="C73" s="14" t="s">
-        <v>98</v>
+        <v>81</v>
+      </c>
+      <c r="D73" s="14" t="s">
+        <v>96</v>
       </c>
       <c r="F73" s="17"/>
       <c r="G73" s="14" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -6223,7 +6230,7 @@
       </c>
       <c r="F74" s="17"/>
       <c r="G74" s="14" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -6234,17 +6241,11 @@
         <v>81</v>
       </c>
       <c r="C75" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D75" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E75" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F75" s="17"/>
       <c r="G75" s="14" t="s">
-        <v>99</v>
+        <v>147</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -6258,14 +6259,11 @@
         <v>81</v>
       </c>
       <c r="D76" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E76" s="14" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F76" s="17"/>
       <c r="G76" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -6282,11 +6280,11 @@
         <v>81</v>
       </c>
       <c r="E77" s="14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F77" s="17"/>
       <c r="G77" s="14" t="s">
-        <v>150</v>
+        <v>99</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -6303,11 +6301,11 @@
         <v>81</v>
       </c>
       <c r="E78" s="14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F78" s="17"/>
       <c r="G78" s="14" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -6324,20 +6322,32 @@
         <v>81</v>
       </c>
       <c r="E79" s="14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F79" s="17"/>
       <c r="G79" s="14" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="14" t="s">
-        <v>106</v>
+        <v>81</v>
+      </c>
+      <c r="B80" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C80" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D80" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E80" s="14" t="s">
+        <v>102</v>
       </c>
       <c r="F80" s="17"/>
       <c r="G80" s="14" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -6345,26 +6355,29 @@
         <v>81</v>
       </c>
       <c r="B81" s="14" t="s">
-        <v>63</v>
+        <v>81</v>
+      </c>
+      <c r="C81" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D81" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E81" s="14" t="s">
+        <v>103</v>
       </c>
       <c r="F81" s="17"/>
       <c r="G81" s="14" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B82" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C82" s="14" t="s">
-        <v>30</v>
+        <v>106</v>
       </c>
       <c r="F82" s="17"/>
       <c r="G82" s="14" t="s">
-        <v>128</v>
+        <v>155</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -6372,17 +6385,11 @@
         <v>81</v>
       </c>
       <c r="B83" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C83" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D83" s="14" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="F83" s="17"/>
       <c r="G83" s="14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -6393,14 +6400,11 @@
         <v>81</v>
       </c>
       <c r="C84" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D84" s="14" t="s">
-        <v>105</v>
+        <v>30</v>
       </c>
       <c r="F84" s="17"/>
       <c r="G84" s="14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -6408,11 +6412,17 @@
         <v>81</v>
       </c>
       <c r="B85" s="14" t="s">
-        <v>30</v>
+        <v>81</v>
+      </c>
+      <c r="C85" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D85" s="14" t="s">
+        <v>29</v>
       </c>
       <c r="F85" s="17"/>
       <c r="G85" s="14" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -6423,11 +6433,14 @@
         <v>81</v>
       </c>
       <c r="C86" s="14" t="s">
-        <v>63</v>
+        <v>81</v>
+      </c>
+      <c r="D86" s="14" t="s">
+        <v>105</v>
       </c>
       <c r="F86" s="17"/>
       <c r="G86" s="14" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -6441,11 +6454,11 @@
         <v>81</v>
       </c>
       <c r="D87" s="14" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F87" s="17"/>
       <c r="G87" s="14" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -6459,11 +6472,11 @@
         <v>81</v>
       </c>
       <c r="D88" s="14" t="s">
-        <v>105</v>
+        <v>33</v>
       </c>
       <c r="F88" s="17"/>
       <c r="G88" s="14" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -6471,13 +6484,17 @@
         <v>81</v>
       </c>
       <c r="B89" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="C89" s="14"/>
-      <c r="D89" s="14"/>
+        <v>81</v>
+      </c>
+      <c r="C89" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D89" s="14" t="s">
+        <v>89</v>
+      </c>
       <c r="F89" s="17"/>
       <c r="G89" s="14" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -6485,15 +6502,11 @@
         <v>81</v>
       </c>
       <c r="B90" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C90" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="D90" s="14"/>
+        <v>30</v>
+      </c>
       <c r="F90" s="17"/>
       <c r="G90" s="14" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -6504,12 +6517,11 @@
         <v>81</v>
       </c>
       <c r="C91" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D91" s="14"/>
+        <v>63</v>
+      </c>
       <c r="F91" s="17"/>
       <c r="G91" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -6520,6 +6532,9 @@
         <v>81</v>
       </c>
       <c r="C92" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D92" s="14" t="s">
         <v>29</v>
       </c>
       <c r="F92" s="17"/>
@@ -6535,11 +6550,14 @@
         <v>81</v>
       </c>
       <c r="C93" s="14" t="s">
-        <v>169</v>
+        <v>81</v>
+      </c>
+      <c r="D93" s="14" t="s">
+        <v>105</v>
       </c>
       <c r="F93" s="17"/>
       <c r="G93" s="14" t="s">
-        <v>170</v>
+        <v>130</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -6550,11 +6568,14 @@
         <v>81</v>
       </c>
       <c r="C94" s="14" t="s">
-        <v>104</v>
+        <v>81</v>
+      </c>
+      <c r="D94" s="14" t="s">
+        <v>32</v>
       </c>
       <c r="F94" s="17"/>
       <c r="G94" s="14" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -6568,11 +6589,11 @@
         <v>81</v>
       </c>
       <c r="D95" s="14" t="s">
-        <v>94</v>
+        <v>33</v>
       </c>
       <c r="F95" s="17"/>
       <c r="G95" s="14" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -6586,14 +6607,11 @@
         <v>81</v>
       </c>
       <c r="D96" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E96" s="14" t="s">
-        <v>30</v>
+        <v>89</v>
       </c>
       <c r="F96" s="17"/>
       <c r="G96" s="14" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -6601,14 +6619,13 @@
         <v>81</v>
       </c>
       <c r="B97" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C97" s="14" t="s">
-        <v>31</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="C97" s="14"/>
+      <c r="D97" s="14"/>
       <c r="F97" s="17"/>
       <c r="G97" s="14" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -6619,11 +6636,12 @@
         <v>81</v>
       </c>
       <c r="C98" s="14" t="s">
-        <v>32</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="D98" s="14"/>
       <c r="F98" s="17"/>
       <c r="G98" s="14" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -6634,11 +6652,12 @@
         <v>81</v>
       </c>
       <c r="C99" s="14" t="s">
-        <v>33</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="D99" s="14"/>
       <c r="F99" s="17"/>
       <c r="G99" s="14" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -6649,11 +6668,11 @@
         <v>81</v>
       </c>
       <c r="C100" s="14" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="F100" s="17"/>
       <c r="G100" s="14" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -6664,14 +6683,11 @@
         <v>81</v>
       </c>
       <c r="C101" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="D101" s="16" t="s">
-        <v>112</v>
+        <v>169</v>
       </c>
       <c r="F101" s="17"/>
       <c r="G101" s="14" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -6682,11 +6698,11 @@
         <v>81</v>
       </c>
       <c r="C102" s="14" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F102" s="17"/>
       <c r="G102" s="14" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -6700,11 +6716,11 @@
         <v>81</v>
       </c>
       <c r="D103" s="14" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="F103" s="17"/>
       <c r="G103" s="14" t="s">
-        <v>157</v>
+        <v>132</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -6721,11 +6737,11 @@
         <v>81</v>
       </c>
       <c r="E104" s="14" t="s">
-        <v>110</v>
+        <v>30</v>
       </c>
       <c r="F104" s="17"/>
       <c r="G104" s="14" t="s">
-        <v>158</v>
+        <v>128</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -6736,17 +6752,11 @@
         <v>81</v>
       </c>
       <c r="C105" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D105" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E105" s="14" t="s">
-        <v>108</v>
+        <v>31</v>
       </c>
       <c r="F105" s="17"/>
       <c r="G105" s="14" t="s">
-        <v>159</v>
+        <v>134</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -6757,17 +6767,11 @@
         <v>81</v>
       </c>
       <c r="C106" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D106" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E106" s="14" t="s">
-        <v>109</v>
+        <v>32</v>
       </c>
       <c r="F106" s="17"/>
       <c r="G106" s="14" t="s">
-        <v>160</v>
+        <v>136</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -6778,17 +6782,11 @@
         <v>81</v>
       </c>
       <c r="C107" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D107" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E107" s="14" t="s">
-        <v>89</v>
+        <v>33</v>
       </c>
       <c r="F107" s="17"/>
       <c r="G107" s="14" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
@@ -6799,90 +6797,208 @@
         <v>81</v>
       </c>
       <c r="C108" s="14" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F108" s="17"/>
       <c r="G108" s="14" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B109" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C109" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D109" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="F109" s="17"/>
+      <c r="G109" s="14" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B110" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C110" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F110" s="17"/>
+      <c r="G110" s="14" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B111" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C111" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D111" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="F111" s="17"/>
+      <c r="G111" s="14" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B112" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C112" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D112" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E112" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="F112" s="17"/>
+      <c r="G112" s="14" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B113" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C113" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D113" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E113" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="F113" s="17"/>
+      <c r="G113" s="14" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B114" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C114" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D114" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E114" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="F114" s="17"/>
+      <c r="G114" s="14" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B115" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C115" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D115" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E115" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="F115" s="17"/>
+      <c r="G115" s="14" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B116" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C116" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F116" s="17"/>
+      <c r="G116" s="14" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A109" s="14"/>
-      <c r="B109" s="14"/>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A110" s="14"/>
-      <c r="B110" s="14"/>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A111" s="14"/>
-      <c r="B111" s="14"/>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A112" s="14"/>
-      <c r="B112" s="14"/>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="14"/>
-      <c r="B113" s="14"/>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="14"/>
-      <c r="B114" s="14"/>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="14"/>
-      <c r="B115" s="14"/>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="14"/>
-      <c r="B116" s="14"/>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="14"/>
       <c r="B117" s="14"/>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="14"/>
       <c r="B118" s="14"/>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="14"/>
       <c r="B119" s="14"/>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="14"/>
       <c r="B120" s="14"/>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="14"/>
       <c r="B121" s="14"/>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="14"/>
       <c r="B122" s="14"/>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="14"/>
       <c r="B123" s="14"/>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="14"/>
       <c r="B124" s="14"/>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="14"/>
       <c r="B125" s="14"/>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="14"/>
       <c r="B126" s="14"/>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="14"/>
       <c r="B127" s="14"/>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="14"/>
       <c r="B128" s="14"/>
     </row>
@@ -6976,27 +7092,35 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="14"/>
+      <c r="B151" s="14"/>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="14"/>
+      <c r="B152" s="14"/>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="14"/>
+      <c r="B153" s="14"/>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="14"/>
+      <c r="B154" s="14"/>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="14"/>
+      <c r="B155" s="14"/>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="14"/>
+      <c r="B156" s="14"/>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="14"/>
+      <c r="B157" s="14"/>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="14"/>
+      <c r="B158" s="14"/>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="14"/>
@@ -7060,6 +7184,30 @@
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" s="14"/>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" s="14"/>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" s="14"/>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" s="14"/>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" s="14"/>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" s="14"/>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" s="14"/>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" s="14"/>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finished more of DPR page. Trying to figure out how to dynamically add new fields when needed. Need to figure out how to save pages as PDF.
</commit_message>
<xml_diff>
--- a/Accessibility Chart.xlsx
+++ b/Accessibility Chart.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1363" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1378" uniqueCount="174">
   <si>
     <t>APP</t>
   </si>
@@ -4958,10 +4958,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H187"/>
+  <dimension ref="A1:H190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I64" sqref="I64"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5585,11 +5585,20 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
-        <v>27</v>
+        <v>81</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>122</v>
       </c>
       <c r="F37" s="17"/>
       <c r="G37" s="14" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -5597,11 +5606,17 @@
         <v>81</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>63</v>
+        <v>81</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>123</v>
       </c>
       <c r="F38" s="17"/>
       <c r="G38" s="14" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -5612,45 +5627,35 @@
         <v>81</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>30</v>
+        <v>81</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>124</v>
       </c>
       <c r="F39" s="17"/>
       <c r="G39" s="14" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B40" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C40" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D40" s="14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F40" s="17"/>
       <c r="G40" s="14" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="14"/>
+      <c r="A41" s="14" t="s">
+        <v>81</v>
+      </c>
       <c r="B41" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C41" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D41" s="14" t="s">
-        <v>168</v>
+        <v>63</v>
       </c>
       <c r="F41" s="17"/>
       <c r="G41" s="14" t="s">
-        <v>166</v>
+        <v>127</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -5661,14 +5666,11 @@
         <v>81</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D42" s="14" t="s">
-        <v>105</v>
+        <v>30</v>
       </c>
       <c r="F42" s="17"/>
       <c r="G42" s="14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -5676,26 +5678,33 @@
         <v>81</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>30</v>
+        <v>81</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>29</v>
       </c>
       <c r="F43" s="17"/>
       <c r="G43" s="14" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="14" t="s">
-        <v>81</v>
-      </c>
+      <c r="A44" s="14"/>
       <c r="B44" s="14" t="s">
         <v>81</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>63</v>
+        <v>81</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>168</v>
       </c>
       <c r="F44" s="17"/>
       <c r="G44" s="14" t="s">
-        <v>127</v>
+        <v>166</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -5709,11 +5718,11 @@
         <v>81</v>
       </c>
       <c r="D45" s="14" t="s">
-        <v>29</v>
+        <v>105</v>
       </c>
       <c r="F45" s="17"/>
       <c r="G45" s="14" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -5721,17 +5730,11 @@
         <v>81</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C46" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D46" s="14" t="s">
-        <v>168</v>
+        <v>30</v>
       </c>
       <c r="F46" s="17"/>
       <c r="G46" s="14" t="s">
-        <v>166</v>
+        <v>128</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -5742,14 +5745,11 @@
         <v>81</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D47" s="14" t="s">
-        <v>105</v>
+        <v>63</v>
       </c>
       <c r="F47" s="17"/>
       <c r="G47" s="14" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -5757,13 +5757,17 @@
         <v>81</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
+        <v>81</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>29</v>
+      </c>
       <c r="F48" s="17"/>
       <c r="G48" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -5774,15 +5778,14 @@
         <v>81</v>
       </c>
       <c r="C49" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="D49" s="14"/>
+        <v>81</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>168</v>
+      </c>
       <c r="F49" s="17"/>
       <c r="G49" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="H49" s="14" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -5793,15 +5796,14 @@
         <v>81</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D50" s="14"/>
+        <v>81</v>
+      </c>
+      <c r="D50" s="14" t="s">
+        <v>105</v>
+      </c>
       <c r="F50" s="17"/>
       <c r="G50" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="H50" s="14" t="s">
-        <v>171</v>
+        <v>130</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -5809,14 +5811,13 @@
         <v>81</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C51" s="14" t="s">
-        <v>29</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
       <c r="F51" s="17"/>
       <c r="G51" s="14" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -5827,11 +5828,15 @@
         <v>81</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>169</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="D52" s="14"/>
       <c r="F52" s="17"/>
       <c r="G52" s="14" t="s">
-        <v>170</v>
+        <v>127</v>
+      </c>
+      <c r="H52" s="14" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -5842,11 +5847,15 @@
         <v>81</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>104</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="D53" s="14"/>
       <c r="F53" s="17"/>
       <c r="G53" s="14" t="s">
-        <v>131</v>
+        <v>128</v>
+      </c>
+      <c r="H53" s="14" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -5857,14 +5866,11 @@
         <v>81</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D54" s="14" t="s">
-        <v>94</v>
+        <v>29</v>
       </c>
       <c r="F54" s="17"/>
       <c r="G54" s="14" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -5875,17 +5881,11 @@
         <v>81</v>
       </c>
       <c r="C55" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D55" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E55" s="14" t="s">
-        <v>30</v>
+        <v>169</v>
       </c>
       <c r="F55" s="17"/>
       <c r="G55" s="14" t="s">
-        <v>128</v>
+        <v>170</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -5896,14 +5896,11 @@
         <v>81</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>31</v>
+        <v>104</v>
       </c>
       <c r="F56" s="17"/>
       <c r="G56" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="H56" s="14" t="s">
-        <v>171</v>
+        <v>131</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -5914,14 +5911,14 @@
         <v>81</v>
       </c>
       <c r="C57" s="14" t="s">
-        <v>87</v>
+        <v>81</v>
+      </c>
+      <c r="D57" s="14" t="s">
+        <v>94</v>
       </c>
       <c r="F57" s="17"/>
       <c r="G57" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="H57" s="14" t="s">
-        <v>171</v>
+        <v>132</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -5932,14 +5929,17 @@
         <v>81</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>32</v>
+        <v>81</v>
+      </c>
+      <c r="D58" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E58" s="14" t="s">
+        <v>30</v>
       </c>
       <c r="F58" s="17"/>
       <c r="G58" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="H58" s="14" t="s">
-        <v>171</v>
+        <v>128</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -5950,11 +5950,11 @@
         <v>81</v>
       </c>
       <c r="C59" s="14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F59" s="17"/>
       <c r="G59" s="14" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="H59" s="14" t="s">
         <v>171</v>
@@ -5968,11 +5968,11 @@
         <v>81</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>9</v>
+        <v>87</v>
       </c>
       <c r="F60" s="17"/>
       <c r="G60" s="14" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="H60" s="14" t="s">
         <v>171</v>
@@ -5986,11 +5986,11 @@
         <v>81</v>
       </c>
       <c r="C61" s="14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F61" s="17"/>
       <c r="G61" s="14" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="H61" s="14" t="s">
         <v>171</v>
@@ -6004,14 +6004,14 @@
         <v>81</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D62" s="14" t="s">
-        <v>94</v>
+        <v>33</v>
       </c>
       <c r="F62" s="17"/>
       <c r="G62" s="14" t="s">
-        <v>132</v>
+        <v>137</v>
+      </c>
+      <c r="H62" s="14" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -6022,17 +6022,14 @@
         <v>81</v>
       </c>
       <c r="C63" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D63" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E63" s="14" t="s">
-        <v>88</v>
+        <v>9</v>
       </c>
       <c r="F63" s="17"/>
       <c r="G63" s="14" t="s">
-        <v>141</v>
+        <v>138</v>
+      </c>
+      <c r="H63" s="14" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -6043,17 +6040,14 @@
         <v>81</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D64" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E64" s="14" t="s">
-        <v>89</v>
+        <v>34</v>
       </c>
       <c r="F64" s="17"/>
       <c r="G64" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
+      </c>
+      <c r="H64" s="14" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -6124,11 +6118,14 @@
         <v>81</v>
       </c>
       <c r="C68" s="14" t="s">
-        <v>90</v>
+        <v>81</v>
+      </c>
+      <c r="D68" s="14" t="s">
+        <v>94</v>
       </c>
       <c r="F68" s="17"/>
       <c r="G68" s="14" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -6139,11 +6136,17 @@
         <v>81</v>
       </c>
       <c r="C69" s="14" t="s">
-        <v>91</v>
+        <v>81</v>
+      </c>
+      <c r="D69" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E69" s="14" t="s">
+        <v>88</v>
       </c>
       <c r="F69" s="17"/>
       <c r="G69" s="14" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -6157,11 +6160,14 @@
         <v>81</v>
       </c>
       <c r="D70" s="14" t="s">
-        <v>92</v>
+        <v>81</v>
+      </c>
+      <c r="E70" s="14" t="s">
+        <v>89</v>
       </c>
       <c r="F70" s="17"/>
       <c r="G70" s="14" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -6172,14 +6178,11 @@
         <v>81</v>
       </c>
       <c r="C71" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D71" s="14" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F71" s="17"/>
       <c r="G71" s="14" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -6190,11 +6193,11 @@
         <v>81</v>
       </c>
       <c r="C72" s="14" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F72" s="17"/>
       <c r="G72" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -6208,11 +6211,11 @@
         <v>81</v>
       </c>
       <c r="D73" s="14" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F73" s="17"/>
       <c r="G73" s="14" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -6226,11 +6229,11 @@
         <v>81</v>
       </c>
       <c r="D74" s="14" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F74" s="17"/>
       <c r="G74" s="14" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -6241,11 +6244,11 @@
         <v>81</v>
       </c>
       <c r="C75" s="14" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F75" s="17"/>
       <c r="G75" s="14" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -6259,11 +6262,11 @@
         <v>81</v>
       </c>
       <c r="D76" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F76" s="17"/>
       <c r="G76" s="14" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -6277,14 +6280,11 @@
         <v>81</v>
       </c>
       <c r="D77" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E77" s="14" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F77" s="17"/>
       <c r="G77" s="14" t="s">
-        <v>99</v>
+        <v>146</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -6295,17 +6295,11 @@
         <v>81</v>
       </c>
       <c r="C78" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D78" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E78" s="14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F78" s="17"/>
       <c r="G78" s="14" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -6319,14 +6313,11 @@
         <v>81</v>
       </c>
       <c r="D79" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E79" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F79" s="17"/>
       <c r="G79" s="14" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -6343,11 +6334,11 @@
         <v>81</v>
       </c>
       <c r="E80" s="14" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F80" s="17"/>
       <c r="G80" s="14" t="s">
-        <v>151</v>
+        <v>99</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -6364,20 +6355,32 @@
         <v>81</v>
       </c>
       <c r="E81" s="14" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F81" s="17"/>
       <c r="G81" s="14" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="14" t="s">
-        <v>106</v>
+        <v>81</v>
+      </c>
+      <c r="B82" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C82" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D82" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E82" s="14" t="s">
+        <v>101</v>
       </c>
       <c r="F82" s="17"/>
       <c r="G82" s="14" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -6385,11 +6388,20 @@
         <v>81</v>
       </c>
       <c r="B83" s="14" t="s">
-        <v>63</v>
+        <v>81</v>
+      </c>
+      <c r="C83" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D83" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E83" s="14" t="s">
+        <v>102</v>
       </c>
       <c r="F83" s="17"/>
       <c r="G83" s="14" t="s">
-        <v>127</v>
+        <v>151</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -6400,29 +6412,26 @@
         <v>81</v>
       </c>
       <c r="C84" s="14" t="s">
-        <v>30</v>
+        <v>81</v>
+      </c>
+      <c r="D84" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E84" s="14" t="s">
+        <v>103</v>
       </c>
       <c r="F84" s="17"/>
       <c r="G84" s="14" t="s">
-        <v>128</v>
+        <v>154</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B85" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C85" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D85" s="14" t="s">
-        <v>29</v>
+        <v>106</v>
       </c>
       <c r="F85" s="17"/>
       <c r="G85" s="14" t="s">
-        <v>129</v>
+        <v>155</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -6430,17 +6439,11 @@
         <v>81</v>
       </c>
       <c r="B86" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C86" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D86" s="14" t="s">
-        <v>105</v>
+        <v>63</v>
       </c>
       <c r="F86" s="17"/>
       <c r="G86" s="14" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -6451,14 +6454,11 @@
         <v>81</v>
       </c>
       <c r="C87" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D87" s="14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F87" s="17"/>
       <c r="G87" s="14" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -6472,11 +6472,11 @@
         <v>81</v>
       </c>
       <c r="D88" s="14" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F88" s="17"/>
       <c r="G88" s="14" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -6490,11 +6490,11 @@
         <v>81</v>
       </c>
       <c r="D89" s="14" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="F89" s="17"/>
       <c r="G89" s="14" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -6502,11 +6502,17 @@
         <v>81</v>
       </c>
       <c r="B90" s="14" t="s">
-        <v>30</v>
+        <v>81</v>
+      </c>
+      <c r="C90" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D90" s="14" t="s">
+        <v>32</v>
       </c>
       <c r="F90" s="17"/>
       <c r="G90" s="14" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -6517,11 +6523,14 @@
         <v>81</v>
       </c>
       <c r="C91" s="14" t="s">
-        <v>63</v>
+        <v>81</v>
+      </c>
+      <c r="D91" s="14" t="s">
+        <v>33</v>
       </c>
       <c r="F91" s="17"/>
       <c r="G91" s="14" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -6535,11 +6544,11 @@
         <v>81</v>
       </c>
       <c r="D92" s="14" t="s">
-        <v>29</v>
+        <v>89</v>
       </c>
       <c r="F92" s="17"/>
       <c r="G92" s="14" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -6547,17 +6556,11 @@
         <v>81</v>
       </c>
       <c r="B93" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C93" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D93" s="14" t="s">
-        <v>105</v>
+        <v>30</v>
       </c>
       <c r="F93" s="17"/>
       <c r="G93" s="14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -6568,14 +6571,11 @@
         <v>81</v>
       </c>
       <c r="C94" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D94" s="14" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="F94" s="17"/>
       <c r="G94" s="14" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -6589,11 +6589,11 @@
         <v>81</v>
       </c>
       <c r="D95" s="14" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F95" s="17"/>
       <c r="G95" s="14" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -6607,11 +6607,11 @@
         <v>81</v>
       </c>
       <c r="D96" s="14" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="F96" s="17"/>
       <c r="G96" s="14" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -6619,13 +6619,17 @@
         <v>81</v>
       </c>
       <c r="B97" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="C97" s="14"/>
-      <c r="D97" s="14"/>
+        <v>81</v>
+      </c>
+      <c r="C97" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D97" s="14" t="s">
+        <v>32</v>
+      </c>
       <c r="F97" s="17"/>
       <c r="G97" s="14" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -6636,12 +6640,14 @@
         <v>81</v>
       </c>
       <c r="C98" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="D98" s="14"/>
+        <v>81</v>
+      </c>
+      <c r="D98" s="14" t="s">
+        <v>33</v>
+      </c>
       <c r="F98" s="17"/>
       <c r="G98" s="14" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -6652,12 +6658,14 @@
         <v>81</v>
       </c>
       <c r="C99" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D99" s="14"/>
+        <v>81</v>
+      </c>
+      <c r="D99" s="14" t="s">
+        <v>89</v>
+      </c>
       <c r="F99" s="17"/>
       <c r="G99" s="14" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -6665,14 +6673,13 @@
         <v>81</v>
       </c>
       <c r="B100" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C100" s="14" t="s">
-        <v>29</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="C100" s="14"/>
+      <c r="D100" s="14"/>
       <c r="F100" s="17"/>
       <c r="G100" s="14" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -6683,11 +6690,12 @@
         <v>81</v>
       </c>
       <c r="C101" s="14" t="s">
-        <v>169</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="D101" s="14"/>
       <c r="F101" s="17"/>
       <c r="G101" s="14" t="s">
-        <v>170</v>
+        <v>127</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -6698,11 +6706,12 @@
         <v>81</v>
       </c>
       <c r="C102" s="14" t="s">
-        <v>104</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="D102" s="14"/>
       <c r="F102" s="17"/>
       <c r="G102" s="14" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -6713,14 +6722,11 @@
         <v>81</v>
       </c>
       <c r="C103" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D103" s="14" t="s">
-        <v>94</v>
+        <v>29</v>
       </c>
       <c r="F103" s="17"/>
       <c r="G103" s="14" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -6731,17 +6737,11 @@
         <v>81</v>
       </c>
       <c r="C104" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D104" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E104" s="14" t="s">
-        <v>30</v>
+        <v>169</v>
       </c>
       <c r="F104" s="17"/>
       <c r="G104" s="14" t="s">
-        <v>128</v>
+        <v>170</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -6752,11 +6752,11 @@
         <v>81</v>
       </c>
       <c r="C105" s="14" t="s">
-        <v>31</v>
+        <v>104</v>
       </c>
       <c r="F105" s="17"/>
       <c r="G105" s="14" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -6767,11 +6767,14 @@
         <v>81</v>
       </c>
       <c r="C106" s="14" t="s">
-        <v>32</v>
+        <v>81</v>
+      </c>
+      <c r="D106" s="14" t="s">
+        <v>94</v>
       </c>
       <c r="F106" s="17"/>
       <c r="G106" s="14" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -6782,11 +6785,17 @@
         <v>81</v>
       </c>
       <c r="C107" s="14" t="s">
-        <v>33</v>
+        <v>81</v>
+      </c>
+      <c r="D107" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E107" s="14" t="s">
+        <v>30</v>
       </c>
       <c r="F107" s="17"/>
       <c r="G107" s="14" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
@@ -6797,11 +6806,11 @@
         <v>81</v>
       </c>
       <c r="C108" s="14" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="F108" s="17"/>
       <c r="G108" s="14" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
@@ -6812,14 +6821,11 @@
         <v>81</v>
       </c>
       <c r="C109" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="D109" s="16" t="s">
-        <v>112</v>
+        <v>32</v>
       </c>
       <c r="F109" s="17"/>
       <c r="G109" s="14" t="s">
-        <v>156</v>
+        <v>136</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
@@ -6830,11 +6836,11 @@
         <v>81</v>
       </c>
       <c r="C110" s="14" t="s">
-        <v>107</v>
+        <v>33</v>
       </c>
       <c r="F110" s="17"/>
       <c r="G110" s="14" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
@@ -6845,14 +6851,11 @@
         <v>81</v>
       </c>
       <c r="C111" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D111" s="14" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="F111" s="17"/>
       <c r="G111" s="14" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
@@ -6863,17 +6866,14 @@
         <v>81</v>
       </c>
       <c r="C112" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D112" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E112" s="14" t="s">
-        <v>110</v>
+        <v>111</v>
+      </c>
+      <c r="D112" s="16" t="s">
+        <v>112</v>
       </c>
       <c r="F112" s="17"/>
       <c r="G112" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
@@ -6884,17 +6884,11 @@
         <v>81</v>
       </c>
       <c r="C113" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D113" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E113" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F113" s="17"/>
       <c r="G113" s="14" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
@@ -6908,14 +6902,11 @@
         <v>81</v>
       </c>
       <c r="D114" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E114" s="14" t="s">
-        <v>109</v>
+        <v>65</v>
       </c>
       <c r="F114" s="17"/>
       <c r="G114" s="14" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
@@ -6932,11 +6923,11 @@
         <v>81</v>
       </c>
       <c r="E115" s="14" t="s">
-        <v>89</v>
+        <v>110</v>
       </c>
       <c r="F115" s="17"/>
       <c r="G115" s="14" t="s">
-        <v>140</v>
+        <v>158</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
@@ -6947,24 +6938,75 @@
         <v>81</v>
       </c>
       <c r="C116" s="14" t="s">
-        <v>54</v>
+        <v>81</v>
+      </c>
+      <c r="D116" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E116" s="14" t="s">
+        <v>108</v>
       </c>
       <c r="F116" s="17"/>
       <c r="G116" s="14" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B117" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C117" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D117" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E117" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="F117" s="17"/>
+      <c r="G117" s="14" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B118" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C118" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D118" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E118" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="F118" s="17"/>
+      <c r="G118" s="14" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B119" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C119" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F119" s="17"/>
+      <c r="G119" s="14" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A117" s="14"/>
-      <c r="B117" s="14"/>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A118" s="14"/>
-      <c r="B118" s="14"/>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A119" s="14"/>
-      <c r="B119" s="14"/>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="14"/>
@@ -7124,56 +7166,59 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="14"/>
+      <c r="B159" s="14"/>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="14"/>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B160" s="14"/>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="14"/>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B161" s="14"/>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="14"/>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="14"/>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="14"/>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="14"/>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="14"/>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="14"/>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="14"/>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="14"/>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="14"/>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="14"/>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="14"/>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="14"/>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="14"/>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="14"/>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="14"/>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
@@ -7208,6 +7253,15 @@
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187" s="14"/>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" s="14"/>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" s="14"/>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed formatting in DPR to look better on phones without overlapping.
</commit_message>
<xml_diff>
--- a/Accessibility Chart.xlsx
+++ b/Accessibility Chart.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1378" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1389" uniqueCount="174">
   <si>
     <t>APP</t>
   </si>
@@ -4960,8 +4960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5520,7 +5520,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>81</v>
       </c>
@@ -5535,7 +5535,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
         <v>81</v>
       </c>
@@ -5553,7 +5553,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>81</v>
       </c>
@@ -5567,7 +5567,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
         <v>81</v>
       </c>
@@ -5583,7 +5583,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
         <v>81</v>
       </c>
@@ -5601,7 +5601,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
         <v>81</v>
       </c>
@@ -5619,7 +5619,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
         <v>81</v>
       </c>
@@ -5637,7 +5637,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
         <v>27</v>
       </c>
@@ -5646,7 +5646,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
         <v>81</v>
       </c>
@@ -5657,8 +5657,11 @@
       <c r="G41" s="14" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H41" s="15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
         <v>81</v>
       </c>
@@ -5672,8 +5675,11 @@
       <c r="G42" s="14" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H42" s="15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
         <v>81</v>
       </c>
@@ -5690,8 +5696,11 @@
       <c r="G43" s="14" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H43" s="15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="14"/>
       <c r="B44" s="14" t="s">
         <v>81</v>
@@ -5706,8 +5715,11 @@
       <c r="G44" s="14" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H44" s="15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
         <v>81</v>
       </c>
@@ -5724,8 +5736,11 @@
       <c r="G45" s="14" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H45" s="15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
         <v>81</v>
       </c>
@@ -5736,8 +5751,11 @@
       <c r="G46" s="14" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H46" s="15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
         <v>81</v>
       </c>
@@ -5751,8 +5769,11 @@
       <c r="G47" s="14" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H47" s="15" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
         <v>81</v>
       </c>
@@ -5769,6 +5790,9 @@
       <c r="G48" s="14" t="s">
         <v>129</v>
       </c>
+      <c r="H48" s="15" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
@@ -5787,6 +5811,9 @@
       <c r="G49" s="14" t="s">
         <v>166</v>
       </c>
+      <c r="H49" s="15" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
@@ -5804,6 +5831,9 @@
       <c r="F50" s="17"/>
       <c r="G50" s="14" t="s">
         <v>130</v>
+      </c>
+      <c r="H50" s="15" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -5819,6 +5849,9 @@
       <c r="G51" s="14" t="s">
         <v>130</v>
       </c>
+      <c r="H51" s="15" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">

</xml_diff>

<commit_message>
Figured out DPR adding techs. Next is to add hours to individual techs.
</commit_message>
<xml_diff>
--- a/Accessibility Chart.xlsx
+++ b/Accessibility Chart.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1389" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1419" uniqueCount="175">
   <si>
     <t>APP</t>
   </si>
@@ -445,9 +445,6 @@
     <t>hours</t>
   </si>
   <si>
-    <t>class</t>
-  </si>
-  <si>
     <t>iqr</t>
   </si>
   <si>
@@ -542,6 +539,12 @@
   </si>
   <si>
     <t>Contact #</t>
+  </si>
+  <si>
+    <t>techClass</t>
+  </si>
+  <si>
+    <t>#</t>
   </si>
 </sst>
 </file>
@@ -4958,10 +4961,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H190"/>
+  <dimension ref="A1:H193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="H54" sqref="H54"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4994,14 +4997,14 @@
         <v>77</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F2" s="17"/>
       <c r="G2" s="14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -5012,14 +5015,14 @@
         <v>81</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F3" s="17"/>
       <c r="G3" s="14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -5037,7 +5040,7 @@
         <v>114</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -5055,7 +5058,7 @@
         <v>115</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -5073,7 +5076,7 @@
         <v>116</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -5088,10 +5091,10 @@
       </c>
       <c r="F7" s="17"/>
       <c r="G7" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -5109,7 +5112,7 @@
         <v>117</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -5127,7 +5130,7 @@
         <v>118</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -5145,7 +5148,7 @@
         <v>119</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -5160,10 +5163,10 @@
       </c>
       <c r="F11" s="17"/>
       <c r="G11" s="14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -5174,14 +5177,14 @@
         <v>81</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F12" s="17"/>
       <c r="G12" s="14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -5199,7 +5202,7 @@
         <v>121</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -5217,7 +5220,7 @@
         <v>122</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -5235,7 +5238,7 @@
         <v>123</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -5256,7 +5259,7 @@
         <v>124</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -5267,12 +5270,12 @@
         <v>81</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D17" s="14"/>
       <c r="F17" s="17"/>
       <c r="G17" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H17" s="14"/>
     </row>
@@ -5411,7 +5414,7 @@
       </c>
       <c r="F25" s="17"/>
       <c r="G25" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -5482,11 +5485,11 @@
         <v>81</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F30" s="17"/>
       <c r="G30" s="14" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H30" s="14"/>
     </row>
@@ -5658,7 +5661,7 @@
         <v>127</v>
       </c>
       <c r="H41" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -5676,7 +5679,7 @@
         <v>128</v>
       </c>
       <c r="H42" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -5697,7 +5700,7 @@
         <v>129</v>
       </c>
       <c r="H43" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -5709,14 +5712,14 @@
         <v>81</v>
       </c>
       <c r="D44" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F44" s="17"/>
       <c r="G44" s="14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H44" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -5737,7 +5740,7 @@
         <v>130</v>
       </c>
       <c r="H45" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -5752,7 +5755,7 @@
         <v>128</v>
       </c>
       <c r="H46" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -5770,7 +5773,7 @@
         <v>127</v>
       </c>
       <c r="H47" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -5791,7 +5794,7 @@
         <v>129</v>
       </c>
       <c r="H48" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -5805,14 +5808,14 @@
         <v>81</v>
       </c>
       <c r="D49" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F49" s="17"/>
       <c r="G49" s="14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H49" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -5833,7 +5836,7 @@
         <v>130</v>
       </c>
       <c r="H50" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -5850,7 +5853,7 @@
         <v>130</v>
       </c>
       <c r="H51" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -5869,7 +5872,7 @@
         <v>127</v>
       </c>
       <c r="H52" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -5888,7 +5891,7 @@
         <v>128</v>
       </c>
       <c r="H53" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -5905,6 +5908,9 @@
       <c r="G54" s="14" t="s">
         <v>129</v>
       </c>
+      <c r="H54" s="15" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
@@ -5914,10 +5920,13 @@
         <v>81</v>
       </c>
       <c r="C55" s="14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F55" s="17"/>
       <c r="G55" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="H55" s="15" t="s">
         <v>170</v>
       </c>
     </row>
@@ -5990,7 +5999,7 @@
         <v>134</v>
       </c>
       <c r="H59" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -6008,7 +6017,7 @@
         <v>135</v>
       </c>
       <c r="H60" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -6026,7 +6035,7 @@
         <v>136</v>
       </c>
       <c r="H61" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -6044,7 +6053,7 @@
         <v>137</v>
       </c>
       <c r="H62" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -6062,7 +6071,7 @@
         <v>138</v>
       </c>
       <c r="H63" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -6080,10 +6089,10 @@
         <v>139</v>
       </c>
       <c r="H64" s="14" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="14" t="s">
         <v>81</v>
       </c>
@@ -6094,14 +6103,17 @@
         <v>81</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>94</v>
+        <v>174</v>
       </c>
       <c r="F65" s="17"/>
-      <c r="G65" s="14" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G65" s="14">
+        <v>0</v>
+      </c>
+      <c r="H65" s="14" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="14" t="s">
         <v>81</v>
       </c>
@@ -6115,14 +6127,17 @@
         <v>81</v>
       </c>
       <c r="E66" s="14" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F66" s="17"/>
       <c r="G66" s="14" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+      <c r="H66" s="14" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="14" t="s">
         <v>81</v>
       </c>
@@ -6136,14 +6151,17 @@
         <v>81</v>
       </c>
       <c r="E67" s="14" t="s">
-        <v>89</v>
+        <v>25</v>
       </c>
       <c r="F67" s="17"/>
       <c r="G67" s="14" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="H67" s="14" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="14" t="s">
         <v>81</v>
       </c>
@@ -6154,14 +6172,20 @@
         <v>81</v>
       </c>
       <c r="D68" s="14" t="s">
-        <v>94</v>
+        <v>81</v>
+      </c>
+      <c r="E68" s="14" t="s">
+        <v>85</v>
       </c>
       <c r="F68" s="17"/>
       <c r="G68" s="14" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="H68" s="14" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="14" t="s">
         <v>81</v>
       </c>
@@ -6175,14 +6199,17 @@
         <v>81</v>
       </c>
       <c r="E69" s="14" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="F69" s="17"/>
       <c r="G69" s="14" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+      <c r="H69" s="14" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="14" t="s">
         <v>81</v>
       </c>
@@ -6202,8 +6229,11 @@
       <c r="G70" s="14" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H70" s="14" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="14" t="s">
         <v>81</v>
       </c>
@@ -6211,14 +6241,20 @@
         <v>81</v>
       </c>
       <c r="C71" s="14" t="s">
-        <v>90</v>
+        <v>81</v>
+      </c>
+      <c r="D71" s="14" t="s">
+        <v>174</v>
       </c>
       <c r="F71" s="17"/>
-      <c r="G71" s="14" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G71" s="14">
+        <v>1</v>
+      </c>
+      <c r="H71" s="14" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="14" t="s">
         <v>81</v>
       </c>
@@ -6226,14 +6262,23 @@
         <v>81</v>
       </c>
       <c r="C72" s="14" t="s">
-        <v>91</v>
+        <v>81</v>
+      </c>
+      <c r="D72" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E72" s="14" t="s">
+        <v>88</v>
       </c>
       <c r="F72" s="17"/>
       <c r="G72" s="14" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+      <c r="H72" s="14" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="14" t="s">
         <v>81</v>
       </c>
@@ -6244,14 +6289,17 @@
         <v>81</v>
       </c>
       <c r="D73" s="14" t="s">
-        <v>92</v>
+        <v>81</v>
+      </c>
+      <c r="E73" s="14" t="s">
+        <v>89</v>
       </c>
       <c r="F73" s="17"/>
       <c r="G73" s="14" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="14" t="s">
         <v>81</v>
       </c>
@@ -6259,17 +6307,17 @@
         <v>81</v>
       </c>
       <c r="C74" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D74" s="14" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F74" s="17"/>
       <c r="G74" s="14" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+      <c r="H74" s="15" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="14" t="s">
         <v>81</v>
       </c>
@@ -6277,14 +6325,17 @@
         <v>81</v>
       </c>
       <c r="C75" s="14" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F75" s="17"/>
       <c r="G75" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="H75" s="15" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="14" t="s">
         <v>81</v>
       </c>
@@ -6295,14 +6346,17 @@
         <v>81</v>
       </c>
       <c r="D76" s="14" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F76" s="17"/>
       <c r="G76" s="14" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+      <c r="H76" s="15" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="14" t="s">
         <v>81</v>
       </c>
@@ -6313,14 +6367,17 @@
         <v>81</v>
       </c>
       <c r="D77" s="14" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F77" s="17"/>
       <c r="G77" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+      <c r="H77" s="15" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="14" t="s">
         <v>81</v>
       </c>
@@ -6328,14 +6385,14 @@
         <v>81</v>
       </c>
       <c r="C78" s="14" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F78" s="17"/>
       <c r="G78" s="14" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="14" t="s">
         <v>81</v>
       </c>
@@ -6346,14 +6403,14 @@
         <v>81</v>
       </c>
       <c r="D79" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F79" s="17"/>
       <c r="G79" s="14" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="14" t="s">
         <v>81</v>
       </c>
@@ -6364,14 +6421,11 @@
         <v>81</v>
       </c>
       <c r="D80" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E80" s="14" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F80" s="17"/>
       <c r="G80" s="14" t="s">
-        <v>99</v>
+        <v>145</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -6382,17 +6436,11 @@
         <v>81</v>
       </c>
       <c r="C81" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D81" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E81" s="14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F81" s="17"/>
       <c r="G81" s="14" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -6406,14 +6454,11 @@
         <v>81</v>
       </c>
       <c r="D82" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E82" s="14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="F82" s="17"/>
       <c r="G82" s="14" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -6430,11 +6475,11 @@
         <v>81</v>
       </c>
       <c r="E83" s="14" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F83" s="17"/>
       <c r="G83" s="14" t="s">
-        <v>151</v>
+        <v>99</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -6451,20 +6496,32 @@
         <v>81</v>
       </c>
       <c r="E84" s="14" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F84" s="17"/>
       <c r="G84" s="14" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="14" t="s">
-        <v>106</v>
+        <v>81</v>
+      </c>
+      <c r="B85" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C85" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D85" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E85" s="14" t="s">
+        <v>101</v>
       </c>
       <c r="F85" s="17"/>
       <c r="G85" s="14" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -6472,11 +6529,20 @@
         <v>81</v>
       </c>
       <c r="B86" s="14" t="s">
-        <v>63</v>
+        <v>81</v>
+      </c>
+      <c r="C86" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D86" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E86" s="14" t="s">
+        <v>102</v>
       </c>
       <c r="F86" s="17"/>
       <c r="G86" s="14" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -6487,29 +6553,26 @@
         <v>81</v>
       </c>
       <c r="C87" s="14" t="s">
-        <v>30</v>
+        <v>81</v>
+      </c>
+      <c r="D87" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E87" s="14" t="s">
+        <v>103</v>
       </c>
       <c r="F87" s="17"/>
       <c r="G87" s="14" t="s">
-        <v>128</v>
+        <v>153</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B88" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C88" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D88" s="14" t="s">
-        <v>29</v>
+        <v>106</v>
       </c>
       <c r="F88" s="17"/>
       <c r="G88" s="14" t="s">
-        <v>129</v>
+        <v>154</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -6517,17 +6580,11 @@
         <v>81</v>
       </c>
       <c r="B89" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C89" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D89" s="14" t="s">
-        <v>105</v>
+        <v>63</v>
       </c>
       <c r="F89" s="17"/>
       <c r="G89" s="14" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -6538,14 +6595,11 @@
         <v>81</v>
       </c>
       <c r="C90" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D90" s="14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F90" s="17"/>
       <c r="G90" s="14" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -6559,11 +6613,11 @@
         <v>81</v>
       </c>
       <c r="D91" s="14" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F91" s="17"/>
       <c r="G91" s="14" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -6577,11 +6631,11 @@
         <v>81</v>
       </c>
       <c r="D92" s="14" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="F92" s="17"/>
       <c r="G92" s="14" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -6589,11 +6643,17 @@
         <v>81</v>
       </c>
       <c r="B93" s="14" t="s">
-        <v>30</v>
+        <v>81</v>
+      </c>
+      <c r="C93" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D93" s="14" t="s">
+        <v>32</v>
       </c>
       <c r="F93" s="17"/>
       <c r="G93" s="14" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -6604,11 +6664,14 @@
         <v>81</v>
       </c>
       <c r="C94" s="14" t="s">
-        <v>63</v>
+        <v>81</v>
+      </c>
+      <c r="D94" s="14" t="s">
+        <v>33</v>
       </c>
       <c r="F94" s="17"/>
       <c r="G94" s="14" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -6622,11 +6685,11 @@
         <v>81</v>
       </c>
       <c r="D95" s="14" t="s">
-        <v>29</v>
+        <v>89</v>
       </c>
       <c r="F95" s="17"/>
       <c r="G95" s="14" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -6634,17 +6697,11 @@
         <v>81</v>
       </c>
       <c r="B96" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C96" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D96" s="14" t="s">
-        <v>105</v>
+        <v>30</v>
       </c>
       <c r="F96" s="17"/>
       <c r="G96" s="14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -6655,14 +6712,11 @@
         <v>81</v>
       </c>
       <c r="C97" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D97" s="14" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="F97" s="17"/>
       <c r="G97" s="14" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -6676,11 +6730,11 @@
         <v>81</v>
       </c>
       <c r="D98" s="14" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F98" s="17"/>
       <c r="G98" s="14" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -6694,11 +6748,11 @@
         <v>81</v>
       </c>
       <c r="D99" s="14" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="F99" s="17"/>
       <c r="G99" s="14" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -6706,13 +6760,17 @@
         <v>81</v>
       </c>
       <c r="B100" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="C100" s="14"/>
-      <c r="D100" s="14"/>
+        <v>81</v>
+      </c>
+      <c r="C100" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D100" s="14" t="s">
+        <v>32</v>
+      </c>
       <c r="F100" s="17"/>
       <c r="G100" s="14" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -6723,12 +6781,14 @@
         <v>81</v>
       </c>
       <c r="C101" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="D101" s="14"/>
+        <v>81</v>
+      </c>
+      <c r="D101" s="14" t="s">
+        <v>33</v>
+      </c>
       <c r="F101" s="17"/>
       <c r="G101" s="14" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -6739,12 +6799,14 @@
         <v>81</v>
       </c>
       <c r="C102" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D102" s="14"/>
+        <v>81</v>
+      </c>
+      <c r="D102" s="14" t="s">
+        <v>89</v>
+      </c>
       <c r="F102" s="17"/>
       <c r="G102" s="14" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -6752,14 +6814,13 @@
         <v>81</v>
       </c>
       <c r="B103" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C103" s="14" t="s">
-        <v>29</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="C103" s="14"/>
+      <c r="D103" s="14"/>
       <c r="F103" s="17"/>
       <c r="G103" s="14" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -6770,11 +6831,12 @@
         <v>81</v>
       </c>
       <c r="C104" s="14" t="s">
-        <v>169</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="D104" s="14"/>
       <c r="F104" s="17"/>
       <c r="G104" s="14" t="s">
-        <v>170</v>
+        <v>127</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -6785,11 +6847,12 @@
         <v>81</v>
       </c>
       <c r="C105" s="14" t="s">
-        <v>104</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="D105" s="14"/>
       <c r="F105" s="17"/>
       <c r="G105" s="14" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -6800,14 +6863,11 @@
         <v>81</v>
       </c>
       <c r="C106" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D106" s="14" t="s">
-        <v>94</v>
+        <v>29</v>
       </c>
       <c r="F106" s="17"/>
       <c r="G106" s="14" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -6818,17 +6878,11 @@
         <v>81</v>
       </c>
       <c r="C107" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D107" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E107" s="14" t="s">
-        <v>30</v>
+        <v>168</v>
       </c>
       <c r="F107" s="17"/>
       <c r="G107" s="14" t="s">
-        <v>128</v>
+        <v>169</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
@@ -6839,11 +6893,11 @@
         <v>81</v>
       </c>
       <c r="C108" s="14" t="s">
-        <v>31</v>
+        <v>104</v>
       </c>
       <c r="F108" s="17"/>
       <c r="G108" s="14" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
@@ -6854,11 +6908,14 @@
         <v>81</v>
       </c>
       <c r="C109" s="14" t="s">
-        <v>32</v>
+        <v>81</v>
+      </c>
+      <c r="D109" s="14" t="s">
+        <v>94</v>
       </c>
       <c r="F109" s="17"/>
       <c r="G109" s="14" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
@@ -6869,11 +6926,17 @@
         <v>81</v>
       </c>
       <c r="C110" s="14" t="s">
-        <v>33</v>
+        <v>81</v>
+      </c>
+      <c r="D110" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E110" s="14" t="s">
+        <v>30</v>
       </c>
       <c r="F110" s="17"/>
       <c r="G110" s="14" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
@@ -6884,11 +6947,11 @@
         <v>81</v>
       </c>
       <c r="C111" s="14" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="F111" s="17"/>
       <c r="G111" s="14" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
@@ -6899,14 +6962,11 @@
         <v>81</v>
       </c>
       <c r="C112" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="D112" s="16" t="s">
-        <v>112</v>
+        <v>32</v>
       </c>
       <c r="F112" s="17"/>
       <c r="G112" s="14" t="s">
-        <v>156</v>
+        <v>136</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
@@ -6917,11 +6977,11 @@
         <v>81</v>
       </c>
       <c r="C113" s="14" t="s">
-        <v>107</v>
+        <v>33</v>
       </c>
       <c r="F113" s="17"/>
       <c r="G113" s="14" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
@@ -6932,14 +6992,11 @@
         <v>81</v>
       </c>
       <c r="C114" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D114" s="14" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="F114" s="17"/>
       <c r="G114" s="14" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
@@ -6950,17 +7007,14 @@
         <v>81</v>
       </c>
       <c r="C115" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D115" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E115" s="14" t="s">
-        <v>110</v>
+        <v>111</v>
+      </c>
+      <c r="D115" s="16" t="s">
+        <v>112</v>
       </c>
       <c r="F115" s="17"/>
       <c r="G115" s="14" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
@@ -6971,17 +7025,11 @@
         <v>81</v>
       </c>
       <c r="C116" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D116" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E116" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F116" s="17"/>
       <c r="G116" s="14" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
@@ -6995,14 +7043,11 @@
         <v>81</v>
       </c>
       <c r="D117" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E117" s="14" t="s">
-        <v>109</v>
+        <v>65</v>
       </c>
       <c r="F117" s="17"/>
       <c r="G117" s="14" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
@@ -7019,11 +7064,11 @@
         <v>81</v>
       </c>
       <c r="E118" s="14" t="s">
-        <v>89</v>
+        <v>110</v>
       </c>
       <c r="F118" s="17"/>
       <c r="G118" s="14" t="s">
-        <v>140</v>
+        <v>157</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
@@ -7034,24 +7079,75 @@
         <v>81</v>
       </c>
       <c r="C119" s="14" t="s">
-        <v>54</v>
+        <v>81</v>
+      </c>
+      <c r="D119" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E119" s="14" t="s">
+        <v>108</v>
       </c>
       <c r="F119" s="17"/>
       <c r="G119" s="14" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A120" s="14"/>
-      <c r="B120" s="14"/>
+      <c r="A120" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B120" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C120" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D120" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E120" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="F120" s="17"/>
+      <c r="G120" s="14" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A121" s="14"/>
-      <c r="B121" s="14"/>
+      <c r="A121" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B121" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C121" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D121" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E121" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="F121" s="17"/>
+      <c r="G121" s="14" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A122" s="14"/>
-      <c r="B122" s="14"/>
+      <c r="A122" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B122" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C122" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="F122" s="17"/>
+      <c r="G122" s="14" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="14"/>
@@ -7211,12 +7307,15 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="14"/>
+      <c r="B162" s="14"/>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="14"/>
+      <c r="B163" s="14"/>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="14"/>
+      <c r="B164" s="14"/>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="14"/>
@@ -7295,6 +7394,15 @@
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190" s="14"/>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" s="14"/>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" s="14"/>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finished all data fields for DPR and confirmed. Edited Accessibily excel to confirm what has been completed and confirmed correct in the database.
</commit_message>
<xml_diff>
--- a/Accessibility Chart.xlsx
+++ b/Accessibility Chart.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1419" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1554" uniqueCount="178">
   <si>
     <t>APP</t>
   </si>
@@ -286,24 +286,12 @@
     <t>Contractor</t>
   </si>
   <si>
-    <t>Class/Step</t>
-  </si>
-  <si>
     <t>Hours</t>
   </si>
   <si>
     <t>IQR</t>
   </si>
   <si>
-    <t>Materials</t>
-  </si>
-  <si>
-    <t>Needed</t>
-  </si>
-  <si>
-    <t>By</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -448,27 +436,18 @@
     <t>iqr</t>
   </si>
   <si>
-    <t>materials</t>
-  </si>
-  <si>
     <t>work</t>
   </si>
   <si>
     <t>workDone</t>
   </si>
   <si>
-    <t>workLocation</t>
-  </si>
-  <si>
     <t>progress</t>
   </si>
   <si>
     <t>location</t>
   </si>
   <si>
-    <t>pathways</t>
-  </si>
-  <si>
     <t>roughIn</t>
   </si>
   <si>
@@ -541,10 +520,40 @@
     <t>Contact #</t>
   </si>
   <si>
-    <t>techClass</t>
-  </si>
-  <si>
     <t>#</t>
+  </si>
+  <si>
+    <t>tr</t>
+  </si>
+  <si>
+    <t>pathway</t>
+  </si>
+  <si>
+    <t>techs</t>
+  </si>
+  <si>
+    <t>(true/false)</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>Materials Needed</t>
+  </si>
+  <si>
+    <t>Materials By</t>
+  </si>
+  <si>
+    <t>Data Name</t>
+  </si>
+  <si>
+    <t>Confirmed</t>
+  </si>
+  <si>
+    <t>Top</t>
+  </si>
+  <si>
+    <t>userID</t>
   </si>
 </sst>
 </file>
@@ -4961,10 +4970,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H193"/>
+  <dimension ref="A1:K200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="H56" sqref="H56"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4974,1752 +4983,2094 @@
     <col min="3" max="3" width="16.5703125" style="15" customWidth="1"/>
     <col min="4" max="4" width="12.140625" style="15" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" style="15" customWidth="1"/>
-    <col min="6" max="6" width="1.42578125" style="15" customWidth="1"/>
-    <col min="7" max="7" width="27.5703125" style="15" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" style="15" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="15"/>
+    <col min="8" max="8" width="1.42578125" style="15" customWidth="1"/>
+    <col min="9" max="9" width="27.5703125" style="15" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" style="15" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" style="15" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="B1" s="15">
+        <v>1</v>
+      </c>
+      <c r="C1" s="15">
+        <v>2</v>
+      </c>
+      <c r="D1" s="15">
+        <v>3</v>
+      </c>
+      <c r="E1" s="15">
+        <v>4</v>
+      </c>
+      <c r="F1" s="15">
+        <v>5</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="F1" s="17"/>
-      <c r="G1" s="14" t="s">
+      <c r="H3" s="17"/>
+      <c r="I3" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="H4" s="17"/>
+      <c r="I4" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K4" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="H5" s="17"/>
+      <c r="I5" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K5" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="H6" s="17"/>
+      <c r="I6" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="17"/>
+      <c r="I7" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K7" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="17"/>
+      <c r="I8" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K8" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="H9" s="17"/>
+      <c r="I9" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="J9" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K9" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="H10" s="17"/>
+      <c r="I10" s="14" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2" s="14" t="s">
+      <c r="J10" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K10" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="17"/>
+      <c r="I11" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="J11" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K11" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="H12" s="17"/>
+      <c r="I12" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="J12" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K12" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="17"/>
+      <c r="I13" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="J13" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K13" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="H14" s="17"/>
+      <c r="I14" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="F2" s="17"/>
-      <c r="G2" s="14" t="s">
+      <c r="J14" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K14" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="H15" s="17"/>
+      <c r="I15" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="J15" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K15" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" s="17"/>
+      <c r="I16" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="J16" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K16" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="H17" s="17"/>
+      <c r="I17" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="J17" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K17" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="H18" s="17"/>
+      <c r="I18" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="J18" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K18" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="D19" s="14"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="J19" s="14"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H20" s="17"/>
+      <c r="I20" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="J20" s="14"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="H21" s="17"/>
+      <c r="I21" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="J21" s="14"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="H22" s="17"/>
+      <c r="I22" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="J22" s="14"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="H23" s="17"/>
+      <c r="I23" s="14" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="H24" s="17"/>
+      <c r="I24" s="14" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H25" s="17"/>
+      <c r="I25" s="14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H26" s="17"/>
+      <c r="I26" s="14" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="H27" s="17"/>
+      <c r="I27" s="14" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="H28" s="17"/>
+      <c r="I28" s="14" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="H29" s="17"/>
+      <c r="I29" s="14" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="H30" s="17"/>
+      <c r="I30" s="14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H31" s="17"/>
+      <c r="I31" s="14" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C32" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H32" s="17"/>
+      <c r="I32" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="J32" s="14"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="H33" s="17"/>
+      <c r="I33" s="14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="H34" s="17"/>
+      <c r="I34" s="14" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="H35" s="17"/>
+      <c r="I35" s="14" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="H36" s="17"/>
+      <c r="I36" s="14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="J37" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K37" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="D38" s="14"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="J38" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K38" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="H39" s="17"/>
+      <c r="I39" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="J39" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K39" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="H40" s="17"/>
+      <c r="I40" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="J40" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K40" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="H41" s="17"/>
+      <c r="I41" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="J41" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K41" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="H42" s="17"/>
+      <c r="I42" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="J42" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K42" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="H43" s="17"/>
+      <c r="I43" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="J43" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K43" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="H44" s="17"/>
+      <c r="I44" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="J44" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="K44" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B45" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H45" s="17"/>
+      <c r="I45" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="J45" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="K45" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C46" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H46" s="17"/>
+      <c r="I46" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="J46" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="K46" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="14"/>
+      <c r="B47" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D47" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="H47" s="17"/>
+      <c r="I47" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="J47" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="K47" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="H48" s="17"/>
+      <c r="I48" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="J48" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="K48" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B49" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H49" s="17"/>
+      <c r="I49" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="J49" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="K49" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B50" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="H50" s="17"/>
+      <c r="I50" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="J50" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="K50" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B51" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C51" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D51" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H51" s="17"/>
+      <c r="I51" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="J51" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="K51" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B52" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C52" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D52" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="H52" s="17"/>
+      <c r="I52" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="J52" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="K52" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B53" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D53" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="H53" s="17"/>
+      <c r="I53" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="J53" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="K53" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B54" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
+      <c r="H54" s="17"/>
+      <c r="I54" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="J54" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="K54" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B55" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C55" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D55" s="14"/>
+      <c r="H55" s="17"/>
+      <c r="I55" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="J55" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K55" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B56" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C56" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D56" s="14"/>
+      <c r="H56" s="17"/>
+      <c r="I56" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="J56" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K56" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A57" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B57" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C57" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H57" s="17"/>
+      <c r="I57" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="J57" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="K57" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A58" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B58" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C58" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="H58" s="17"/>
+      <c r="I58" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="J58" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="K58" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A59" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B59" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C59" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="H59" s="17"/>
+      <c r="I59" s="14" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A60" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B60" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C60" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D60" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="H60" s="17"/>
+      <c r="I60" s="14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B61" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C61" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D61" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E61" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H61" s="17"/>
+      <c r="I61" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="K61" s="14"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B62" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C62" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="H62" s="17"/>
+      <c r="I62" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="J62" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K62" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B63" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C63" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="H63" s="17"/>
+      <c r="I63" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="J63" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K63" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B64" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C64" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H64" s="17"/>
+      <c r="I64" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="J64" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K64" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B65" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C65" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H65" s="17"/>
+      <c r="I65" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="J65" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K65" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B66" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C66" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="H66" s="17"/>
+      <c r="I66" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="J66" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K66" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B67" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C67" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="H67" s="17"/>
+      <c r="I67" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="J67" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K67" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B68" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C68" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D68" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="H68" s="17"/>
+      <c r="I68" s="14">
+        <v>0</v>
+      </c>
+      <c r="J68" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K68" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A69" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B69" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C69" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D69" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E69" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="F69" s="16" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="H3" s="14" t="s">
+      <c r="H69" s="17"/>
+      <c r="I69" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="J69" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K69" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B70" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C70" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D70" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E70" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F70" s="16" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="H4" s="14" t="s">
+      <c r="H70" s="17"/>
+      <c r="I70" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="J70" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K70" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B71" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C71" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D71" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E71" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="H71" s="17"/>
+      <c r="I71" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="J71" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K71" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A72" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B72" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C72" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D72" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E72" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="H72" s="17"/>
+      <c r="I72" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="J72" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K72" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B73" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C73" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D73" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E73" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H73" s="17"/>
+      <c r="I73" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="J73" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K73" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A74" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B74" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C74" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D74" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="H74" s="17"/>
+      <c r="I74" s="14">
+        <v>1</v>
+      </c>
+      <c r="J74" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K74" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A75" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B75" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C75" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D75" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E75" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="F75" s="16" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="17"/>
-      <c r="G5" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="H5" s="14" t="s">
+      <c r="H75" s="17"/>
+      <c r="I75" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="J75" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K75" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A76" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B76" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C76" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D76" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E76" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F76" s="16" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="17"/>
-      <c r="G6" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="F7" s="17"/>
-      <c r="G7" s="14" t="s">
+      <c r="H76" s="17"/>
+      <c r="I76" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="J76" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K76" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A77" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B77" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C77" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D77" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E77" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="H77" s="17"/>
+      <c r="I77" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="J77" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K77" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A78" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B78" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C78" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D78" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E78" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="H78" s="17"/>
+      <c r="I78" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="J78" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K78" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A79" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B79" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C79" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D79" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E79" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H79" s="17"/>
+      <c r="I79" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="J79" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K79" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A80" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B80" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C80" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="H80" s="17"/>
+      <c r="I80" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="J80" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="K80" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A81" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B81" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C81" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="H81" s="17"/>
+      <c r="I81" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="J81" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="K81" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A82" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B82" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C82" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="H82" s="17"/>
+      <c r="I82" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="J82" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="K82" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A83" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B83" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C83" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="H83" s="17"/>
+      <c r="I83" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="J83" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="K83" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A84" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B84" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C84" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D84" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="H7" s="14" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="F8" s="17"/>
-      <c r="G8" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="H9" s="14" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="17"/>
-      <c r="G11" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="H11" s="14" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="F12" s="17"/>
-      <c r="G12" s="14" t="s">
+      <c r="H84" s="17"/>
+      <c r="I84" s="14">
+        <v>0</v>
+      </c>
+      <c r="J84" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K84" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A85" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B85" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C85" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D85" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E85" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="H85" s="17"/>
+      <c r="I85" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="H12" s="14" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="F13" s="17"/>
-      <c r="G13" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="H13" s="14" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" s="17"/>
-      <c r="G14" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="H14" s="14" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="F15" s="17"/>
-      <c r="G15" s="14" t="s">
+      <c r="J85" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="K85" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A86" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B86" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C86" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D86" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E86" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="H86" s="17"/>
+      <c r="I86" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="J86" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="K86" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A87" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B87" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C87" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="H87" s="17"/>
+      <c r="I87" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="J87" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="K87" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A88" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B88" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C88" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D88" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="H88" s="17"/>
+      <c r="I88" s="14">
+        <v>0</v>
+      </c>
+      <c r="J88" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K88" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A89" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B89" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C89" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D89" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E89" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="F89" s="15"/>
+      <c r="H89" s="17"/>
+      <c r="I89" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="J89" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="K89" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A90" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B90" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C90" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D90" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E90" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F90" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="H90" s="17"/>
+      <c r="I90" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="J90" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="K90" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A91" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B91" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C91" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D91" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E91" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F91" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="H91" s="17"/>
+      <c r="I91" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="J91" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="K91" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A92" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B92" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C92" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D92" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E92" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F92" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="H92" s="17"/>
+      <c r="I92" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="J92" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="K92" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A93" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B93" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C93" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D93" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E93" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F93" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="H93" s="17"/>
+      <c r="I93" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="J93" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="K93" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A94" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B94" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C94" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D94" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E94" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F94" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="H94" s="17"/>
+      <c r="I94" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="J94" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="K94" s="14" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A95" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="H95" s="17"/>
+      <c r="I95" s="14" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A96" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B96" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="H96" s="17"/>
+      <c r="I96" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="H15" s="14" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="F16" s="17"/>
-      <c r="G16" s="14" t="s">
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B97" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C97" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H97" s="17"/>
+      <c r="I97" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="H16" s="14" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="D17" s="14"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="H17" s="14"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="F18" s="17"/>
-      <c r="G18" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="H18" s="14"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="F19" s="17"/>
-      <c r="G19" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="H19" s="14"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="F20" s="17"/>
-      <c r="G20" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="H20" s="14"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="F21" s="17"/>
-      <c r="G21" s="14" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="F22" s="17"/>
-      <c r="G22" s="14" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="F23" s="17"/>
-      <c r="G23" s="14" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="F24" s="17"/>
-      <c r="G24" s="14" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="F25" s="17"/>
-      <c r="G25" s="14" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B26" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="F26" s="17"/>
-      <c r="G26" s="14" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F27" s="17"/>
-      <c r="G27" s="14" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B28" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="F28" s="17"/>
-      <c r="G28" s="14" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B29" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="F29" s="17"/>
-      <c r="G29" s="14" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B30" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="F30" s="17"/>
-      <c r="G30" s="14" t="s">
-        <v>171</v>
-      </c>
-      <c r="H30" s="14"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B31" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C31" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="F31" s="17"/>
-      <c r="G31" s="14" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B32" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C32" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="F32" s="17"/>
-      <c r="G32" s="14" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B33" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C33" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="F33" s="17"/>
-      <c r="G33" s="14" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B34" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C34" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D34" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="F34" s="17"/>
-      <c r="G34" s="14" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B35" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B36" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C36" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="D36" s="14"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="14" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B37" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C37" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D37" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="F37" s="17"/>
-      <c r="G37" s="14" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B38" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C38" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D38" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="F38" s="17"/>
-      <c r="G38" s="14" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B39" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C39" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D39" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="F39" s="17"/>
-      <c r="G39" s="14" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="F40" s="17"/>
-      <c r="G40" s="14" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B41" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="F41" s="17"/>
-      <c r="G41" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="H41" s="15" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B42" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C42" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="F42" s="17"/>
-      <c r="G42" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="H42" s="15" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B43" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C43" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D43" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="F43" s="17"/>
-      <c r="G43" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="H43" s="15" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="14"/>
-      <c r="B44" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C44" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D44" s="14" t="s">
-        <v>167</v>
-      </c>
-      <c r="F44" s="17"/>
-      <c r="G44" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="H44" s="15" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B45" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C45" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D45" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="F45" s="17"/>
-      <c r="G45" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="H45" s="15" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B46" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="F46" s="17"/>
-      <c r="G46" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="H46" s="15" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B47" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C47" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="F47" s="17"/>
-      <c r="G47" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="H47" s="15" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B48" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C48" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D48" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="F48" s="17"/>
-      <c r="G48" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="H48" s="15" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B49" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C49" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D49" s="14" t="s">
-        <v>167</v>
-      </c>
-      <c r="F49" s="17"/>
-      <c r="G49" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="H49" s="15" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B50" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C50" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D50" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="F50" s="17"/>
-      <c r="G50" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="H50" s="15" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B51" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="C51" s="14"/>
-      <c r="D51" s="14"/>
-      <c r="F51" s="17"/>
-      <c r="G51" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="H51" s="15" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B52" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C52" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="D52" s="14"/>
-      <c r="F52" s="17"/>
-      <c r="G52" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="H52" s="14" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B53" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C53" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D53" s="14"/>
-      <c r="F53" s="17"/>
-      <c r="G53" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="H53" s="14" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B54" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C54" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="F54" s="17"/>
-      <c r="G54" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="H54" s="15" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B55" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C55" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="F55" s="17"/>
-      <c r="G55" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="H55" s="15" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B56" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C56" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="F56" s="17"/>
-      <c r="G56" s="14" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B57" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C57" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D57" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="F57" s="17"/>
-      <c r="G57" s="14" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B58" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C58" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D58" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E58" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="F58" s="17"/>
-      <c r="G58" s="14" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B59" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C59" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="F59" s="17"/>
-      <c r="G59" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="H59" s="14" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B60" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C60" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="F60" s="17"/>
-      <c r="G60" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="H60" s="14" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B61" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C61" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="F61" s="17"/>
-      <c r="G61" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="H61" s="14" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B62" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C62" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="F62" s="17"/>
-      <c r="G62" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="H62" s="14" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B63" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C63" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F63" s="17"/>
-      <c r="G63" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="H63" s="14" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B64" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C64" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F64" s="17"/>
-      <c r="G64" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="H64" s="14" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B65" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C65" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D65" s="14" t="s">
-        <v>174</v>
-      </c>
-      <c r="F65" s="17"/>
-      <c r="G65" s="14">
-        <v>0</v>
-      </c>
-      <c r="H65" s="14" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B66" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C66" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D66" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E66" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="F66" s="17"/>
-      <c r="G66" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="H66" s="14" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B67" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C67" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D67" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E67" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="F67" s="17"/>
-      <c r="G67" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="H67" s="14" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B68" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C68" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D68" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E68" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="F68" s="17"/>
-      <c r="G68" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="H68" s="14" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B69" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C69" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D69" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E69" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="F69" s="17"/>
-      <c r="G69" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="H69" s="14" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B70" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C70" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D70" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E70" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="F70" s="17"/>
-      <c r="G70" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="H70" s="14" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B71" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C71" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D71" s="14" t="s">
-        <v>174</v>
-      </c>
-      <c r="F71" s="17"/>
-      <c r="G71" s="14">
-        <v>1</v>
-      </c>
-      <c r="H71" s="14" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B72" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C72" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D72" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E72" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="F72" s="17"/>
-      <c r="G72" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="H72" s="14" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B73" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C73" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D73" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E73" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="F73" s="17"/>
-      <c r="G73" s="14" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B74" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C74" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="F74" s="17"/>
-      <c r="G74" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="H74" s="15" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B75" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C75" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="F75" s="17"/>
-      <c r="G75" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="H75" s="15" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B76" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C76" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D76" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="F76" s="17"/>
-      <c r="G76" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="H76" s="15" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B77" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C77" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D77" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="F77" s="17"/>
-      <c r="G77" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="H77" s="15" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B78" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C78" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="F78" s="17"/>
-      <c r="G78" s="14" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B79" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C79" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D79" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="F79" s="17"/>
-      <c r="G79" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B80" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C80" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D80" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="F80" s="17"/>
-      <c r="G80" s="14" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B81" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C81" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="F81" s="17"/>
-      <c r="G81" s="14" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B82" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C82" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D82" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="F82" s="17"/>
-      <c r="G82" s="14" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B83" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C83" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D83" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E83" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="F83" s="17"/>
-      <c r="G83" s="14" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B84" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C84" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D84" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E84" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="F84" s="17"/>
-      <c r="G84" s="14" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B85" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C85" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D85" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E85" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="F85" s="17"/>
-      <c r="G85" s="14" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B86" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C86" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D86" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E86" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="F86" s="17"/>
-      <c r="G86" s="14" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B87" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C87" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D87" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E87" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="F87" s="17"/>
-      <c r="G87" s="14" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="F88" s="17"/>
-      <c r="G88" s="14" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B89" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="F89" s="17"/>
-      <c r="G89" s="14" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B90" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C90" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="F90" s="17"/>
-      <c r="G90" s="14" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B91" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C91" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D91" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="F91" s="17"/>
-      <c r="G91" s="14" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B92" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C92" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D92" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="F92" s="17"/>
-      <c r="G92" s="14" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B93" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C93" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D93" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="F93" s="17"/>
-      <c r="G93" s="14" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B94" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C94" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D94" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="F94" s="17"/>
-      <c r="G94" s="14" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B95" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C95" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D95" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="F95" s="17"/>
-      <c r="G95" s="14" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B96" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="F96" s="17"/>
-      <c r="G96" s="14" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B97" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C97" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="F97" s="17"/>
-      <c r="G97" s="14" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="14" t="s">
         <v>81</v>
       </c>
@@ -6732,12 +7083,12 @@
       <c r="D98" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="F98" s="17"/>
-      <c r="G98" s="14" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H98" s="17"/>
+      <c r="I98" s="14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="14" t="s">
         <v>81</v>
       </c>
@@ -6748,14 +7099,14 @@
         <v>81</v>
       </c>
       <c r="D99" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="F99" s="17"/>
-      <c r="G99" s="14" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="H99" s="17"/>
+      <c r="I99" s="14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="14" t="s">
         <v>81</v>
       </c>
@@ -6768,12 +7119,12 @@
       <c r="D100" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="F100" s="17"/>
-      <c r="G100" s="14" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H100" s="17"/>
+      <c r="I100" s="14" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="14" t="s">
         <v>81</v>
       </c>
@@ -6786,12 +7137,12 @@
       <c r="D101" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="F101" s="17"/>
-      <c r="G101" s="14" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H101" s="17"/>
+      <c r="I101" s="14" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="14" t="s">
         <v>81</v>
       </c>
@@ -6802,28 +7153,26 @@
         <v>81</v>
       </c>
       <c r="D102" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="F102" s="17"/>
-      <c r="G102" s="14" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="H102" s="17"/>
+      <c r="I102" s="14" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="14" t="s">
         <v>81</v>
       </c>
       <c r="B103" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="C103" s="14"/>
-      <c r="D103" s="14"/>
-      <c r="F103" s="17"/>
-      <c r="G103" s="14" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="H103" s="17"/>
+      <c r="I103" s="14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="14" t="s">
         <v>81</v>
       </c>
@@ -6833,407 +7182,498 @@
       <c r="C104" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D104" s="14"/>
-      <c r="F104" s="17"/>
-      <c r="G104" s="14" t="s">
+      <c r="H104" s="17"/>
+      <c r="I104" s="14" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A105" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B105" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C105" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D105" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H105" s="17"/>
+      <c r="I105" s="14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A106" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B106" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C106" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D106" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="H106" s="17"/>
+      <c r="I106" s="14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A107" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B107" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C107" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D107" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H107" s="17"/>
+      <c r="I107" s="14" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A108" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B108" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C108" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D108" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H108" s="17"/>
+      <c r="I108" s="14" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A109" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B109" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C109" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D109" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H109" s="17"/>
+      <c r="I109" s="14" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A110" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B110" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C110" s="14"/>
+      <c r="D110" s="14"/>
+      <c r="H110" s="17"/>
+      <c r="I110" s="14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A111" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B111" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C111" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D111" s="14"/>
+      <c r="H111" s="17"/>
+      <c r="I111" s="14" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A112" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B112" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C112" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D112" s="14"/>
+      <c r="H112" s="17"/>
+      <c r="I112" s="14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A113" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B113" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C113" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H113" s="17"/>
+      <c r="I113" s="14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A114" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B114" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C114" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="H114" s="17"/>
+      <c r="I114" s="14" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A115" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B115" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C115" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="H115" s="17"/>
+      <c r="I115" s="14" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B105" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C105" s="14" t="s">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A116" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B116" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C116" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D116" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="H116" s="17"/>
+      <c r="I116" s="14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A117" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B117" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C117" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D117" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E117" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D105" s="14"/>
-      <c r="F105" s="17"/>
-      <c r="G105" s="14" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B106" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C106" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="F106" s="17"/>
-      <c r="G106" s="14" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B107" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C107" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="F107" s="17"/>
-      <c r="G107" s="14" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B108" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C108" s="14" t="s">
+      <c r="H117" s="17"/>
+      <c r="I117" s="14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A118" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B118" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C118" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="H118" s="17"/>
+      <c r="I118" s="14" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A119" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B119" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C119" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="H119" s="17"/>
+      <c r="I119" s="14" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A120" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B120" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C120" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H120" s="17"/>
+      <c r="I120" s="14" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A121" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B121" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C121" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H121" s="17"/>
+      <c r="I121" s="14" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A122" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B122" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C122" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="D122" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="H122" s="17"/>
+      <c r="I122" s="14" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A123" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B123" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C123" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="H123" s="17"/>
+      <c r="I123" s="14" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A124" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B124" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C124" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D124" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="H124" s="17"/>
+      <c r="I124" s="14" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A125" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B125" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C125" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D125" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E125" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="H125" s="17"/>
+      <c r="I125" s="14" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A126" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B126" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C126" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D126" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E126" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="F108" s="17"/>
-      <c r="G108" s="14" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A109" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B109" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C109" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D109" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="F109" s="17"/>
-      <c r="G109" s="14" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A110" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B110" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C110" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D110" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E110" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="F110" s="17"/>
-      <c r="G110" s="14" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A111" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B111" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C111" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="F111" s="17"/>
-      <c r="G111" s="14" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A112" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B112" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C112" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="F112" s="17"/>
-      <c r="G112" s="14" t="s">
+      <c r="H126" s="17"/>
+      <c r="I126" s="14" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A127" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B127" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C127" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D127" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E127" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="H127" s="17"/>
+      <c r="I127" s="14" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A128" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B128" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C128" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D128" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E128" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H128" s="17"/>
+      <c r="I128" s="14" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A113" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B113" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C113" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="F113" s="17"/>
-      <c r="G113" s="14" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A114" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B114" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C114" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="F114" s="17"/>
-      <c r="G114" s="14" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A115" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B115" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C115" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="D115" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="F115" s="17"/>
-      <c r="G115" s="14" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A116" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B116" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C116" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="F116" s="17"/>
-      <c r="G116" s="14" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A117" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B117" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C117" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D117" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="F117" s="17"/>
-      <c r="G117" s="14" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A118" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B118" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C118" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D118" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E118" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="F118" s="17"/>
-      <c r="G118" s="14" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A119" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B119" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C119" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D119" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E119" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="F119" s="17"/>
-      <c r="G119" s="14" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A120" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B120" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C120" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D120" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E120" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="F120" s="17"/>
-      <c r="G120" s="14" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A121" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B121" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C121" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D121" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E121" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="F121" s="17"/>
-      <c r="G121" s="14" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A122" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B122" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C122" s="14" t="s">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A129" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B129" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C129" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="F122" s="17"/>
-      <c r="G122" s="14" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A123" s="14"/>
-      <c r="B123" s="14"/>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A124" s="14"/>
-      <c r="B124" s="14"/>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A125" s="14"/>
-      <c r="B125" s="14"/>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A126" s="14"/>
-      <c r="B126" s="14"/>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A127" s="14"/>
-      <c r="B127" s="14"/>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A128" s="14"/>
-      <c r="B128" s="14"/>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="14"/>
-      <c r="B129" s="14"/>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="H129" s="17"/>
+      <c r="I129" s="14" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="14"/>
       <c r="B130" s="14"/>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="14"/>
       <c r="B131" s="14"/>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" s="14"/>
       <c r="B132" s="14"/>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="14"/>
       <c r="B133" s="14"/>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="14"/>
       <c r="B134" s="14"/>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="14"/>
       <c r="B135" s="14"/>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="14"/>
       <c r="B136" s="14"/>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="14"/>
       <c r="B137" s="14"/>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="14"/>
       <c r="B138" s="14"/>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="14"/>
       <c r="B139" s="14"/>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="14"/>
       <c r="B140" s="14"/>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="14"/>
       <c r="B141" s="14"/>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="14"/>
       <c r="B142" s="14"/>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="14"/>
       <c r="B143" s="14"/>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="14"/>
       <c r="B144" s="14"/>
     </row>
@@ -7319,24 +7759,31 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="14"/>
+      <c r="B165" s="14"/>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="14"/>
+      <c r="B166" s="14"/>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="14"/>
+      <c r="B167" s="14"/>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="14"/>
+      <c r="B168" s="14"/>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="14"/>
+      <c r="B169" s="14"/>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="14"/>
+      <c r="B170" s="14"/>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="14"/>
+      <c r="B171" s="14"/>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="14"/>
@@ -7403,6 +7850,27 @@
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193" s="14"/>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" s="14"/>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" s="14"/>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" s="14"/>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" s="14"/>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" s="14"/>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199" s="14"/>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added history path to users for saved DPRs. All tasks for creating and saving DPRs are now complete.
</commit_message>
<xml_diff>
--- a/Accessibility Chart.xlsx
+++ b/Accessibility Chart.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1554" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1571" uniqueCount="178">
   <si>
     <t>APP</t>
   </si>
@@ -4970,10 +4970,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K200"/>
+  <dimension ref="A1:K201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4983,6 +4983,8 @@
     <col min="3" max="3" width="16.5703125" style="15" customWidth="1"/>
     <col min="4" max="4" width="12.140625" style="15" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" style="15" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" customWidth="1"/>
     <col min="8" max="8" width="1.42578125" style="15" customWidth="1"/>
     <col min="9" max="9" width="27.5703125" style="15" customWidth="1"/>
     <col min="10" max="10" width="14.28515625" style="15" customWidth="1"/>
@@ -5380,7 +5382,12 @@
       <c r="I19" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="J19" s="14"/>
+      <c r="J19" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K19" s="14" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
@@ -5393,13 +5400,18 @@
         <v>81</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H20" s="17"/>
       <c r="I20" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="J20" s="14"/>
+        <v>122</v>
+      </c>
+      <c r="J20" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K20" s="14" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
@@ -5415,13 +5427,19 @@
         <v>81</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>63</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="F21" s="15"/>
       <c r="H21" s="17"/>
       <c r="I21" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="J21" s="14"/>
+        <v>124</v>
+      </c>
+      <c r="J21" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K21" s="14" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
@@ -5433,31 +5451,51 @@
       <c r="C22" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="D22" s="14" t="s">
-        <v>81</v>
-      </c>
       <c r="E22" s="14" t="s">
-        <v>101</v>
+        <v>81</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>63</v>
       </c>
       <c r="H22" s="17"/>
       <c r="I22" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="J22" s="14"/>
+        <v>123</v>
+      </c>
+      <c r="J22" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K22" s="14" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>81</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>101</v>
       </c>
       <c r="H23" s="17"/>
       <c r="I23" s="14" t="s">
-        <v>121</v>
+        <v>126</v>
+      </c>
+      <c r="J23" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="K23" s="14" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -5465,14 +5503,14 @@
         <v>81</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="H24" s="17"/>
       <c r="I24" s="14" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -5483,11 +5521,11 @@
         <v>81</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>19</v>
+        <v>79</v>
       </c>
       <c r="H25" s="17"/>
       <c r="I25" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -5498,11 +5536,11 @@
         <v>81</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H26" s="17"/>
       <c r="I26" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -5513,11 +5551,11 @@
         <v>81</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>129</v>
+        <v>20</v>
       </c>
       <c r="H27" s="17"/>
       <c r="I27" s="14" t="s">
-        <v>159</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -5528,11 +5566,11 @@
         <v>81</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>78</v>
+        <v>129</v>
       </c>
       <c r="H28" s="17"/>
       <c r="I28" s="14" t="s">
-        <v>113</v>
+        <v>159</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -5543,11 +5581,11 @@
         <v>81</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>21</v>
+        <v>78</v>
       </c>
       <c r="H29" s="17"/>
       <c r="I29" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -5558,11 +5596,11 @@
         <v>81</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>82</v>
+        <v>21</v>
       </c>
       <c r="H30" s="17"/>
       <c r="I30" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -5573,11 +5611,11 @@
         <v>81</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
       <c r="H31" s="17"/>
       <c r="I31" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -5588,13 +5626,12 @@
         <v>81</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>165</v>
+        <v>23</v>
       </c>
       <c r="H32" s="17"/>
       <c r="I32" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="J32" s="14"/>
+        <v>116</v>
+      </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
@@ -5604,12 +5641,13 @@
         <v>81</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>83</v>
+        <v>165</v>
       </c>
       <c r="H33" s="17"/>
       <c r="I33" s="14" t="s">
-        <v>117</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="J33" s="14"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
@@ -5619,11 +5657,11 @@
         <v>81</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>25</v>
+        <v>83</v>
       </c>
       <c r="H34" s="17"/>
       <c r="I34" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -5634,11 +5672,11 @@
         <v>81</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>84</v>
+        <v>25</v>
       </c>
       <c r="H35" s="17"/>
       <c r="I35" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -5649,14 +5687,11 @@
         <v>81</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D36" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H36" s="17"/>
       <c r="I36" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -5664,19 +5699,17 @@
         <v>81</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
+        <v>81</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>85</v>
+      </c>
       <c r="H37" s="17"/>
       <c r="I37" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="J37" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="K37" s="14" t="s">
-        <v>163</v>
+        <v>120</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -5684,15 +5717,13 @@
         <v>81</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C38" s="14" t="s">
-        <v>128</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="C38" s="14"/>
       <c r="D38" s="14"/>
       <c r="H38" s="17"/>
       <c r="I38" s="14" t="s">
-        <v>90</v>
+        <v>135</v>
       </c>
       <c r="J38" s="14" t="s">
         <v>163</v>
@@ -5709,14 +5740,12 @@
         <v>81</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D39" s="14" t="s">
         <v>128</v>
       </c>
+      <c r="D39" s="14"/>
       <c r="H39" s="17"/>
       <c r="I39" s="14" t="s">
-        <v>128</v>
+        <v>90</v>
       </c>
       <c r="J39" s="14" t="s">
         <v>163</v>
@@ -5736,11 +5765,11 @@
         <v>81</v>
       </c>
       <c r="D40" s="14" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="H40" s="17"/>
       <c r="I40" s="14" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="J40" s="14" t="s">
         <v>163</v>
@@ -5760,11 +5789,11 @@
         <v>81</v>
       </c>
       <c r="D41" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H41" s="17"/>
       <c r="I41" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J41" s="14" t="s">
         <v>163</v>
@@ -5784,11 +5813,11 @@
         <v>81</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H42" s="17"/>
       <c r="I42" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J42" s="14" t="s">
         <v>163</v>
@@ -5799,11 +5828,20 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
-        <v>27</v>
+        <v>81</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>120</v>
       </c>
       <c r="H43" s="17"/>
       <c r="I43" s="14" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J43" s="14" t="s">
         <v>163</v>
@@ -5814,16 +5852,13 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B44" s="14" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="H44" s="17"/>
       <c r="I44" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="J44" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="J44" s="14" t="s">
         <v>163</v>
       </c>
       <c r="K44" s="14" t="s">
@@ -5835,14 +5870,11 @@
         <v>81</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C45" s="14" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="H45" s="17"/>
       <c r="I45" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J45" s="15" t="s">
         <v>163</v>
@@ -5859,14 +5891,11 @@
         <v>81</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D46" s="14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H46" s="17"/>
       <c r="I46" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J46" s="15" t="s">
         <v>163</v>
@@ -5876,7 +5905,9 @@
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="14"/>
+      <c r="A47" s="14" t="s">
+        <v>81</v>
+      </c>
       <c r="B47" s="14" t="s">
         <v>81</v>
       </c>
@@ -5884,11 +5915,11 @@
         <v>81</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>160</v>
+        <v>29</v>
       </c>
       <c r="H47" s="17"/>
       <c r="I47" s="14" t="s">
-        <v>158</v>
+        <v>125</v>
       </c>
       <c r="J47" s="15" t="s">
         <v>163</v>
@@ -5898,9 +5929,7 @@
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="14" t="s">
-        <v>81</v>
-      </c>
+      <c r="A48" s="14"/>
       <c r="B48" s="14" t="s">
         <v>81</v>
       </c>
@@ -5908,11 +5937,11 @@
         <v>81</v>
       </c>
       <c r="D48" s="14" t="s">
-        <v>101</v>
+        <v>160</v>
       </c>
       <c r="H48" s="17"/>
       <c r="I48" s="14" t="s">
-        <v>126</v>
+        <v>158</v>
       </c>
       <c r="J48" s="15" t="s">
         <v>163</v>
@@ -5926,11 +5955,17 @@
         <v>81</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>30</v>
+        <v>81</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>101</v>
       </c>
       <c r="H49" s="17"/>
       <c r="I49" s="14" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="J49" s="15" t="s">
         <v>163</v>
@@ -5944,14 +5979,11 @@
         <v>81</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C50" s="14" t="s">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="H50" s="17"/>
       <c r="I50" s="14" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J50" s="15" t="s">
         <v>163</v>
@@ -5968,14 +6000,11 @@
         <v>81</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D51" s="14" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="H51" s="17"/>
       <c r="I51" s="14" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J51" s="15" t="s">
         <v>163</v>
@@ -5995,11 +6024,11 @@
         <v>81</v>
       </c>
       <c r="D52" s="14" t="s">
-        <v>160</v>
+        <v>29</v>
       </c>
       <c r="H52" s="17"/>
       <c r="I52" s="14" t="s">
-        <v>158</v>
+        <v>125</v>
       </c>
       <c r="J52" s="15" t="s">
         <v>163</v>
@@ -6019,11 +6048,11 @@
         <v>81</v>
       </c>
       <c r="D53" s="14" t="s">
-        <v>101</v>
+        <v>160</v>
       </c>
       <c r="H53" s="17"/>
       <c r="I53" s="14" t="s">
-        <v>126</v>
+        <v>158</v>
       </c>
       <c r="J53" s="15" t="s">
         <v>163</v>
@@ -6037,10 +6066,14 @@
         <v>81</v>
       </c>
       <c r="B54" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C54" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D54" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="C54" s="14"/>
-      <c r="D54" s="14"/>
       <c r="H54" s="17"/>
       <c r="I54" s="14" t="s">
         <v>126</v>
@@ -6057,17 +6090,15 @@
         <v>81</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C55" s="14" t="s">
-        <v>63</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="C55" s="14"/>
       <c r="D55" s="14"/>
       <c r="H55" s="17"/>
       <c r="I55" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="J55" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="J55" s="15" t="s">
         <v>163</v>
       </c>
       <c r="K55" s="14" t="s">
@@ -6082,12 +6113,12 @@
         <v>81</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="D56" s="14"/>
       <c r="H56" s="17"/>
       <c r="I56" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J56" s="14" t="s">
         <v>163</v>
@@ -6104,13 +6135,14 @@
         <v>81</v>
       </c>
       <c r="C57" s="14" t="s">
-        <v>29</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="D57" s="14"/>
       <c r="H57" s="17"/>
       <c r="I57" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="J57" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="J57" s="14" t="s">
         <v>163</v>
       </c>
       <c r="K57" s="14" t="s">
@@ -6125,11 +6157,11 @@
         <v>81</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>161</v>
+        <v>29</v>
       </c>
       <c r="H58" s="17"/>
       <c r="I58" s="14" t="s">
-        <v>162</v>
+        <v>125</v>
       </c>
       <c r="J58" s="15" t="s">
         <v>163</v>
@@ -6146,11 +6178,17 @@
         <v>81</v>
       </c>
       <c r="C59" s="14" t="s">
-        <v>100</v>
+        <v>161</v>
       </c>
       <c r="H59" s="17"/>
       <c r="I59" s="14" t="s">
-        <v>127</v>
+        <v>162</v>
+      </c>
+      <c r="J59" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="K59" s="14" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
@@ -6161,14 +6199,11 @@
         <v>81</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D60" s="14" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="H60" s="17"/>
       <c r="I60" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
@@ -6182,16 +6217,12 @@
         <v>81</v>
       </c>
       <c r="D61" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E61" s="14" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="H61" s="17"/>
       <c r="I61" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="K61" s="14"/>
+        <v>128</v>
+      </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="14" t="s">
@@ -6201,18 +6232,19 @@
         <v>81</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>31</v>
+        <v>81</v>
+      </c>
+      <c r="D62" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E62" s="14" t="s">
+        <v>30</v>
       </c>
       <c r="H62" s="17"/>
       <c r="I62" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="J62" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="K62" s="14" t="s">
-        <v>163</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="K62" s="14"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="s">
@@ -6222,11 +6254,11 @@
         <v>81</v>
       </c>
       <c r="C63" s="14" t="s">
-        <v>87</v>
+        <v>31</v>
       </c>
       <c r="H63" s="17"/>
       <c r="I63" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J63" s="14" t="s">
         <v>163</v>
@@ -6243,11 +6275,11 @@
         <v>81</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="H64" s="17"/>
       <c r="I64" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J64" s="14" t="s">
         <v>163</v>
@@ -6264,11 +6296,11 @@
         <v>81</v>
       </c>
       <c r="C65" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H65" s="17"/>
       <c r="I65" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J65" s="14" t="s">
         <v>163</v>
@@ -6285,11 +6317,11 @@
         <v>81</v>
       </c>
       <c r="C66" s="14" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="H66" s="17"/>
       <c r="I66" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J66" s="14" t="s">
         <v>163</v>
@@ -6306,11 +6338,11 @@
         <v>81</v>
       </c>
       <c r="C67" s="14" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="H67" s="17"/>
       <c r="I67" s="14" t="s">
-        <v>169</v>
+        <v>134</v>
       </c>
       <c r="J67" s="14" t="s">
         <v>163</v>
@@ -6327,14 +6359,11 @@
         <v>81</v>
       </c>
       <c r="C68" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D68" s="14" t="s">
-        <v>166</v>
+        <v>34</v>
       </c>
       <c r="H68" s="17"/>
-      <c r="I68" s="14">
-        <v>0</v>
+      <c r="I68" s="14" t="s">
+        <v>169</v>
       </c>
       <c r="J68" s="14" t="s">
         <v>163</v>
@@ -6354,17 +6383,11 @@
         <v>81</v>
       </c>
       <c r="D69" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E69" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="F69" s="16" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="H69" s="17"/>
-      <c r="I69" s="14" t="s">
-        <v>119</v>
+      <c r="I69" s="14">
+        <v>0</v>
       </c>
       <c r="J69" s="14" t="s">
         <v>163</v>
@@ -6387,14 +6410,14 @@
         <v>81</v>
       </c>
       <c r="E70" s="14" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="F70" s="16" t="s">
         <v>170</v>
       </c>
       <c r="H70" s="17"/>
       <c r="I70" s="14" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="J70" s="14" t="s">
         <v>163</v>
@@ -6417,11 +6440,14 @@
         <v>81</v>
       </c>
       <c r="E71" s="14" t="s">
-        <v>85</v>
+        <v>25</v>
+      </c>
+      <c r="F71" s="16" t="s">
+        <v>170</v>
       </c>
       <c r="H71" s="17"/>
       <c r="I71" s="14" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J71" s="14" t="s">
         <v>163</v>
@@ -6444,11 +6470,11 @@
         <v>81</v>
       </c>
       <c r="E72" s="14" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="H72" s="17"/>
       <c r="I72" s="14" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="J72" s="14" t="s">
         <v>163</v>
@@ -6471,11 +6497,11 @@
         <v>81</v>
       </c>
       <c r="E73" s="14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H73" s="17"/>
       <c r="I73" s="14" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="J73" s="14" t="s">
         <v>163</v>
@@ -6495,11 +6521,14 @@
         <v>81</v>
       </c>
       <c r="D74" s="14" t="s">
-        <v>166</v>
+        <v>81</v>
+      </c>
+      <c r="E74" s="14" t="s">
+        <v>88</v>
       </c>
       <c r="H74" s="17"/>
-      <c r="I74" s="14">
-        <v>1</v>
+      <c r="I74" s="14" t="s">
+        <v>136</v>
       </c>
       <c r="J74" s="14" t="s">
         <v>163</v>
@@ -6519,17 +6548,11 @@
         <v>81</v>
       </c>
       <c r="D75" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E75" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="F75" s="16" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="H75" s="17"/>
-      <c r="I75" s="14" t="s">
-        <v>119</v>
+      <c r="I75" s="14">
+        <v>1</v>
       </c>
       <c r="J75" s="14" t="s">
         <v>163</v>
@@ -6552,14 +6575,14 @@
         <v>81</v>
       </c>
       <c r="E76" s="14" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="F76" s="16" t="s">
         <v>170</v>
       </c>
       <c r="H76" s="17"/>
       <c r="I76" s="14" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="J76" s="14" t="s">
         <v>163</v>
@@ -6582,11 +6605,14 @@
         <v>81</v>
       </c>
       <c r="E77" s="14" t="s">
-        <v>85</v>
+        <v>25</v>
+      </c>
+      <c r="F77" s="16" t="s">
+        <v>170</v>
       </c>
       <c r="H77" s="17"/>
       <c r="I77" s="14" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J77" s="14" t="s">
         <v>163</v>
@@ -6609,11 +6635,11 @@
         <v>81</v>
       </c>
       <c r="E78" s="14" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="H78" s="17"/>
       <c r="I78" s="14" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="J78" s="14" t="s">
         <v>163</v>
@@ -6636,11 +6662,11 @@
         <v>81</v>
       </c>
       <c r="E79" s="14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H79" s="17"/>
       <c r="I79" s="14" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="J79" s="14" t="s">
         <v>163</v>
@@ -6657,13 +6683,19 @@
         <v>81</v>
       </c>
       <c r="C80" s="14" t="s">
-        <v>89</v>
+        <v>81</v>
+      </c>
+      <c r="D80" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E80" s="14" t="s">
+        <v>88</v>
       </c>
       <c r="H80" s="17"/>
       <c r="I80" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="J80" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="J80" s="14" t="s">
         <v>163</v>
       </c>
       <c r="K80" s="14" t="s">
@@ -6678,11 +6710,11 @@
         <v>81</v>
       </c>
       <c r="C81" s="14" t="s">
-        <v>172</v>
+        <v>89</v>
       </c>
       <c r="H81" s="17"/>
       <c r="I81" s="14" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="J81" s="15" t="s">
         <v>163</v>
@@ -6699,11 +6731,11 @@
         <v>81</v>
       </c>
       <c r="C82" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H82" s="17"/>
       <c r="I82" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="J82" s="15" t="s">
         <v>163</v>
@@ -6720,11 +6752,11 @@
         <v>81</v>
       </c>
       <c r="C83" s="14" t="s">
-        <v>91</v>
+        <v>173</v>
       </c>
       <c r="H83" s="17"/>
       <c r="I83" s="14" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="J83" s="15" t="s">
         <v>163</v>
@@ -6741,16 +6773,13 @@
         <v>81</v>
       </c>
       <c r="C84" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D84" s="14" t="s">
-        <v>166</v>
+        <v>91</v>
       </c>
       <c r="H84" s="17"/>
-      <c r="I84" s="14">
-        <v>0</v>
-      </c>
-      <c r="J84" s="14" t="s">
+      <c r="I84" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="J84" s="15" t="s">
         <v>163</v>
       </c>
       <c r="K84" s="14" t="s">
@@ -6768,16 +6797,13 @@
         <v>81</v>
       </c>
       <c r="D85" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E85" s="14" t="s">
-        <v>92</v>
+        <v>166</v>
       </c>
       <c r="H85" s="17"/>
-      <c r="I85" s="14" t="s">
-        <v>171</v>
-      </c>
-      <c r="J85" s="15" t="s">
+      <c r="I85" s="14">
+        <v>0</v>
+      </c>
+      <c r="J85" s="14" t="s">
         <v>163</v>
       </c>
       <c r="K85" s="14" t="s">
@@ -6798,11 +6824,11 @@
         <v>81</v>
       </c>
       <c r="E86" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H86" s="17"/>
       <c r="I86" s="14" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
       <c r="J86" s="15" t="s">
         <v>163</v>
@@ -6819,11 +6845,17 @@
         <v>81</v>
       </c>
       <c r="C87" s="14" t="s">
-        <v>94</v>
+        <v>81</v>
+      </c>
+      <c r="D87" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E87" s="14" t="s">
+        <v>93</v>
       </c>
       <c r="H87" s="17"/>
       <c r="I87" s="14" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J87" s="15" t="s">
         <v>163</v>
@@ -6840,16 +6872,13 @@
         <v>81</v>
       </c>
       <c r="C88" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D88" s="14" t="s">
-        <v>166</v>
+        <v>94</v>
       </c>
       <c r="H88" s="17"/>
-      <c r="I88" s="14">
-        <v>0</v>
-      </c>
-      <c r="J88" s="14" t="s">
+      <c r="I88" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="J88" s="15" t="s">
         <v>163</v>
       </c>
       <c r="K88" s="14" t="s">
@@ -6867,17 +6896,13 @@
         <v>81</v>
       </c>
       <c r="D89" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E89" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="F89" s="15"/>
+        <v>166</v>
+      </c>
       <c r="H89" s="17"/>
-      <c r="I89" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="J89" s="15" t="s">
+      <c r="I89" s="14">
+        <v>0</v>
+      </c>
+      <c r="J89" s="14" t="s">
         <v>163</v>
       </c>
       <c r="K89" s="14" t="s">
@@ -6898,14 +6923,12 @@
         <v>81</v>
       </c>
       <c r="E90" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="F90" s="14" t="s">
-        <v>95</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="F90" s="15"/>
       <c r="H90" s="17"/>
       <c r="I90" s="14" t="s">
-        <v>167</v>
+        <v>141</v>
       </c>
       <c r="J90" s="15" t="s">
         <v>163</v>
@@ -6931,11 +6954,11 @@
         <v>81</v>
       </c>
       <c r="F91" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H91" s="17"/>
       <c r="I91" s="14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="J91" s="15" t="s">
         <v>163</v>
@@ -6961,11 +6984,11 @@
         <v>81</v>
       </c>
       <c r="F92" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H92" s="17"/>
       <c r="I92" s="14" t="s">
-        <v>142</v>
+        <v>168</v>
       </c>
       <c r="J92" s="15" t="s">
         <v>163</v>
@@ -6991,11 +7014,11 @@
         <v>81</v>
       </c>
       <c r="F93" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H93" s="17"/>
       <c r="I93" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J93" s="15" t="s">
         <v>163</v>
@@ -7021,11 +7044,11 @@
         <v>81</v>
       </c>
       <c r="F94" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H94" s="17"/>
       <c r="I94" s="14" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="J94" s="15" t="s">
         <v>163</v>
@@ -7036,23 +7059,41 @@
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="14" t="s">
-        <v>102</v>
+        <v>81</v>
+      </c>
+      <c r="B95" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C95" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D95" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E95" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F95" s="14" t="s">
+        <v>99</v>
       </c>
       <c r="H95" s="17"/>
       <c r="I95" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
+      </c>
+      <c r="J95" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="K95" s="14" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B96" s="14" t="s">
-        <v>63</v>
+        <v>102</v>
       </c>
       <c r="H96" s="17"/>
       <c r="I96" s="14" t="s">
-        <v>123</v>
+        <v>147</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
@@ -7060,14 +7101,11 @@
         <v>81</v>
       </c>
       <c r="B97" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C97" s="14" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="H97" s="17"/>
       <c r="I97" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
@@ -7078,14 +7116,11 @@
         <v>81</v>
       </c>
       <c r="C98" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D98" s="14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H98" s="17"/>
       <c r="I98" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
@@ -7099,11 +7134,11 @@
         <v>81</v>
       </c>
       <c r="D99" s="14" t="s">
-        <v>101</v>
+        <v>29</v>
       </c>
       <c r="H99" s="17"/>
       <c r="I99" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
@@ -7117,11 +7152,11 @@
         <v>81</v>
       </c>
       <c r="D100" s="14" t="s">
-        <v>32</v>
+        <v>101</v>
       </c>
       <c r="H100" s="17"/>
       <c r="I100" s="14" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
@@ -7135,11 +7170,11 @@
         <v>81</v>
       </c>
       <c r="D101" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H101" s="17"/>
       <c r="I101" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
@@ -7153,11 +7188,11 @@
         <v>81</v>
       </c>
       <c r="D102" s="14" t="s">
-        <v>88</v>
+        <v>33</v>
       </c>
       <c r="H102" s="17"/>
       <c r="I102" s="14" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
@@ -7165,11 +7200,17 @@
         <v>81</v>
       </c>
       <c r="B103" s="14" t="s">
-        <v>30</v>
+        <v>81</v>
+      </c>
+      <c r="C103" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D103" s="14" t="s">
+        <v>88</v>
       </c>
       <c r="H103" s="17"/>
       <c r="I103" s="14" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
@@ -7177,14 +7218,11 @@
         <v>81</v>
       </c>
       <c r="B104" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C104" s="14" t="s">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="H104" s="17"/>
       <c r="I104" s="14" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
@@ -7195,14 +7233,11 @@
         <v>81</v>
       </c>
       <c r="C105" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D105" s="14" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="H105" s="17"/>
       <c r="I105" s="14" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
@@ -7216,11 +7251,11 @@
         <v>81</v>
       </c>
       <c r="D106" s="14" t="s">
-        <v>101</v>
+        <v>29</v>
       </c>
       <c r="H106" s="17"/>
       <c r="I106" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
@@ -7234,11 +7269,11 @@
         <v>81</v>
       </c>
       <c r="D107" s="14" t="s">
-        <v>32</v>
+        <v>101</v>
       </c>
       <c r="H107" s="17"/>
       <c r="I107" s="14" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
@@ -7252,11 +7287,11 @@
         <v>81</v>
       </c>
       <c r="D108" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H108" s="17"/>
       <c r="I108" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
@@ -7270,11 +7305,11 @@
         <v>81</v>
       </c>
       <c r="D109" s="14" t="s">
-        <v>88</v>
+        <v>33</v>
       </c>
       <c r="H109" s="17"/>
       <c r="I109" s="14" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
@@ -7282,13 +7317,17 @@
         <v>81</v>
       </c>
       <c r="B110" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="C110" s="14"/>
-      <c r="D110" s="14"/>
+        <v>81</v>
+      </c>
+      <c r="C110" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D110" s="14" t="s">
+        <v>88</v>
+      </c>
       <c r="H110" s="17"/>
       <c r="I110" s="14" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
@@ -7296,15 +7335,13 @@
         <v>81</v>
       </c>
       <c r="B111" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C111" s="14" t="s">
-        <v>63</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="C111" s="14"/>
       <c r="D111" s="14"/>
       <c r="H111" s="17"/>
       <c r="I111" s="14" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
@@ -7315,12 +7352,12 @@
         <v>81</v>
       </c>
       <c r="C112" s="14" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="D112" s="14"/>
       <c r="H112" s="17"/>
       <c r="I112" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
@@ -7331,11 +7368,12 @@
         <v>81</v>
       </c>
       <c r="C113" s="14" t="s">
-        <v>29</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="D113" s="14"/>
       <c r="H113" s="17"/>
       <c r="I113" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
@@ -7346,11 +7384,11 @@
         <v>81</v>
       </c>
       <c r="C114" s="14" t="s">
-        <v>161</v>
+        <v>29</v>
       </c>
       <c r="H114" s="17"/>
       <c r="I114" s="14" t="s">
-        <v>162</v>
+        <v>125</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
@@ -7361,11 +7399,11 @@
         <v>81</v>
       </c>
       <c r="C115" s="14" t="s">
-        <v>100</v>
+        <v>161</v>
       </c>
       <c r="H115" s="17"/>
       <c r="I115" s="14" t="s">
-        <v>127</v>
+        <v>162</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
@@ -7376,14 +7414,11 @@
         <v>81</v>
       </c>
       <c r="C116" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D116" s="14" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="H116" s="17"/>
       <c r="I116" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
@@ -7397,14 +7432,11 @@
         <v>81</v>
       </c>
       <c r="D117" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E117" s="14" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="H117" s="17"/>
       <c r="I117" s="14" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
@@ -7415,11 +7447,17 @@
         <v>81</v>
       </c>
       <c r="C118" s="14" t="s">
-        <v>31</v>
+        <v>81</v>
+      </c>
+      <c r="D118" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E118" s="14" t="s">
+        <v>30</v>
       </c>
       <c r="H118" s="17"/>
       <c r="I118" s="14" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
@@ -7430,11 +7468,11 @@
         <v>81</v>
       </c>
       <c r="C119" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H119" s="17"/>
       <c r="I119" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
@@ -7445,11 +7483,11 @@
         <v>81</v>
       </c>
       <c r="C120" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H120" s="17"/>
       <c r="I120" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
@@ -7460,11 +7498,11 @@
         <v>81</v>
       </c>
       <c r="C121" s="14" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="H121" s="17"/>
       <c r="I121" s="14" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
@@ -7475,14 +7513,11 @@
         <v>81</v>
       </c>
       <c r="C122" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="D122" s="16" t="s">
-        <v>108</v>
+        <v>50</v>
       </c>
       <c r="H122" s="17"/>
       <c r="I122" s="14" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
@@ -7493,11 +7528,14 @@
         <v>81</v>
       </c>
       <c r="C123" s="14" t="s">
-        <v>103</v>
+        <v>107</v>
+      </c>
+      <c r="D123" s="16" t="s">
+        <v>108</v>
       </c>
       <c r="H123" s="17"/>
       <c r="I123" s="14" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
@@ -7508,14 +7546,11 @@
         <v>81</v>
       </c>
       <c r="C124" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D124" s="14" t="s">
-        <v>65</v>
+        <v>103</v>
       </c>
       <c r="H124" s="17"/>
       <c r="I124" s="14" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
@@ -7529,14 +7564,11 @@
         <v>81</v>
       </c>
       <c r="D125" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E125" s="14" t="s">
-        <v>106</v>
+        <v>65</v>
       </c>
       <c r="H125" s="17"/>
       <c r="I125" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
@@ -7553,11 +7585,11 @@
         <v>81</v>
       </c>
       <c r="E126" s="14" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="H126" s="17"/>
       <c r="I126" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
@@ -7574,11 +7606,11 @@
         <v>81</v>
       </c>
       <c r="E127" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H127" s="17"/>
       <c r="I127" s="14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
@@ -7595,11 +7627,11 @@
         <v>81</v>
       </c>
       <c r="E128" s="14" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="H128" s="17"/>
       <c r="I128" s="14" t="s">
-        <v>136</v>
+        <v>152</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
@@ -7610,16 +7642,33 @@
         <v>81</v>
       </c>
       <c r="C129" s="14" t="s">
-        <v>54</v>
+        <v>81</v>
+      </c>
+      <c r="D129" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E129" s="14" t="s">
+        <v>88</v>
       </c>
       <c r="H129" s="17"/>
       <c r="I129" s="14" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A130" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B130" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C130" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="H130" s="17"/>
+      <c r="I130" s="14" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A130" s="14"/>
-      <c r="B130" s="14"/>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="14"/>
@@ -7787,6 +7836,7 @@
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="14"/>
+      <c r="B172" s="14"/>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="14"/>
@@ -7871,6 +7921,9 @@
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200" s="14"/>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
DTR: 	Finished saving data to firebase. DPR: 	Edited how data for job#/date and date/job# and user history to 	avoid overwrites for the same date and job #
</commit_message>
<xml_diff>
--- a/Accessibility Chart.xlsx
+++ b/Accessibility Chart.xlsx
@@ -14,13 +14,14 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1571" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1757" uniqueCount="248">
   <si>
     <t>APP</t>
   </si>
@@ -331,18 +332,9 @@
     <t>DTR</t>
   </si>
   <si>
-    <t>Work Perfomed</t>
-  </si>
-  <si>
     <t>Materials Issued</t>
   </si>
   <si>
-    <t>Materials Used</t>
-  </si>
-  <si>
-    <t>Work Performed</t>
-  </si>
-  <si>
     <t>OSP/ISP</t>
   </si>
   <si>
@@ -439,9 +431,6 @@
     <t>work</t>
   </si>
   <si>
-    <t>workDone</t>
-  </si>
-  <si>
     <t>progress</t>
   </si>
   <si>
@@ -469,21 +458,9 @@
     <t>type</t>
   </si>
   <si>
-    <t>costCode</t>
-  </si>
-  <si>
-    <t>performed</t>
-  </si>
-  <si>
     <t>matIssued</t>
   </si>
   <si>
-    <t>matUsed</t>
-  </si>
-  <si>
-    <t>issues</t>
-  </si>
-  <si>
     <t>cellNum</t>
   </si>
   <si>
@@ -554,6 +531,240 @@
   </si>
   <si>
     <t>userID</t>
+  </si>
+  <si>
+    <t>OSP</t>
+  </si>
+  <si>
+    <t>ISP</t>
+  </si>
+  <si>
+    <t>cost code</t>
+  </si>
+  <si>
+    <t>OSP (Including Site Work):</t>
+  </si>
+  <si>
+    <t>MAINTENANCE HOLE SETUP</t>
+  </si>
+  <si>
+    <t>ROD AND ROPE</t>
+  </si>
+  <si>
+    <t>INSTALL INNDERDUCT</t>
+  </si>
+  <si>
+    <t>INSTALL CABLE</t>
+  </si>
+  <si>
+    <t>MAINTENENANCE HOLE/OUTDOOR WORK:</t>
+  </si>
+  <si>
+    <t>DRESS CABLES</t>
+  </si>
+  <si>
+    <t>INSTALL DUCT SEAL</t>
+  </si>
+  <si>
+    <t>INSTALL TERMINATIONS BAGS</t>
+  </si>
+  <si>
+    <t>INSTALL LABLEING</t>
+  </si>
+  <si>
+    <t>SPLICING WORK</t>
+  </si>
+  <si>
+    <t>MOUNT EQUIPMENT</t>
+  </si>
+  <si>
+    <t>TERMINATIONS</t>
+  </si>
+  <si>
+    <t>TESTING</t>
+  </si>
+  <si>
+    <t>MAINTENANCE HOLD GUARD</t>
+  </si>
+  <si>
+    <t>TRAFFIC CONTROL</t>
+  </si>
+  <si>
+    <t>INDIRECT LABOR COSTS</t>
+  </si>
+  <si>
+    <t>PUNCHLIST</t>
+  </si>
+  <si>
+    <t>TROUBLESHOOTING</t>
+  </si>
+  <si>
+    <t>MATERIALS HANDLING</t>
+  </si>
+  <si>
+    <t>OSP DEMO</t>
+  </si>
+  <si>
+    <t>2-001</t>
+  </si>
+  <si>
+    <t>2-002</t>
+  </si>
+  <si>
+    <t>8-006</t>
+  </si>
+  <si>
+    <t>8-007</t>
+  </si>
+  <si>
+    <t>11-002</t>
+  </si>
+  <si>
+    <t>PATHWAYS AND SPACES</t>
+  </si>
+  <si>
+    <t>INSTALL CEILING HANGER</t>
+  </si>
+  <si>
+    <t>INSTALL J-HOOK</t>
+  </si>
+  <si>
+    <t>INSTALL SLEEPVE (DRYWALL)</t>
+  </si>
+  <si>
+    <t>INSTALL SLEEVE (CONCRETE)</t>
+  </si>
+  <si>
+    <t>INSTALL CONDUIT</t>
+  </si>
+  <si>
+    <t>INSTALL CABLE/RUNWAY/TRAY</t>
+  </si>
+  <si>
+    <t>INSTALL BACKBOARD</t>
+  </si>
+  <si>
+    <t>INSTALL CABLE RUNWAY/TRAY</t>
+  </si>
+  <si>
+    <t>INSTALL GROUND WIRE</t>
+  </si>
+  <si>
+    <t>INSTALL RACK/CABINET</t>
+  </si>
+  <si>
+    <t>IDF EQUIPMENT MOUNTING</t>
+  </si>
+  <si>
+    <t>IDF HORIZ CABLE DRESSING</t>
+  </si>
+  <si>
+    <t>IDF HORIZ CABLE TERMINATIONS</t>
+  </si>
+  <si>
+    <t>IDF LABELING</t>
+  </si>
+  <si>
+    <t>RISER CABLE ROUGH IN</t>
+  </si>
+  <si>
+    <t>RISER CABLE DRESSING</t>
+  </si>
+  <si>
+    <t>RISER CABLE TERMINATIONS</t>
+  </si>
+  <si>
+    <t>HORIZONTAL WORK:</t>
+  </si>
+  <si>
+    <t>IDF TESTING</t>
+  </si>
+  <si>
+    <t>RISERS:</t>
+  </si>
+  <si>
+    <t>MDF/IDF WORK:</t>
+  </si>
+  <si>
+    <t>INSTALL PULL STRING</t>
+  </si>
+  <si>
+    <t>CABLE ROUGH-IN</t>
+  </si>
+  <si>
+    <t>FISH WALL</t>
+  </si>
+  <si>
+    <t>INSTALL MPLS</t>
+  </si>
+  <si>
+    <t>INSTALL WIREMOLD</t>
+  </si>
+  <si>
+    <t>TERMINATE JACKS</t>
+  </si>
+  <si>
+    <t>INSTALL FACEPLATES</t>
+  </si>
+  <si>
+    <t>INDIRECT LABOR COSTS:</t>
+  </si>
+  <si>
+    <t>MATERIAL HANDLING</t>
+  </si>
+  <si>
+    <t>DEMO:</t>
+  </si>
+  <si>
+    <t>ISP DEMO</t>
+  </si>
+  <si>
+    <t>RISER DEMO</t>
+  </si>
+  <si>
+    <t>3-001</t>
+  </si>
+  <si>
+    <t>4-001</t>
+  </si>
+  <si>
+    <t>4-002</t>
+  </si>
+  <si>
+    <t>4-003</t>
+  </si>
+  <si>
+    <t>4-004</t>
+  </si>
+  <si>
+    <t>4-005</t>
+  </si>
+  <si>
+    <t>5-001</t>
+  </si>
+  <si>
+    <t>6-x0x/7-00x</t>
+  </si>
+  <si>
+    <t>11-001</t>
+  </si>
+  <si>
+    <t>11-003</t>
+  </si>
+  <si>
+    <t>timeTotal</t>
+  </si>
+  <si>
+    <t>Issues/Questions/Remarks</t>
+  </si>
+  <si>
+    <t># According to Sheet3 (work performed/cost code)</t>
+  </si>
+  <si>
+    <t>matInstalled</t>
+  </si>
+  <si>
+    <t>Materials Installed</t>
   </si>
 </sst>
 </file>
@@ -586,7 +797,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -608,6 +819,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -712,7 +929,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -752,6 +969,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4970,10 +5190,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K201"/>
+  <dimension ref="A1:K207"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
+      <selection activeCell="D125" sqref="D125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4981,7 +5201,7 @@
     <col min="1" max="1" width="11.140625" style="15" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" style="15" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" style="15" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" style="15" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="15" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" style="15" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
     <col min="7" max="7" width="10.5703125" customWidth="1"/>
@@ -4994,7 +5214,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="B1" s="15">
         <v>1</v>
@@ -5012,13 +5232,13 @@
         <v>5</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="J1" s="14" t="s">
         <v>92</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5040,13 +5260,13 @@
       </c>
       <c r="H3" s="17"/>
       <c r="I3" s="14" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K3" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -5057,17 +5277,17 @@
         <v>77</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="H4" s="17"/>
       <c r="I4" s="14" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -5078,17 +5298,17 @@
         <v>81</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="H5" s="17"/>
       <c r="I5" s="14" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="J5" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K5" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -5103,13 +5323,13 @@
       </c>
       <c r="H6" s="17"/>
       <c r="I6" s="14" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -5124,13 +5344,13 @@
       </c>
       <c r="H7" s="17"/>
       <c r="I7" s="14" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -5145,13 +5365,13 @@
       </c>
       <c r="H8" s="17"/>
       <c r="I8" s="14" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K8" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -5162,17 +5382,17 @@
         <v>81</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="H9" s="17"/>
       <c r="I9" s="14" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -5187,13 +5407,13 @@
       </c>
       <c r="H10" s="17"/>
       <c r="I10" s="14" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K10" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -5208,13 +5428,13 @@
       </c>
       <c r="H11" s="17"/>
       <c r="I11" s="14" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K11" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -5229,13 +5449,13 @@
       </c>
       <c r="H12" s="17"/>
       <c r="I12" s="14" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K12" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -5250,13 +5470,13 @@
       </c>
       <c r="H13" s="17"/>
       <c r="I13" s="14" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K13" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -5267,17 +5487,17 @@
         <v>81</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="H14" s="17"/>
       <c r="I14" s="14" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="J14" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K14" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -5292,13 +5512,13 @@
       </c>
       <c r="H15" s="17"/>
       <c r="I15" s="14" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="J15" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K15" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -5313,13 +5533,13 @@
       </c>
       <c r="H16" s="17"/>
       <c r="I16" s="14" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="J16" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K16" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -5334,13 +5554,13 @@
       </c>
       <c r="H17" s="17"/>
       <c r="I17" s="14" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J17" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K17" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -5358,13 +5578,13 @@
       </c>
       <c r="H18" s="17"/>
       <c r="I18" s="14" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J18" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K18" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -5375,18 +5595,18 @@
         <v>81</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="D19" s="14"/>
       <c r="H19" s="17"/>
       <c r="I19" s="14" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="J19" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K19" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -5404,13 +5624,13 @@
       </c>
       <c r="H20" s="17"/>
       <c r="I20" s="14" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="J20" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K20" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -5432,13 +5652,13 @@
       <c r="F21" s="15"/>
       <c r="H21" s="17"/>
       <c r="I21" s="14" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="J21" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K21" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -5459,13 +5679,13 @@
       </c>
       <c r="H22" s="17"/>
       <c r="I22" s="14" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="J22" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K22" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -5489,13 +5709,13 @@
       </c>
       <c r="H23" s="17"/>
       <c r="I23" s="14" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="J23" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K23" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -5503,14 +5723,23 @@
         <v>81</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>102</v>
       </c>
       <c r="H24" s="17"/>
       <c r="I24" s="14" t="s">
-        <v>121</v>
+        <v>143</v>
+      </c>
+      <c r="J24" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="K24" s="14" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -5521,11 +5750,24 @@
         <v>81</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>79</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" s="15"/>
       <c r="H25" s="17"/>
       <c r="I25" s="14" t="s">
-        <v>110</v>
+        <v>121</v>
+      </c>
+      <c r="J25" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="K25" s="14" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -5536,11 +5778,23 @@
         <v>81</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>19</v>
+        <v>81</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>63</v>
       </c>
       <c r="H26" s="17"/>
       <c r="I26" s="14" t="s">
-        <v>111</v>
+        <v>120</v>
+      </c>
+      <c r="J26" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="K26" s="14" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -5551,11 +5805,26 @@
         <v>81</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>20</v>
+        <v>81</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>101</v>
       </c>
       <c r="H27" s="17"/>
       <c r="I27" s="14" t="s">
-        <v>112</v>
+        <v>123</v>
+      </c>
+      <c r="J27" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="K27" s="14" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -5563,14 +5832,14 @@
         <v>81</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>129</v>
+        <v>82</v>
       </c>
       <c r="H28" s="17"/>
       <c r="I28" s="14" t="s">
-        <v>159</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -5581,11 +5850,11 @@
         <v>81</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H29" s="17"/>
       <c r="I29" s="14" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -5596,11 +5865,11 @@
         <v>81</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="H30" s="17"/>
       <c r="I30" s="14" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -5611,11 +5880,11 @@
         <v>81</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>82</v>
+        <v>20</v>
       </c>
       <c r="H31" s="17"/>
       <c r="I31" s="14" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -5626,11 +5895,11 @@
         <v>81</v>
       </c>
       <c r="C32" s="14" t="s">
-        <v>23</v>
+        <v>126</v>
       </c>
       <c r="H32" s="17"/>
       <c r="I32" s="14" t="s">
-        <v>116</v>
+        <v>151</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -5641,13 +5910,12 @@
         <v>81</v>
       </c>
       <c r="C33" s="14" t="s">
-        <v>165</v>
+        <v>78</v>
       </c>
       <c r="H33" s="17"/>
       <c r="I33" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="J33" s="14"/>
+        <v>110</v>
+      </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
@@ -5657,11 +5925,11 @@
         <v>81</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>83</v>
+        <v>21</v>
       </c>
       <c r="H34" s="17"/>
       <c r="I34" s="14" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -5672,11 +5940,11 @@
         <v>81</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>25</v>
+        <v>82</v>
       </c>
       <c r="H35" s="17"/>
       <c r="I35" s="14" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -5687,11 +5955,11 @@
         <v>81</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>84</v>
+        <v>23</v>
       </c>
       <c r="H36" s="17"/>
       <c r="I36" s="14" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -5702,34 +5970,27 @@
         <v>81</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D37" s="14" t="s">
-        <v>85</v>
+        <v>157</v>
       </c>
       <c r="H37" s="17"/>
       <c r="I37" s="14" t="s">
-        <v>120</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="J37" s="14"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
         <v>81</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
+        <v>81</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>83</v>
+      </c>
       <c r="H38" s="17"/>
       <c r="I38" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="J38" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="K38" s="14" t="s">
-        <v>163</v>
+        <v>114</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -5740,18 +6001,11 @@
         <v>81</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="D39" s="14"/>
+        <v>25</v>
+      </c>
       <c r="H39" s="17"/>
       <c r="I39" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="J39" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="K39" s="14" t="s">
-        <v>163</v>
+        <v>115</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -5762,20 +6016,11 @@
         <v>81</v>
       </c>
       <c r="C40" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D40" s="14" t="s">
-        <v>128</v>
+        <v>84</v>
       </c>
       <c r="H40" s="17"/>
       <c r="I40" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="J40" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="K40" s="14" t="s">
-        <v>163</v>
+        <v>116</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -5789,17 +6034,11 @@
         <v>81</v>
       </c>
       <c r="D41" s="14" t="s">
-        <v>118</v>
+        <v>85</v>
       </c>
       <c r="H41" s="17"/>
       <c r="I41" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="J41" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="K41" s="14" t="s">
-        <v>163</v>
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -5807,23 +6046,19 @@
         <v>81</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C42" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D42" s="14" t="s">
-        <v>119</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
       <c r="H42" s="17"/>
       <c r="I42" s="14" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="J42" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K42" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -5834,35 +6069,42 @@
         <v>81</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D43" s="14" t="s">
-        <v>120</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="D43" s="14"/>
       <c r="H43" s="17"/>
       <c r="I43" s="14" t="s">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="J43" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K43" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
-        <v>27</v>
+        <v>81</v>
+      </c>
+      <c r="B44" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>125</v>
       </c>
       <c r="H44" s="17"/>
       <c r="I44" s="14" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="J44" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K44" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -5870,17 +6112,23 @@
         <v>81</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>63</v>
+        <v>81</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D45" s="14" t="s">
+        <v>115</v>
       </c>
       <c r="H45" s="17"/>
       <c r="I45" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="J45" s="15" t="s">
-        <v>163</v>
+        <v>115</v>
+      </c>
+      <c r="J45" s="14" t="s">
+        <v>155</v>
       </c>
       <c r="K45" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
@@ -5891,17 +6139,20 @@
         <v>81</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>30</v>
+        <v>81</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>116</v>
       </c>
       <c r="H46" s="17"/>
       <c r="I46" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="J46" s="15" t="s">
-        <v>163</v>
+        <v>116</v>
+      </c>
+      <c r="J46" s="14" t="s">
+        <v>155</v>
       </c>
       <c r="K46" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -5915,39 +6166,32 @@
         <v>81</v>
       </c>
       <c r="D47" s="14" t="s">
-        <v>29</v>
+        <v>117</v>
       </c>
       <c r="H47" s="17"/>
       <c r="I47" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="J47" s="15" t="s">
-        <v>163</v>
+        <v>117</v>
+      </c>
+      <c r="J47" s="14" t="s">
+        <v>155</v>
       </c>
       <c r="K47" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="14"/>
-      <c r="B48" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C48" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D48" s="14" t="s">
-        <v>160</v>
+      <c r="A48" s="14" t="s">
+        <v>27</v>
       </c>
       <c r="H48" s="17"/>
       <c r="I48" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="J48" s="15" t="s">
-        <v>163</v>
+        <v>119</v>
+      </c>
+      <c r="J48" s="14" t="s">
+        <v>155</v>
       </c>
       <c r="K48" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -5955,23 +6199,17 @@
         <v>81</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C49" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D49" s="14" t="s">
-        <v>101</v>
+        <v>63</v>
       </c>
       <c r="H49" s="17"/>
       <c r="I49" s="14" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="J49" s="15" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K49" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -5979,17 +6217,20 @@
         <v>81</v>
       </c>
       <c r="B50" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C50" s="14" t="s">
         <v>30</v>
       </c>
       <c r="H50" s="17"/>
       <c r="I50" s="14" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="J50" s="15" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K50" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -6000,17 +6241,20 @@
         <v>81</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>63</v>
+        <v>81</v>
+      </c>
+      <c r="D51" s="14" t="s">
+        <v>29</v>
       </c>
       <c r="H51" s="17"/>
       <c r="I51" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J51" s="15" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K51" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -6024,17 +6268,17 @@
         <v>81</v>
       </c>
       <c r="D52" s="14" t="s">
-        <v>29</v>
+        <v>152</v>
       </c>
       <c r="H52" s="17"/>
       <c r="I52" s="14" t="s">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="J52" s="15" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K52" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
@@ -6048,17 +6292,17 @@
         <v>81</v>
       </c>
       <c r="D53" s="14" t="s">
-        <v>160</v>
+        <v>101</v>
       </c>
       <c r="H53" s="17"/>
       <c r="I53" s="14" t="s">
-        <v>158</v>
+        <v>123</v>
       </c>
       <c r="J53" s="15" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K53" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -6066,23 +6310,17 @@
         <v>81</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C54" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D54" s="14" t="s">
-        <v>101</v>
+        <v>30</v>
       </c>
       <c r="H54" s="17"/>
       <c r="I54" s="14" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="J54" s="15" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K54" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
@@ -6090,19 +6328,20 @@
         <v>81</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="C55" s="14"/>
-      <c r="D55" s="14"/>
+        <v>81</v>
+      </c>
+      <c r="C55" s="14" t="s">
+        <v>63</v>
+      </c>
       <c r="H55" s="17"/>
       <c r="I55" s="14" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="J55" s="15" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K55" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
@@ -6113,18 +6352,20 @@
         <v>81</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="D56" s="14"/>
+        <v>81</v>
+      </c>
+      <c r="D56" s="14" t="s">
+        <v>29</v>
+      </c>
       <c r="H56" s="17"/>
       <c r="I56" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="J56" s="14" t="s">
-        <v>163</v>
+        <v>122</v>
+      </c>
+      <c r="J56" s="15" t="s">
+        <v>155</v>
       </c>
       <c r="K56" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
@@ -6135,18 +6376,20 @@
         <v>81</v>
       </c>
       <c r="C57" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D57" s="14"/>
+        <v>81</v>
+      </c>
+      <c r="D57" s="14" t="s">
+        <v>152</v>
+      </c>
       <c r="H57" s="17"/>
       <c r="I57" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="J57" s="14" t="s">
-        <v>163</v>
+        <v>150</v>
+      </c>
+      <c r="J57" s="15" t="s">
+        <v>155</v>
       </c>
       <c r="K57" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
@@ -6157,17 +6400,20 @@
         <v>81</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>29</v>
+        <v>81</v>
+      </c>
+      <c r="D58" s="14" t="s">
+        <v>101</v>
       </c>
       <c r="H58" s="17"/>
       <c r="I58" s="14" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J58" s="15" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K58" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
@@ -6175,20 +6421,19 @@
         <v>81</v>
       </c>
       <c r="B59" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C59" s="14" t="s">
-        <v>161</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="C59" s="14"/>
+      <c r="D59" s="14"/>
       <c r="H59" s="17"/>
       <c r="I59" s="14" t="s">
-        <v>162</v>
+        <v>123</v>
       </c>
       <c r="J59" s="15" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K59" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
@@ -6199,11 +6444,18 @@
         <v>81</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>100</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="D60" s="14"/>
       <c r="H60" s="17"/>
       <c r="I60" s="14" t="s">
-        <v>127</v>
+        <v>120</v>
+      </c>
+      <c r="J60" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="K60" s="14" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
@@ -6214,14 +6466,18 @@
         <v>81</v>
       </c>
       <c r="C61" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D61" s="14" t="s">
-        <v>90</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="D61" s="14"/>
       <c r="H61" s="17"/>
       <c r="I61" s="14" t="s">
-        <v>128</v>
+        <v>121</v>
+      </c>
+      <c r="J61" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="K61" s="14" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
@@ -6232,19 +6488,18 @@
         <v>81</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D62" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E62" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H62" s="17"/>
       <c r="I62" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="K62" s="14"/>
+        <v>122</v>
+      </c>
+      <c r="J62" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="K62" s="14" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="14" t="s">
@@ -6254,17 +6509,17 @@
         <v>81</v>
       </c>
       <c r="C63" s="14" t="s">
-        <v>31</v>
+        <v>153</v>
       </c>
       <c r="H63" s="17"/>
       <c r="I63" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="J63" s="14" t="s">
-        <v>163</v>
+        <v>154</v>
+      </c>
+      <c r="J63" s="15" t="s">
+        <v>155</v>
       </c>
       <c r="K63" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
@@ -6275,17 +6530,11 @@
         <v>81</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="H64" s="17"/>
       <c r="I64" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="J64" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="K64" s="14" t="s">
-        <v>163</v>
+        <v>124</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
@@ -6296,17 +6545,14 @@
         <v>81</v>
       </c>
       <c r="C65" s="14" t="s">
-        <v>32</v>
+        <v>81</v>
+      </c>
+      <c r="D65" s="14" t="s">
+        <v>90</v>
       </c>
       <c r="H65" s="17"/>
       <c r="I65" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="J65" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="K65" s="14" t="s">
-        <v>163</v>
+        <v>125</v>
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
@@ -6317,18 +6563,19 @@
         <v>81</v>
       </c>
       <c r="C66" s="14" t="s">
-        <v>33</v>
+        <v>81</v>
+      </c>
+      <c r="D66" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E66" s="14" t="s">
+        <v>30</v>
       </c>
       <c r="H66" s="17"/>
       <c r="I66" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="J66" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="K66" s="14" t="s">
-        <v>163</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="K66" s="14"/>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="14" t="s">
@@ -6338,17 +6585,17 @@
         <v>81</v>
       </c>
       <c r="C67" s="14" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="H67" s="17"/>
       <c r="I67" s="14" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="J67" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K67" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
@@ -6359,17 +6606,17 @@
         <v>81</v>
       </c>
       <c r="C68" s="14" t="s">
-        <v>34</v>
+        <v>87</v>
       </c>
       <c r="H68" s="17"/>
       <c r="I68" s="14" t="s">
-        <v>169</v>
+        <v>128</v>
       </c>
       <c r="J68" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K68" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
@@ -6380,20 +6627,17 @@
         <v>81</v>
       </c>
       <c r="C69" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D69" s="14" t="s">
-        <v>166</v>
+        <v>32</v>
       </c>
       <c r="H69" s="17"/>
-      <c r="I69" s="14">
-        <v>0</v>
+      <c r="I69" s="14" t="s">
+        <v>129</v>
       </c>
       <c r="J69" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K69" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
@@ -6404,26 +6648,17 @@
         <v>81</v>
       </c>
       <c r="C70" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D70" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E70" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="F70" s="16" t="s">
-        <v>170</v>
+        <v>33</v>
       </c>
       <c r="H70" s="17"/>
       <c r="I70" s="14" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="J70" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K70" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
@@ -6434,26 +6669,17 @@
         <v>81</v>
       </c>
       <c r="C71" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D71" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E71" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="F71" s="16" t="s">
-        <v>170</v>
+        <v>9</v>
       </c>
       <c r="H71" s="17"/>
       <c r="I71" s="14" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="J71" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K71" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
@@ -6464,23 +6690,17 @@
         <v>81</v>
       </c>
       <c r="C72" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D72" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E72" s="14" t="s">
-        <v>85</v>
+        <v>34</v>
       </c>
       <c r="H72" s="17"/>
       <c r="I72" s="14" t="s">
-        <v>120</v>
+        <v>161</v>
       </c>
       <c r="J72" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K72" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
@@ -6494,20 +6714,17 @@
         <v>81</v>
       </c>
       <c r="D73" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E73" s="14" t="s">
-        <v>90</v>
+        <v>158</v>
       </c>
       <c r="H73" s="17"/>
-      <c r="I73" s="14" t="s">
-        <v>128</v>
+      <c r="I73" s="14">
+        <v>0</v>
       </c>
       <c r="J73" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K73" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
@@ -6524,17 +6741,20 @@
         <v>81</v>
       </c>
       <c r="E74" s="14" t="s">
-        <v>88</v>
+        <v>84</v>
+      </c>
+      <c r="F74" s="16" t="s">
+        <v>162</v>
       </c>
       <c r="H74" s="17"/>
       <c r="I74" s="14" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
       <c r="J74" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K74" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
@@ -6548,17 +6768,23 @@
         <v>81</v>
       </c>
       <c r="D75" s="14" t="s">
-        <v>166</v>
+        <v>81</v>
+      </c>
+      <c r="E75" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F75" s="16" t="s">
+        <v>162</v>
       </c>
       <c r="H75" s="17"/>
-      <c r="I75" s="14">
-        <v>1</v>
+      <c r="I75" s="14" t="s">
+        <v>115</v>
       </c>
       <c r="J75" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K75" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
@@ -6575,20 +6801,17 @@
         <v>81</v>
       </c>
       <c r="E76" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="F76" s="16" t="s">
-        <v>170</v>
+        <v>85</v>
       </c>
       <c r="H76" s="17"/>
       <c r="I76" s="14" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="J76" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K76" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
@@ -6605,20 +6828,17 @@
         <v>81</v>
       </c>
       <c r="E77" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="F77" s="16" t="s">
-        <v>170</v>
+        <v>90</v>
       </c>
       <c r="H77" s="17"/>
       <c r="I77" s="14" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="J77" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K77" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
@@ -6635,17 +6855,17 @@
         <v>81</v>
       </c>
       <c r="E78" s="14" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="H78" s="17"/>
       <c r="I78" s="14" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="J78" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K78" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
@@ -6659,20 +6879,17 @@
         <v>81</v>
       </c>
       <c r="D79" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E79" s="14" t="s">
-        <v>90</v>
+        <v>158</v>
       </c>
       <c r="H79" s="17"/>
-      <c r="I79" s="14" t="s">
-        <v>128</v>
+      <c r="I79" s="14">
+        <v>1</v>
       </c>
       <c r="J79" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K79" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
@@ -6689,17 +6906,20 @@
         <v>81</v>
       </c>
       <c r="E80" s="14" t="s">
-        <v>88</v>
+        <v>84</v>
+      </c>
+      <c r="F80" s="16" t="s">
+        <v>162</v>
       </c>
       <c r="H80" s="17"/>
       <c r="I80" s="14" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
       <c r="J80" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K80" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
@@ -6710,17 +6930,26 @@
         <v>81</v>
       </c>
       <c r="C81" s="14" t="s">
-        <v>89</v>
+        <v>81</v>
+      </c>
+      <c r="D81" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E81" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F81" s="16" t="s">
+        <v>162</v>
       </c>
       <c r="H81" s="17"/>
       <c r="I81" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="J81" s="15" t="s">
-        <v>163</v>
+        <v>115</v>
+      </c>
+      <c r="J81" s="14" t="s">
+        <v>155</v>
       </c>
       <c r="K81" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
@@ -6731,17 +6960,23 @@
         <v>81</v>
       </c>
       <c r="C82" s="14" t="s">
-        <v>172</v>
+        <v>81</v>
+      </c>
+      <c r="D82" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E82" s="14" t="s">
+        <v>85</v>
       </c>
       <c r="H82" s="17"/>
       <c r="I82" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="J82" s="15" t="s">
-        <v>163</v>
+        <v>117</v>
+      </c>
+      <c r="J82" s="14" t="s">
+        <v>155</v>
       </c>
       <c r="K82" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
@@ -6752,17 +6987,23 @@
         <v>81</v>
       </c>
       <c r="C83" s="14" t="s">
-        <v>173</v>
+        <v>81</v>
+      </c>
+      <c r="D83" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E83" s="14" t="s">
+        <v>90</v>
       </c>
       <c r="H83" s="17"/>
       <c r="I83" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="J83" s="15" t="s">
-        <v>163</v>
+        <v>125</v>
+      </c>
+      <c r="J83" s="14" t="s">
+        <v>155</v>
       </c>
       <c r="K83" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
@@ -6773,17 +7014,23 @@
         <v>81</v>
       </c>
       <c r="C84" s="14" t="s">
-        <v>91</v>
+        <v>81</v>
+      </c>
+      <c r="D84" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E84" s="14" t="s">
+        <v>88</v>
       </c>
       <c r="H84" s="17"/>
       <c r="I84" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="J84" s="15" t="s">
-        <v>163</v>
+        <v>133</v>
+      </c>
+      <c r="J84" s="14" t="s">
+        <v>155</v>
       </c>
       <c r="K84" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
@@ -6794,20 +7041,17 @@
         <v>81</v>
       </c>
       <c r="C85" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D85" s="14" t="s">
-        <v>166</v>
+        <v>89</v>
       </c>
       <c r="H85" s="17"/>
-      <c r="I85" s="14">
-        <v>0</v>
-      </c>
-      <c r="J85" s="14" t="s">
-        <v>163</v>
+      <c r="I85" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="J85" s="15" t="s">
+        <v>155</v>
       </c>
       <c r="K85" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
@@ -6818,23 +7062,17 @@
         <v>81</v>
       </c>
       <c r="C86" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D86" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E86" s="14" t="s">
-        <v>92</v>
+        <v>164</v>
       </c>
       <c r="H86" s="17"/>
       <c r="I86" s="14" t="s">
-        <v>171</v>
+        <v>140</v>
       </c>
       <c r="J86" s="15" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K86" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
@@ -6845,23 +7083,17 @@
         <v>81</v>
       </c>
       <c r="C87" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D87" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E87" s="14" t="s">
-        <v>93</v>
+        <v>165</v>
       </c>
       <c r="H87" s="17"/>
       <c r="I87" s="14" t="s">
         <v>141</v>
       </c>
       <c r="J87" s="15" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K87" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
@@ -6872,17 +7104,17 @@
         <v>81</v>
       </c>
       <c r="C88" s="14" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H88" s="17"/>
       <c r="I88" s="14" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="J88" s="15" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K88" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
@@ -6896,17 +7128,17 @@
         <v>81</v>
       </c>
       <c r="D89" s="14" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="H89" s="17"/>
       <c r="I89" s="14">
         <v>0</v>
       </c>
       <c r="J89" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K89" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
@@ -6923,18 +7155,17 @@
         <v>81</v>
       </c>
       <c r="E90" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="F90" s="15"/>
+        <v>92</v>
+      </c>
       <c r="H90" s="17"/>
       <c r="I90" s="14" t="s">
-        <v>141</v>
+        <v>163</v>
       </c>
       <c r="J90" s="15" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K90" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
@@ -6951,20 +7182,17 @@
         <v>81</v>
       </c>
       <c r="E91" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="F91" s="14" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H91" s="17"/>
       <c r="I91" s="14" t="s">
-        <v>167</v>
+        <v>137</v>
       </c>
       <c r="J91" s="15" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K91" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
@@ -6975,26 +7203,17 @@
         <v>81</v>
       </c>
       <c r="C92" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D92" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E92" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="F92" s="14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H92" s="17"/>
       <c r="I92" s="14" t="s">
-        <v>168</v>
+        <v>136</v>
       </c>
       <c r="J92" s="15" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K92" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
@@ -7008,23 +7227,17 @@
         <v>81</v>
       </c>
       <c r="D93" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E93" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="F93" s="14" t="s">
-        <v>97</v>
+        <v>158</v>
       </c>
       <c r="H93" s="17"/>
-      <c r="I93" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="J93" s="15" t="s">
-        <v>163</v>
+      <c r="I93" s="14">
+        <v>0</v>
+      </c>
+      <c r="J93" s="14" t="s">
+        <v>155</v>
       </c>
       <c r="K93" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
@@ -7041,20 +7254,18 @@
         <v>81</v>
       </c>
       <c r="E94" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="F94" s="14" t="s">
-        <v>98</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="F94" s="15"/>
       <c r="H94" s="17"/>
       <c r="I94" s="14" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="J94" s="15" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K94" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
@@ -7074,41 +7285,80 @@
         <v>81</v>
       </c>
       <c r="F95" s="14" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H95" s="17"/>
       <c r="I95" s="14" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
       <c r="J95" s="15" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="K95" s="14" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="14" t="s">
-        <v>102</v>
+        <v>81</v>
+      </c>
+      <c r="B96" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C96" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D96" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E96" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F96" s="14" t="s">
+        <v>96</v>
       </c>
       <c r="H96" s="17"/>
       <c r="I96" s="14" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+      <c r="J96" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="K96" s="14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="14" t="s">
         <v>81</v>
       </c>
       <c r="B97" s="14" t="s">
-        <v>63</v>
+        <v>81</v>
+      </c>
+      <c r="C97" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D97" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E97" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F97" s="14" t="s">
+        <v>97</v>
       </c>
       <c r="H97" s="17"/>
       <c r="I97" s="14" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+      <c r="J97" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="K97" s="14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="14" t="s">
         <v>81</v>
       </c>
@@ -7116,14 +7366,29 @@
         <v>81</v>
       </c>
       <c r="C98" s="14" t="s">
-        <v>30</v>
+        <v>81</v>
+      </c>
+      <c r="D98" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E98" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F98" s="14" t="s">
+        <v>98</v>
       </c>
       <c r="H98" s="17"/>
       <c r="I98" s="14" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+      <c r="J98" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="K98" s="14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="14" t="s">
         <v>81</v>
       </c>
@@ -7134,50 +7399,50 @@
         <v>81</v>
       </c>
       <c r="D99" s="14" t="s">
-        <v>29</v>
+        <v>81</v>
+      </c>
+      <c r="E99" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F99" s="14" t="s">
+        <v>99</v>
       </c>
       <c r="H99" s="17"/>
       <c r="I99" s="14" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="J99" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="K99" s="14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B100" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C100" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D100" s="14" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H100" s="17"/>
       <c r="I100" s="14" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="14" t="s">
         <v>81</v>
       </c>
       <c r="B101" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C101" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D101" s="14" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="H101" s="17"/>
       <c r="I101" s="14" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="J101" s="14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="14" t="s">
         <v>81</v>
       </c>
@@ -7185,17 +7450,17 @@
         <v>81</v>
       </c>
       <c r="C102" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D102" s="14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H102" s="17"/>
       <c r="I102" s="14" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+      <c r="J102" s="14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="14" t="s">
         <v>81</v>
       </c>
@@ -7206,26 +7471,41 @@
         <v>81</v>
       </c>
       <c r="D103" s="14" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="H103" s="17"/>
       <c r="I103" s="14" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+      <c r="J103" s="14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="14" t="s">
         <v>81</v>
       </c>
       <c r="B104" s="14" t="s">
-        <v>30</v>
+        <v>81</v>
+      </c>
+      <c r="C104" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D104" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E104" s="14" t="s">
+        <v>29</v>
       </c>
       <c r="H104" s="17"/>
       <c r="I104" s="14" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="J104" s="14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="14" t="s">
         <v>81</v>
       </c>
@@ -7233,14 +7513,23 @@
         <v>81</v>
       </c>
       <c r="C105" s="14" t="s">
-        <v>63</v>
+        <v>81</v>
+      </c>
+      <c r="D105" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E105" s="14" t="s">
+        <v>101</v>
       </c>
       <c r="H105" s="17"/>
       <c r="I105" s="14" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J105" s="14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="14" t="s">
         <v>81</v>
       </c>
@@ -7251,14 +7540,20 @@
         <v>81</v>
       </c>
       <c r="D106" s="14" t="s">
-        <v>29</v>
+        <v>81</v>
+      </c>
+      <c r="E106" s="14" t="s">
+        <v>32</v>
       </c>
       <c r="H106" s="17"/>
       <c r="I106" s="14" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="J106" s="14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="14" t="s">
         <v>81</v>
       </c>
@@ -7269,14 +7564,20 @@
         <v>81</v>
       </c>
       <c r="D107" s="14" t="s">
-        <v>101</v>
+        <v>81</v>
+      </c>
+      <c r="E107" s="14" t="s">
+        <v>33</v>
       </c>
       <c r="H107" s="17"/>
       <c r="I107" s="14" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+      <c r="J107" s="14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="14" t="s">
         <v>81</v>
       </c>
@@ -7287,32 +7588,35 @@
         <v>81</v>
       </c>
       <c r="D108" s="14" t="s">
-        <v>32</v>
+        <v>81</v>
+      </c>
+      <c r="E108" s="14" t="s">
+        <v>88</v>
       </c>
       <c r="H108" s="17"/>
       <c r="I108" s="14" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+      <c r="J108" s="14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="14" t="s">
         <v>81</v>
       </c>
       <c r="B109" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C109" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D109" s="14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H109" s="17"/>
       <c r="I109" s="14" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+      <c r="J109" s="14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="14" t="s">
         <v>81</v>
       </c>
@@ -7320,31 +7624,38 @@
         <v>81</v>
       </c>
       <c r="C110" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D110" s="14" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="H110" s="17"/>
       <c r="I110" s="14" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="J110" s="14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="14" t="s">
         <v>81</v>
       </c>
       <c r="B111" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C111" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D111" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="C111" s="14"/>
-      <c r="D111" s="14"/>
       <c r="H111" s="17"/>
       <c r="I111" s="14" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+      <c r="J111" s="14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="14" t="s">
         <v>81</v>
       </c>
@@ -7352,15 +7663,23 @@
         <v>81</v>
       </c>
       <c r="C112" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="D112" s="14"/>
+        <v>81</v>
+      </c>
+      <c r="D112" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E112" s="14" t="s">
+        <v>29</v>
+      </c>
       <c r="H112" s="17"/>
       <c r="I112" s="14" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="J112" s="14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="14" t="s">
         <v>81</v>
       </c>
@@ -7368,15 +7687,23 @@
         <v>81</v>
       </c>
       <c r="C113" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D113" s="14"/>
+        <v>81</v>
+      </c>
+      <c r="D113" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E113" s="14" t="s">
+        <v>101</v>
+      </c>
       <c r="H113" s="17"/>
       <c r="I113" s="14" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+      <c r="J113" s="14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="14" t="s">
         <v>81</v>
       </c>
@@ -7384,14 +7711,23 @@
         <v>81</v>
       </c>
       <c r="C114" s="14" t="s">
-        <v>29</v>
+        <v>81</v>
+      </c>
+      <c r="D114" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E114" s="14" t="s">
+        <v>32</v>
       </c>
       <c r="H114" s="17"/>
       <c r="I114" s="14" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="J114" s="14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="14" t="s">
         <v>81</v>
       </c>
@@ -7399,14 +7735,23 @@
         <v>81</v>
       </c>
       <c r="C115" s="14" t="s">
-        <v>161</v>
+        <v>81</v>
+      </c>
+      <c r="D115" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E115" s="14" t="s">
+        <v>33</v>
       </c>
       <c r="H115" s="17"/>
       <c r="I115" s="14" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+      <c r="J115" s="14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="14" t="s">
         <v>81</v>
       </c>
@@ -7414,32 +7759,37 @@
         <v>81</v>
       </c>
       <c r="C116" s="14" t="s">
-        <v>100</v>
+        <v>81</v>
+      </c>
+      <c r="D116" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E116" s="14" t="s">
+        <v>88</v>
       </c>
       <c r="H116" s="17"/>
       <c r="I116" s="14" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+      <c r="J116" s="14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="14" t="s">
         <v>81</v>
       </c>
       <c r="B117" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="C117" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D117" s="14" t="s">
-        <v>90</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="C117" s="14"/>
+      <c r="D117" s="14"/>
       <c r="H117" s="17"/>
       <c r="I117" s="14" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="14" t="s">
         <v>81</v>
       </c>
@@ -7447,20 +7797,18 @@
         <v>81</v>
       </c>
       <c r="C118" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D118" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E118" s="14" t="s">
-        <v>30</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="D118" s="14"/>
       <c r="H118" s="17"/>
       <c r="I118" s="14" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="J118" s="14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="14" t="s">
         <v>81</v>
       </c>
@@ -7468,14 +7816,18 @@
         <v>81</v>
       </c>
       <c r="C119" s="14" t="s">
-        <v>31</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="D119" s="14"/>
       <c r="H119" s="17"/>
       <c r="I119" s="14" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+      <c r="J119" s="14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="14" t="s">
         <v>81</v>
       </c>
@@ -7483,14 +7835,17 @@
         <v>81</v>
       </c>
       <c r="C120" s="14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H120" s="17"/>
       <c r="I120" s="14" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="J120" s="14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="14" t="s">
         <v>81</v>
       </c>
@@ -7498,14 +7853,17 @@
         <v>81</v>
       </c>
       <c r="C121" s="14" t="s">
-        <v>33</v>
+        <v>153</v>
       </c>
       <c r="H121" s="17"/>
       <c r="I121" s="14" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+      <c r="J121" s="14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="14" t="s">
         <v>81</v>
       </c>
@@ -7513,14 +7871,14 @@
         <v>81</v>
       </c>
       <c r="C122" s="14" t="s">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="H122" s="17"/>
       <c r="I122" s="14" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="14" t="s">
         <v>81</v>
       </c>
@@ -7528,17 +7886,17 @@
         <v>81</v>
       </c>
       <c r="C123" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="D123" s="16" t="s">
-        <v>108</v>
+        <v>81</v>
+      </c>
+      <c r="D123" s="14" t="s">
+        <v>90</v>
       </c>
       <c r="H123" s="17"/>
       <c r="I123" s="14" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="14" t="s">
         <v>81</v>
       </c>
@@ -7546,14 +7904,20 @@
         <v>81</v>
       </c>
       <c r="C124" s="14" t="s">
-        <v>103</v>
+        <v>81</v>
+      </c>
+      <c r="D124" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E124" s="14" t="s">
+        <v>30</v>
       </c>
       <c r="H124" s="17"/>
       <c r="I124" s="14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="14" t="s">
         <v>81</v>
       </c>
@@ -7561,17 +7925,17 @@
         <v>81</v>
       </c>
       <c r="C125" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D125" s="14" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="H125" s="17"/>
       <c r="I125" s="14" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+      <c r="J125" s="14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="14" t="s">
         <v>81</v>
       </c>
@@ -7579,20 +7943,17 @@
         <v>81</v>
       </c>
       <c r="C126" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D126" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E126" s="14" t="s">
-        <v>106</v>
+        <v>32</v>
       </c>
       <c r="H126" s="17"/>
       <c r="I126" s="14" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="J126" s="14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="14" t="s">
         <v>81</v>
       </c>
@@ -7600,20 +7961,17 @@
         <v>81</v>
       </c>
       <c r="C127" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D127" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E127" s="14" t="s">
-        <v>104</v>
+        <v>33</v>
       </c>
       <c r="H127" s="17"/>
       <c r="I127" s="14" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+      <c r="J127" s="14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="14" t="s">
         <v>81</v>
       </c>
@@ -7621,20 +7979,17 @@
         <v>81</v>
       </c>
       <c r="C128" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D128" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E128" s="14" t="s">
-        <v>105</v>
+        <v>50</v>
       </c>
       <c r="H128" s="17"/>
       <c r="I128" s="14" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+      <c r="J128" s="14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="14" t="s">
         <v>81</v>
       </c>
@@ -7642,20 +7997,20 @@
         <v>81</v>
       </c>
       <c r="C129" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="D129" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E129" s="14" t="s">
-        <v>88</v>
+        <v>104</v>
+      </c>
+      <c r="D129" s="16" t="s">
+        <v>105</v>
       </c>
       <c r="H129" s="17"/>
       <c r="I129" s="14" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+      <c r="J129" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="14" t="s">
         <v>81</v>
       </c>
@@ -7663,66 +8018,142 @@
         <v>81</v>
       </c>
       <c r="C130" s="14" t="s">
-        <v>54</v>
+        <v>103</v>
       </c>
       <c r="H130" s="17"/>
       <c r="I130" s="14" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A131" s="14"/>
-      <c r="B131" s="14"/>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A132" s="14"/>
-      <c r="B132" s="14"/>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A133" s="14"/>
-      <c r="B133" s="14"/>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A134" s="14"/>
-      <c r="B134" s="14"/>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A135" s="14"/>
-      <c r="B135" s="14"/>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A136" s="14"/>
-      <c r="B136" s="14"/>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A131" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B131" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C131" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D131" s="16" t="s">
+        <v>245</v>
+      </c>
+      <c r="E131" s="16"/>
+      <c r="H131" s="17"/>
+      <c r="I131" s="14" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A132" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B132" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C132" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="H132" s="17"/>
+      <c r="I132" s="14" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A133" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B133" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C133" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D133" s="16" t="s">
+        <v>245</v>
+      </c>
+      <c r="H133" s="17"/>
+      <c r="I133" s="14" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A134" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B134" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C134" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="H134" s="17"/>
+      <c r="I134" s="14" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A135" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B135" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C135" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D135" s="16" t="s">
+        <v>245</v>
+      </c>
+      <c r="H135" s="17"/>
+      <c r="I135" s="14" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A136" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B136" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C136" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="H136" s="17"/>
+      <c r="I136" s="14" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="14"/>
       <c r="B137" s="14"/>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="14"/>
       <c r="B138" s="14"/>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="14"/>
       <c r="B139" s="14"/>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="14"/>
       <c r="B140" s="14"/>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="14"/>
       <c r="B141" s="14"/>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="14"/>
       <c r="B142" s="14"/>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="14"/>
       <c r="B143" s="14"/>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="14"/>
       <c r="B144" s="14"/>
     </row>
@@ -7840,62 +8271,68 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="14"/>
+      <c r="B173" s="14"/>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="14"/>
+      <c r="B174" s="14"/>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="14"/>
+      <c r="B175" s="14"/>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="14"/>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B176" s="14"/>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="14"/>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B177" s="14"/>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="14"/>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B178" s="14"/>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="14"/>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="14"/>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="14"/>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="14"/>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="14"/>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="14"/>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="14"/>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="14"/>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="14"/>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="14"/>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" s="14"/>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" s="14"/>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="14"/>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" s="14"/>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.25">
@@ -7924,6 +8361,591 @@
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A201" s="14"/>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" s="14"/>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" s="14"/>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" s="14"/>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205" s="14"/>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206" s="14"/>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G40"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="2.140625" style="23" customWidth="1"/>
+    <col min="3" max="3" width="38" customWidth="1"/>
+    <col min="5" max="5" width="2.140625" style="23" customWidth="1"/>
+    <col min="6" max="6" width="29.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="22"/>
+      <c r="C1" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="E1" s="22"/>
+      <c r="F1" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="23" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>173</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>175</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="G5" s="21" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="G7" s="21" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="D8" s="21"/>
+      <c r="F8" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="G8" s="21" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>205</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>207</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>183</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="G13" s="21" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>209</v>
+      </c>
+      <c r="G14" s="21" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="G15" s="21" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="G16" s="21" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>211</v>
+      </c>
+      <c r="G17" s="21" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="F18" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="G18" s="21" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="F19" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="G19" s="21" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="F20" s="21" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>18</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="F21" s="21" t="s">
+        <v>214</v>
+      </c>
+      <c r="G21" s="21" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>19</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="F22" s="21" t="s">
+        <v>215</v>
+      </c>
+      <c r="G22" s="21" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>20</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="F23" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="G23" s="21" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>21</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="F24" s="21" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>22</v>
+      </c>
+      <c r="F25" s="21" t="s">
+        <v>218</v>
+      </c>
+      <c r="G25" s="21" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>23</v>
+      </c>
+      <c r="F26" s="21" t="s">
+        <v>221</v>
+      </c>
+      <c r="G26" s="21" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>24</v>
+      </c>
+      <c r="F27" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="G27" s="21" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>25</v>
+      </c>
+      <c r="F28" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="G28" s="21" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>26</v>
+      </c>
+      <c r="F29" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="G29" s="21" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>27</v>
+      </c>
+      <c r="F30" s="21" t="s">
+        <v>225</v>
+      </c>
+      <c r="G30" s="21" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>28</v>
+      </c>
+      <c r="F31" s="21" t="s">
+        <v>226</v>
+      </c>
+      <c r="G31" s="21" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>29</v>
+      </c>
+      <c r="F32" s="21" t="s">
+        <v>227</v>
+      </c>
+      <c r="G32" s="21" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>30</v>
+      </c>
+      <c r="F33" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="G33" s="21" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>31</v>
+      </c>
+      <c r="F34" s="21" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>32</v>
+      </c>
+      <c r="F35" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="G35" s="21" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>33</v>
+      </c>
+      <c r="F36" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="G36" s="21" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>34</v>
+      </c>
+      <c r="F37" s="21" t="s">
+        <v>229</v>
+      </c>
+      <c r="G37" s="21" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>35</v>
+      </c>
+      <c r="F38" s="21" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>36</v>
+      </c>
+      <c r="F39" s="21" t="s">
+        <v>231</v>
+      </c>
+      <c r="G39" s="21" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>37</v>
+      </c>
+      <c r="F40" s="21" t="s">
+        <v>232</v>
+      </c>
+      <c r="G40" s="21" t="s">
+        <v>242</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>